<commit_message>
Added React framework for UI
</commit_message>
<xml_diff>
--- a/Stored_data/predictions_test.xlsx
+++ b/Stored_data/predictions_test.xlsx
@@ -450,7 +450,7 @@
         <v>-0.9094173066706008</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.8452302813529968</v>
+        <v>-0.8878097534179688</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>-0.9189658448962772</v>
       </c>
       <c r="B3" t="n">
-        <v>-0.8438383936882019</v>
+        <v>-0.8755366206169128</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>0.47480791585524</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4398827850818634</v>
+        <v>0.3697855770587921</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>-0.8492427362615442</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.8133499622344971</v>
+        <v>-0.7920433282852173</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>-0.404843516281526</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.3266681134700775</v>
+        <v>-0.3540193736553192</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>0.653714611237064</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5745821595191956</v>
+        <v>0.6441981196403503</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>-0.43273120341603</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.3899121284484863</v>
+        <v>-0.4144650101661682</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>-0.8602837847814329</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.8070902228355408</v>
+        <v>-0.7925203442573547</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>-0.2862281152629458</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.2500492334365845</v>
+        <v>-0.2449578940868378</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>-0.8113027821924031</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.7594775557518005</v>
+        <v>-0.7803751826286316</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>1.156748682977122</v>
       </c>
       <c r="B12" t="n">
-        <v>1.115044474601746</v>
+        <v>1.176698684692383</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>-0.738764291782665</v>
       </c>
       <c r="B13" t="n">
-        <v>-0.648052990436554</v>
+        <v>-0.6682805418968201</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>1.075976225452425</v>
       </c>
       <c r="B14" t="n">
-        <v>1.094888210296631</v>
+        <v>1.106894850730896</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>-1.094100540851888</v>
       </c>
       <c r="B15" t="n">
-        <v>-1.004178524017334</v>
+        <v>-1.024115681648254</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>-0.9554350771426543</v>
       </c>
       <c r="B16" t="n">
-        <v>-0.8907949924468994</v>
+        <v>-0.8940123915672302</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>0.7495729913740976</v>
       </c>
       <c r="B17" t="n">
-        <v>0.7875055074691772</v>
+        <v>0.8267964124679565</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>0.9426567188449843</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9793114066123962</v>
+        <v>0.9909985661506653</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>1.690232662339384</v>
       </c>
       <c r="B19" t="n">
-        <v>1.600760459899902</v>
+        <v>1.733831167221069</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>-0.7906250040147854</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.825097918510437</v>
+        <v>-0.8332045674324036</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>-0.3938501948895719</v>
       </c>
       <c r="B21" t="n">
-        <v>-0.3901064693927765</v>
+        <v>-0.3316576778888702</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>-1.09069064507022</v>
       </c>
       <c r="B22" t="n">
-        <v>-0.9385937452316284</v>
+        <v>-0.9727312922477722</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>-0.8061010440206735</v>
       </c>
       <c r="B23" t="n">
-        <v>-0.8085546493530273</v>
+        <v>-0.8020515441894531</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>-0.3380110115256079</v>
       </c>
       <c r="B24" t="n">
-        <v>-0.2988918721675873</v>
+        <v>-0.3083298206329346</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>-0.9582883293561292</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.8972727656364441</v>
+        <v>-0.8958705067634583</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>-0.8876921255440731</v>
       </c>
       <c r="B26" t="n">
-        <v>-0.8828449249267578</v>
+        <v>-0.8772546648979187</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>-0.8790825666831948</v>
       </c>
       <c r="B27" t="n">
-        <v>-0.8449691534042358</v>
+        <v>-0.8112837672233582</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>-0.8610188863062499</v>
       </c>
       <c r="B28" t="n">
-        <v>-0.8051952123641968</v>
+        <v>-0.837688148021698</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>0.2110340866358171</v>
       </c>
       <c r="B29" t="n">
-        <v>0.1976082921028137</v>
+        <v>0.1938780248165131</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>-0.9159030083383942</v>
       </c>
       <c r="B30" t="n">
-        <v>-0.8680063486099243</v>
+        <v>-0.9042391180992126</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>0.0936772292299444</v>
       </c>
       <c r="B31" t="n">
-        <v>0.09626086801290512</v>
+        <v>0.1065280586481094</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>0.1690326577340769</v>
       </c>
       <c r="B32" t="n">
-        <v>0.1939053535461426</v>
+        <v>0.1460115760564804</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>0.2303791366431772</v>
       </c>
       <c r="B33" t="n">
-        <v>0.2256170064210892</v>
+        <v>0.1735884249210358</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>-0.3657539609569194</v>
       </c>
       <c r="B34" t="n">
-        <v>-0.3397196531295776</v>
+        <v>-0.3692823946475983</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>-0.9324487585377707</v>
       </c>
       <c r="B35" t="n">
-        <v>-0.8462499380111694</v>
+        <v>-0.8797438740730286</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>-0.8078954802763844</v>
       </c>
       <c r="B36" t="n">
-        <v>-0.8003813624382019</v>
+        <v>-0.8017503619194031</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>-0.7824309824308152</v>
       </c>
       <c r="B37" t="n">
-        <v>-0.7129372358322144</v>
+        <v>-0.7519791722297668</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>-0.9524785890763646</v>
       </c>
       <c r="B38" t="n">
-        <v>-0.8430129885673523</v>
+        <v>-0.907581627368927</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>2.024586094630712</v>
       </c>
       <c r="B39" t="n">
-        <v>2.01188325881958</v>
+        <v>2.019070863723755</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>-1.086685197735631</v>
       </c>
       <c r="B40" t="n">
-        <v>-0.9891252517700195</v>
+        <v>-0.9967902302742004</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1.160109295311466</v>
       </c>
       <c r="B41" t="n">
-        <v>1.09173321723938</v>
+        <v>1.087225675582886</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>0.5045502169285028</v>
       </c>
       <c r="B42" t="n">
-        <v>0.4599553048610687</v>
+        <v>0.4020884037017822</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>-0.8611812622958531</v>
       </c>
       <c r="B43" t="n">
-        <v>-0.8249430656433105</v>
+        <v>-0.8220493793487549</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>-0.7868203218813991</v>
       </c>
       <c r="B44" t="n">
-        <v>-0.7683424949645996</v>
+        <v>-0.7887991070747375</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>2.165053776192603</v>
       </c>
       <c r="B45" t="n">
-        <v>2.079269170761108</v>
+        <v>2.051846265792847</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>-0.08448969566889525</v>
       </c>
       <c r="B46" t="n">
-        <v>-0.1156669184565544</v>
+        <v>-0.06694308668375015</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>0.9014791016732437</v>
       </c>
       <c r="B47" t="n">
-        <v>0.9479469656944275</v>
+        <v>0.9729892611503601</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>0.2604311452748843</v>
       </c>
       <c r="B48" t="n">
-        <v>0.2140144407749176</v>
+        <v>0.2156489789485931</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>0.4204913316270121</v>
       </c>
       <c r="B49" t="n">
-        <v>0.4726128280162811</v>
+        <v>0.4780251383781433</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>-0.8979404887217453</v>
       </c>
       <c r="B50" t="n">
-        <v>-0.8523330092430115</v>
+        <v>-0.8631591200828552</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>0.533028267884631</v>
       </c>
       <c r="B51" t="n">
-        <v>0.4984731078147888</v>
+        <v>0.5152923464775085</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>-0.2774193475202542</v>
       </c>
       <c r="B52" t="n">
-        <v>-0.263801634311676</v>
+        <v>-0.2777296304702759</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>-0.6757177933274634</v>
       </c>
       <c r="B53" t="n">
-        <v>-0.6733380556106567</v>
+        <v>-0.6764419078826904</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>0.950085031289484</v>
       </c>
       <c r="B54" t="n">
-        <v>0.9202001690864563</v>
+        <v>0.9712666869163513</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>-0.9356651519420515</v>
       </c>
       <c r="B55" t="n">
-        <v>-0.8991882801055908</v>
+        <v>-0.9088135361671448</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>-0.7983370853612434</v>
       </c>
       <c r="B56" t="n">
-        <v>-0.7680394649505615</v>
+        <v>-0.7818315625190735</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>0.1286949342593575</v>
       </c>
       <c r="B57" t="n">
-        <v>0.1486649811267853</v>
+        <v>0.2886624932289124</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>-0.2705196648949421</v>
       </c>
       <c r="B58" t="n">
-        <v>-0.2641839683055878</v>
+        <v>-0.2092420309782028</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1.159491955287096</v>
       </c>
       <c r="B59" t="n">
-        <v>1.116173982620239</v>
+        <v>1.221513152122498</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>-1.096643047960659</v>
       </c>
       <c r="B60" t="n">
-        <v>-0.9956561326980591</v>
+        <v>-1.018414974212646</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>-0.665597048339703</v>
       </c>
       <c r="B61" t="n">
-        <v>-0.7292708158493042</v>
+        <v>-0.7341281771659851</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>0.8281780147628132</v>
       </c>
       <c r="B62" t="n">
-        <v>0.8896819353103638</v>
+        <v>0.8598818182945251</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>0.4922080853992694</v>
       </c>
       <c r="B63" t="n">
-        <v>0.4427863955497742</v>
+        <v>0.4520560204982758</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>-0.8859148088016431</v>
       </c>
       <c r="B64" t="n">
-        <v>-0.8307579755783081</v>
+        <v>-0.8441609740257263</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>-0.8704221680556039</v>
       </c>
       <c r="B65" t="n">
-        <v>-0.8083568811416626</v>
+        <v>-0.801014244556427</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>-0.3102058093187298</v>
       </c>
       <c r="B66" t="n">
-        <v>-0.3168452382087708</v>
+        <v>-0.2824037671089172</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>-1.084651607067118</v>
       </c>
       <c r="B67" t="n">
-        <v>-0.9760763645172119</v>
+        <v>-0.9708238244056702</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>2.196812548421097</v>
       </c>
       <c r="B68" t="n">
-        <v>2.147640228271484</v>
+        <v>2.122724771499634</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>2.049692120243643</v>
       </c>
       <c r="B69" t="n">
-        <v>1.853452563285828</v>
+        <v>1.918616652488708</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>1.777559818358128</v>
       </c>
       <c r="B70" t="n">
-        <v>1.706950545310974</v>
+        <v>1.682178497314453</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>0.4902300034556368</v>
       </c>
       <c r="B71" t="n">
-        <v>0.4284267723560333</v>
+        <v>0.4672404825687408</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>2.023204601786261</v>
       </c>
       <c r="B72" t="n">
-        <v>2.005151510238647</v>
+        <v>2.013304471969604</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>-0.7200677081874584</v>
       </c>
       <c r="B73" t="n">
-        <v>-0.6947726011276245</v>
+        <v>-0.7152320742607117</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>0.07702668685836417</v>
       </c>
       <c r="B74" t="n">
-        <v>0.06436733156442642</v>
+        <v>0.05788691714406013</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>-1.085841672626702</v>
       </c>
       <c r="B75" t="n">
-        <v>-0.965711772441864</v>
+        <v>-1.000587582588196</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>-0.7467855619144377</v>
       </c>
       <c r="B76" t="n">
-        <v>-0.7465813159942627</v>
+        <v>-0.7447662949562073</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>0.1639777323580588</v>
       </c>
       <c r="B77" t="n">
-        <v>0.1485158354043961</v>
+        <v>0.1881256848573685</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>0.9499823142097987</v>
       </c>
       <c r="B78" t="n">
-        <v>0.9488096237182617</v>
+        <v>1.011727213859558</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>2.014734592897278</v>
       </c>
       <c r="B79" t="n">
-        <v>1.926090598106384</v>
+        <v>1.944695711135864</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>-0.7490396311630828</v>
       </c>
       <c r="B80" t="n">
-        <v>-0.7283156514167786</v>
+        <v>-0.7390405535697937</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>0.9739133186839077</v>
       </c>
       <c r="B81" t="n">
-        <v>0.9445239901542664</v>
+        <v>0.9747904539108276</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>-0.8642695187370925</v>
       </c>
       <c r="B82" t="n">
-        <v>-0.8505080342292786</v>
+        <v>-0.8249295353889465</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>0.1413291350606244</v>
       </c>
       <c r="B83" t="n">
-        <v>0.1489271521568298</v>
+        <v>0.1730534732341766</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>0.2891893337210631</v>
       </c>
       <c r="B84" t="n">
-        <v>0.2088097184896469</v>
+        <v>0.2554406225681305</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>-0.9208344657095384</v>
       </c>
       <c r="B85" t="n">
-        <v>-0.8794516921043396</v>
+        <v>-0.9222339987754822</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>-0.3228317097499213</v>
       </c>
       <c r="B86" t="n">
-        <v>-0.2889942824840546</v>
+        <v>-0.2397584617137909</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>1.906912266842579</v>
       </c>
       <c r="B87" t="n">
-        <v>1.720868110656738</v>
+        <v>1.745185494422913</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>-0.9109767386985473</v>
       </c>
       <c r="B88" t="n">
-        <v>-0.8862615823745728</v>
+        <v>-0.8605116009712219</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>-0.1366346955761037</v>
       </c>
       <c r="B89" t="n">
-        <v>-0.08074130862951279</v>
+        <v>-0.07674208283424377</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>1.689627254096998</v>
       </c>
       <c r="B90" t="n">
-        <v>1.702900409698486</v>
+        <v>1.699823141098022</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>0.8966187162208719</v>
       </c>
       <c r="B91" t="n">
-        <v>0.8515849113464355</v>
+        <v>0.8835485577583313</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>-0.7225142422672307</v>
       </c>
       <c r="B92" t="n">
-        <v>-0.7319395542144775</v>
+        <v>-0.7337912321090698</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>1.904612026785389</v>
       </c>
       <c r="B93" t="n">
-        <v>1.884366154670715</v>
+        <v>1.91616427898407</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>-0.8272877386385492</v>
       </c>
       <c r="B94" t="n">
-        <v>-0.805617094039917</v>
+        <v>-0.8055287003517151</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>0.6639500050864933</v>
       </c>
       <c r="B95" t="n">
-        <v>0.6943919062614441</v>
+        <v>0.7042441964149475</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>0.106403771648302</v>
       </c>
       <c r="B96" t="n">
-        <v>0.08158699423074722</v>
+        <v>0.1324762105941772</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>-0.8920410006905385</v>
       </c>
       <c r="B97" t="n">
-        <v>-0.8181025981903076</v>
+        <v>-0.8507815599441528</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>-0.1794599362078435</v>
       </c>
       <c r="B98" t="n">
-        <v>-0.1370954662561417</v>
+        <v>-0.139059990644455</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>2.080913962282875</v>
       </c>
       <c r="B99" t="n">
-        <v>1.944074034690857</v>
+        <v>1.980826854705811</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>-0.8948423755910411</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.8918899893760681</v>
+        <v>-0.8630648255348206</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>2.160367698511817</v>
       </c>
       <c r="B101" t="n">
-        <v>2.046450614929199</v>
+        <v>2.038298368453979</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>-0.4265821855094265</v>
       </c>
       <c r="B102" t="n">
-        <v>-0.38846355676651</v>
+        <v>-0.3352189660072327</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>1.120791479809781</v>
       </c>
       <c r="B103" t="n">
-        <v>0.8385453224182129</v>
+        <v>0.9068099856376648</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>-0.9362383962503951</v>
       </c>
       <c r="B104" t="n">
-        <v>-0.9323257207870483</v>
+        <v>-0.9141388535499573</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>1.842842229002435</v>
       </c>
       <c r="B105" t="n">
-        <v>1.914076209068298</v>
+        <v>1.805828094482422</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>0.205449493894352</v>
       </c>
       <c r="B106" t="n">
-        <v>0.1715316921472549</v>
+        <v>0.1942263543605804</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>0.4314332944791235</v>
       </c>
       <c r="B107" t="n">
-        <v>0.4021614491939545</v>
+        <v>0.419674813747406</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>0.2294754338512002</v>
       </c>
       <c r="B108" t="n">
-        <v>0.2218403667211533</v>
+        <v>0.210168331861496</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>-0.9370191498106277</v>
       </c>
       <c r="B109" t="n">
-        <v>-0.9244347810745239</v>
+        <v>-0.9045110940933228</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>-1.086844461086456</v>
       </c>
       <c r="B110" t="n">
-        <v>-0.9861338138580322</v>
+        <v>-0.9951179027557373</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>-0.8611745182451667</v>
       </c>
       <c r="B111" t="n">
-        <v>-0.7613736987113953</v>
+        <v>-0.7677604556083679</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>0.1467368261648541</v>
       </c>
       <c r="B112" t="n">
-        <v>0.1296606957912445</v>
+        <v>0.1447722017765045</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>1.761246478520868</v>
       </c>
       <c r="B113" t="n">
-        <v>1.701205611228943</v>
+        <v>1.681625247001648</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>2.50578811797952</v>
       </c>
       <c r="B114" t="n">
-        <v>2.225299596786499</v>
+        <v>2.276884794235229</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>-0.7564954385834578</v>
       </c>
       <c r="B115" t="n">
-        <v>-0.7494943141937256</v>
+        <v>-0.727025032043457</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>-0.8063401984334757</v>
       </c>
       <c r="B116" t="n">
-        <v>-0.7491816282272339</v>
+        <v>-0.7813805937767029</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>-1.078135297784671</v>
       </c>
       <c r="B117" t="n">
-        <v>-0.9734104871749878</v>
+        <v>-1.004033923149109</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>-0.7636259752514964</v>
       </c>
       <c r="B118" t="n">
-        <v>-0.6698808670043945</v>
+        <v>-0.6941078305244446</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>1.131459530449399</v>
       </c>
       <c r="B119" t="n">
-        <v>1.005248785018921</v>
+        <v>1.057862997055054</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>-0.2510967989181237</v>
       </c>
       <c r="B120" t="n">
-        <v>-0.2756708860397339</v>
+        <v>-0.2364706993103027</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>0.8174010217659536</v>
       </c>
       <c r="B121" t="n">
-        <v>0.7033525109291077</v>
+        <v>0.6915371417999268</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>-0.2299407119149016</v>
       </c>
       <c r="B122" t="n">
-        <v>-0.1937327831983566</v>
+        <v>-0.2606940865516663</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>-0.9634807296115241</v>
       </c>
       <c r="B123" t="n">
-        <v>-0.9041491746902466</v>
+        <v>-0.9101580381393433</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>-1.083976683225349</v>
       </c>
       <c r="B124" t="n">
-        <v>-1.009023666381836</v>
+        <v>-0.990329921245575</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>-0.9274882498713619</v>
       </c>
       <c r="B125" t="n">
-        <v>-0.874769926071167</v>
+        <v>-0.8790587782859802</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>0.7880618074144853</v>
       </c>
       <c r="B126" t="n">
-        <v>0.8365733623504639</v>
+        <v>0.8481859564781189</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>2.013088006983538</v>
       </c>
       <c r="B127" t="n">
-        <v>1.77923047542572</v>
+        <v>1.825780153274536</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>-0.7485846671283161</v>
       </c>
       <c r="B128" t="n">
-        <v>-0.7448289394378662</v>
+        <v>-0.7157131433486938</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>-0.7960155756057342</v>
       </c>
       <c r="B129" t="n">
-        <v>-0.7578598260879517</v>
+        <v>-0.7708980441093445</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>1.211397282008372</v>
       </c>
       <c r="B130" t="n">
-        <v>1.116343975067139</v>
+        <v>1.157229423522949</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>1.91615369137546</v>
       </c>
       <c r="B131" t="n">
-        <v>1.85586416721344</v>
+        <v>1.817526340484619</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>-0.2785077335464124</v>
       </c>
       <c r="B132" t="n">
-        <v>-0.2477476447820663</v>
+        <v>-0.2820464670658112</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>-0.8003691197103672</v>
       </c>
       <c r="B133" t="n">
-        <v>-0.743107795715332</v>
+        <v>-0.747229278087616</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>-0.8937591772961803</v>
       </c>
       <c r="B134" t="n">
-        <v>-0.8825836777687073</v>
+        <v>-0.8558732867240906</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>0.7733820841627219</v>
       </c>
       <c r="B135" t="n">
-        <v>0.7269347310066223</v>
+        <v>0.8115699887275696</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>0.8761972119693371</v>
       </c>
       <c r="B136" t="n">
-        <v>0.8732550144195557</v>
+        <v>0.8969393968582153</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>-0.8806020531801526</v>
       </c>
       <c r="B137" t="n">
-        <v>-0.7879865169525146</v>
+        <v>-0.8113192915916443</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>0.06659934695093758</v>
       </c>
       <c r="B138" t="n">
-        <v>0.09591225534677505</v>
+        <v>0.07096259295940399</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>-0.5936634473992215</v>
       </c>
       <c r="B139" t="n">
-        <v>-0.5024918913841248</v>
+        <v>-0.4411220848560333</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>1.019440329775243</v>
       </c>
       <c r="B140" t="n">
-        <v>0.9043647050857544</v>
+        <v>0.9662563800811768</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>-1.013335864924136</v>
       </c>
       <c r="B141" t="n">
-        <v>-0.9174278378486633</v>
+        <v>-0.9516053199768066</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>1.869127944712355</v>
       </c>
       <c r="B142" t="n">
-        <v>1.924458146095276</v>
+        <v>1.947049140930176</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>1.250865022944547</v>
       </c>
       <c r="B143" t="n">
-        <v>1.228995561599731</v>
+        <v>1.235641241073608</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>-0.8064688541696469</v>
       </c>
       <c r="B144" t="n">
-        <v>-0.7220673561096191</v>
+        <v>-0.720879077911377</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>-0.2326430011476272</v>
       </c>
       <c r="B145" t="n">
-        <v>-0.2913370132446289</v>
+        <v>-0.2401534765958786</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>0.4924539838627579</v>
       </c>
       <c r="B146" t="n">
-        <v>0.4859207570552826</v>
+        <v>0.5061246156692505</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>-0.9421145394907643</v>
       </c>
       <c r="B147" t="n">
-        <v>-0.8966830968856812</v>
+        <v>-0.8990850448608398</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>-1.098519969143996</v>
       </c>
       <c r="B148" t="n">
-        <v>-1.005968689918518</v>
+        <v>-0.9997411966323853</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>0.2756519489009489</v>
       </c>
       <c r="B149" t="n">
-        <v>0.2572323381900787</v>
+        <v>0.2623348534107208</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>0.6467744643076335</v>
       </c>
       <c r="B150" t="n">
-        <v>0.6476446390151978</v>
+        <v>0.6505506038665771</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>-0.7430887845920336</v>
       </c>
       <c r="B151" t="n">
-        <v>-0.7015002369880676</v>
+        <v>-0.6849641799926758</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>-0.8617301242670997</v>
       </c>
       <c r="B152" t="n">
-        <v>-0.7988631725311279</v>
+        <v>-0.797474205493927</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>-1.117750889062816</v>
       </c>
       <c r="B153" t="n">
-        <v>-0.9859139919281006</v>
+        <v>-0.995167076587677</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>0.9869220736848346</v>
       </c>
       <c r="B154" t="n">
-        <v>0.954816460609436</v>
+        <v>0.9670156836509705</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>1.704988126468088</v>
       </c>
       <c r="B155" t="n">
-        <v>1.612564444541931</v>
+        <v>1.648964643478394</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>2.27117712024746</v>
       </c>
       <c r="B156" t="n">
-        <v>2.140841484069824</v>
+        <v>2.189331293106079</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>-1.101087896136123</v>
       </c>
       <c r="B157" t="n">
-        <v>-0.9906349182128906</v>
+        <v>-0.9908252954483032</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>1.560262355057434</v>
       </c>
       <c r="B158" t="n">
-        <v>1.494510054588318</v>
+        <v>1.516843438148499</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>0.6470390386037921</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5676661133766174</v>
+        <v>0.632256805896759</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>-0.07405768680330115</v>
       </c>
       <c r="B160" t="n">
-        <v>-0.04995831102132797</v>
+        <v>-0.06332167237997055</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>0.7063965413335356</v>
       </c>
       <c r="B161" t="n">
-        <v>0.6980938911437988</v>
+        <v>0.7288205027580261</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>1.899995983477116</v>
       </c>
       <c r="B162" t="n">
-        <v>1.838457465171814</v>
+        <v>1.837308406829834</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>-0.7254992628556552</v>
       </c>
       <c r="B163" t="n">
-        <v>-0.7283318042755127</v>
+        <v>-0.7394642233848572</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>-0.7994949869867845</v>
       </c>
       <c r="B164" t="n">
-        <v>-0.7566605806350708</v>
+        <v>-0.7810518145561218</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>-0.1224415815200199</v>
       </c>
       <c r="B165" t="n">
-        <v>-0.1329578310251236</v>
+        <v>-0.1261846125125885</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>-0.966277435553859</v>
       </c>
       <c r="B166" t="n">
-        <v>-0.8960435390472412</v>
+        <v>-0.8997231125831604</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>2.284660552662082</v>
       </c>
       <c r="B167" t="n">
-        <v>2.120935916900635</v>
+        <v>2.11161470413208</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>1.997451666080566</v>
       </c>
       <c r="B168" t="n">
-        <v>1.85837733745575</v>
+        <v>1.890574097633362</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>-0.9071616811025665</v>
       </c>
       <c r="B169" t="n">
-        <v>-0.8661600947380066</v>
+        <v>-0.8447282910346985</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>-0.7535659267199135</v>
       </c>
       <c r="B170" t="n">
-        <v>-0.7622627019882202</v>
+        <v>-0.7641158699989319</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>-0.8255358417794756</v>
       </c>
       <c r="B171" t="n">
-        <v>-0.7805114984512329</v>
+        <v>-0.824252724647522</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>0.5552001126758501</v>
       </c>
       <c r="B172" t="n">
-        <v>0.5431728363037109</v>
+        <v>0.5896007418632507</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>-0.7705308456081058</v>
       </c>
       <c r="B173" t="n">
-        <v>-0.7464489936828613</v>
+        <v>-0.7475765347480774</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>-0.7915847343047725</v>
       </c>
       <c r="B174" t="n">
-        <v>-0.785540759563446</v>
+        <v>-0.7743589878082275</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>0.6531169845916236</v>
       </c>
       <c r="B175" t="n">
-        <v>0.5604187250137329</v>
+        <v>0.6172536015510559</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>0.1094634955674066</v>
       </c>
       <c r="B176" t="n">
-        <v>0.07441508024930954</v>
+        <v>0.08727958798408508</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>-0.8043169832275571</v>
       </c>
       <c r="B177" t="n">
-        <v>-0.7667728662490845</v>
+        <v>-0.797821581363678</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>-0.9204417544503384</v>
       </c>
       <c r="B178" t="n">
-        <v>-0.8693932890892029</v>
+        <v>-0.8575326800346375</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>-0.7709079936734142</v>
       </c>
       <c r="B179" t="n">
-        <v>-0.6842125654220581</v>
+        <v>-0.7283403277397156</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>2.258896722720663</v>
       </c>
       <c r="B180" t="n">
-        <v>2.107322692871094</v>
+        <v>2.148864269256592</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>-0.8555717684441614</v>
       </c>
       <c r="B181" t="n">
-        <v>-0.7825661897659302</v>
+        <v>-0.8178393840789795</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>-0.8523252861983566</v>
       </c>
       <c r="B182" t="n">
-        <v>-0.8416565656661987</v>
+        <v>-0.8284584879875183</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>-0.4121934939834374</v>
       </c>
       <c r="B183" t="n">
-        <v>-0.360899418592453</v>
+        <v>-0.3531922101974487</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>0.9920376955170304</v>
       </c>
       <c r="B184" t="n">
-        <v>0.9600711464881897</v>
+        <v>0.999491274356842</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>0.1137329984250247</v>
       </c>
       <c r="B185" t="n">
-        <v>0.1108575388789177</v>
+        <v>0.1159308180212975</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>-0.6991502568239089</v>
       </c>
       <c r="B186" t="n">
-        <v>-0.663044810295105</v>
+        <v>-0.6414822936058044</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>0.8551033777416818</v>
       </c>
       <c r="B187" t="n">
-        <v>0.8504955768585205</v>
+        <v>0.8764029145240784</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>-0.936393509416182</v>
       </c>
       <c r="B188" t="n">
-        <v>-0.8793033957481384</v>
+        <v>-0.8772793412208557</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>-0.8292570014389766</v>
       </c>
       <c r="B189" t="n">
-        <v>-0.763903021812439</v>
+        <v>-0.7606813907623291</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>-0.02585847532076373</v>
       </c>
       <c r="B190" t="n">
-        <v>-0.02072765491902828</v>
+        <v>-0.004172427114099264</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>-0.7596687738179716</v>
       </c>
       <c r="B191" t="n">
-        <v>-0.7181905508041382</v>
+        <v>-0.735381543636322</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>-0.4128466293537582</v>
       </c>
       <c r="B192" t="n">
-        <v>-0.3615787923336029</v>
+        <v>-0.3214117288589478</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>-0.537978858427915</v>
       </c>
       <c r="B193" t="n">
-        <v>-0.4964614510536194</v>
+        <v>-0.4566988050937653</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>0.2456595991791598</v>
       </c>
       <c r="B194" t="n">
-        <v>0.224776417016983</v>
+        <v>0.2066765129566193</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>1.599636198057128</v>
       </c>
       <c r="B195" t="n">
-        <v>1.634701371192932</v>
+        <v>1.702628135681152</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>1.339406626859971</v>
       </c>
       <c r="B196" t="n">
-        <v>1.309208989143372</v>
+        <v>1.340198040008545</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>0.9135934917985288</v>
       </c>
       <c r="B197" t="n">
-        <v>0.8515028953552246</v>
+        <v>0.8974428176879883</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>-1.106857690884899</v>
       </c>
       <c r="B198" t="n">
-        <v>-0.9678196310997009</v>
+        <v>-0.9951338171958923</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>-0.8678428280546225</v>
       </c>
       <c r="B199" t="n">
-        <v>-0.8169547319412231</v>
+        <v>-0.8078595995903015</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>1.870476754849634</v>
       </c>
       <c r="B200" t="n">
-        <v>1.8770672082901</v>
+        <v>1.898604035377502</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>2.024417493363552</v>
       </c>
       <c r="B201" t="n">
-        <v>1.946374654769897</v>
+        <v>2.007825613021851</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>0.6982746292145968</v>
       </c>
       <c r="B202" t="n">
-        <v>0.6911877393722534</v>
+        <v>0.7320733666419983</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>-0.06304983976371492</v>
       </c>
       <c r="B203" t="n">
-        <v>-0.1254282742738724</v>
+        <v>-0.0490315705537796</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>-0.7316685129143178</v>
       </c>
       <c r="B204" t="n">
-        <v>-0.6633538007736206</v>
+        <v>-0.6759035587310791</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>-0.8296035418896315</v>
       </c>
       <c r="B205" t="n">
-        <v>-0.7857041358947754</v>
+        <v>-0.8667067885398865</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>-1.006882327190386</v>
       </c>
       <c r="B206" t="n">
-        <v>-0.8951621055603027</v>
+        <v>-0.9106230139732361</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>1.688323058448875</v>
       </c>
       <c r="B207" t="n">
-        <v>1.577630519866943</v>
+        <v>1.647025942802429</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>0.7217330313675281</v>
       </c>
       <c r="B208" t="n">
-        <v>0.6302721500396729</v>
+        <v>0.6929500699043274</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>0.9051374897840485</v>
       </c>
       <c r="B209" t="n">
-        <v>0.8996624946594238</v>
+        <v>0.914975106716156</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>0.2945124648051479</v>
       </c>
       <c r="B210" t="n">
-        <v>0.2901941537857056</v>
+        <v>0.2970341145992279</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>-0.05332543744706258</v>
       </c>
       <c r="B211" t="n">
-        <v>-0.01386051066219807</v>
+        <v>-0.04585706070065498</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>0.7588481361604101</v>
       </c>
       <c r="B212" t="n">
-        <v>0.7920198440551758</v>
+        <v>0.8250479102134705</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>1.112597976998941</v>
       </c>
       <c r="B213" t="n">
-        <v>1.096576809883118</v>
+        <v>1.206270813941956</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>-0.04921104775523166</v>
       </c>
       <c r="B214" t="n">
-        <v>-0.06365817040205002</v>
+        <v>-0.05112218856811523</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>-0.226647021314292</v>
       </c>
       <c r="B215" t="n">
-        <v>-0.1604631245136261</v>
+        <v>-0.1606248766183853</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>1.652737296842416</v>
       </c>
       <c r="B216" t="n">
-        <v>1.60370409488678</v>
+        <v>1.557468891143799</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>-0.8060585046240363</v>
       </c>
       <c r="B217" t="n">
-        <v>-0.7862743735313416</v>
+        <v>-0.7697508931159973</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>-0.4118075267749236</v>
       </c>
       <c r="B218" t="n">
-        <v>-0.3618649840354919</v>
+        <v>-0.3647172152996063</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>0.06230442420996318</v>
       </c>
       <c r="B219" t="n">
-        <v>0.07698694616556168</v>
+        <v>0.08492389321327209</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>0.183530291617308</v>
       </c>
       <c r="B220" t="n">
-        <v>0.1386881023645401</v>
+        <v>0.1136712431907654</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>-0.3953437427300435</v>
       </c>
       <c r="B221" t="n">
-        <v>-0.3573647141456604</v>
+        <v>-0.3526947200298309</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>-0.712807478236989</v>
       </c>
       <c r="B222" t="n">
-        <v>-0.7423529624938965</v>
+        <v>-0.73491370677948</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>-0.8560106505119067</v>
       </c>
       <c r="B223" t="n">
-        <v>-0.8162196278572083</v>
+        <v>-0.833342432975769</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>-0.1769070536364781</v>
       </c>
       <c r="B224" t="n">
-        <v>-0.2175402790307999</v>
+        <v>-0.2116938382387161</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>1.220285422039912</v>
       </c>
       <c r="B225" t="n">
-        <v>1.175434708595276</v>
+        <v>1.164517045021057</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>-1.024724491440939</v>
       </c>
       <c r="B226" t="n">
-        <v>-0.9034916162490845</v>
+        <v>-0.9298508763313293</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>0.6476153955509141</v>
       </c>
       <c r="B227" t="n">
-        <v>0.6217923164367676</v>
+        <v>0.6272606253623962</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>0.6065866662674041</v>
       </c>
       <c r="B228" t="n">
-        <v>0.5555281639099121</v>
+        <v>0.5907828211784363</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>0.06469908097676323</v>
       </c>
       <c r="B229" t="n">
-        <v>0.04486875236034393</v>
+        <v>0.06849777698516846</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>-0.8232859227158682</v>
       </c>
       <c r="B230" t="n">
-        <v>-0.7347562313079834</v>
+        <v>-0.7582547068595886</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>-0.731389412970527</v>
       </c>
       <c r="B231" t="n">
-        <v>-0.7237917184829712</v>
+        <v>-0.7477736473083496</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>1.349083820821819</v>
       </c>
       <c r="B232" t="n">
-        <v>1.305959582328796</v>
+        <v>1.390584349632263</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>-0.8733905879038771</v>
       </c>
       <c r="B233" t="n">
-        <v>-0.8316587209701538</v>
+        <v>-0.8622172474861145</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>-0.9043032411577944</v>
       </c>
       <c r="B234" t="n">
-        <v>-0.8775666952133179</v>
+        <v>-0.8687654137611389</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>0.1081152042032574</v>
       </c>
       <c r="B235" t="n">
-        <v>0.09970645606517792</v>
+        <v>0.08575192093849182</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>-0.586966605067631</v>
       </c>
       <c r="B236" t="n">
-        <v>-0.5571165084838867</v>
+        <v>-0.5787181258201599</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>0.09326843600372303</v>
       </c>
       <c r="B237" t="n">
-        <v>0.1276002675294876</v>
+        <v>0.1133575141429901</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>0.05368448988649055</v>
       </c>
       <c r="B238" t="n">
-        <v>0.07000989466905594</v>
+        <v>0.1011259257793427</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>-0.8160687509351658</v>
       </c>
       <c r="B239" t="n">
-        <v>-0.787208080291748</v>
+        <v>-0.791614830493927</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>-0.07487838589452248</v>
       </c>
       <c r="B240" t="n">
-        <v>-0.0709928572177887</v>
+        <v>-0.02068472094833851</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>-1.099918581501728</v>
       </c>
       <c r="B241" t="n">
-        <v>-0.9502178430557251</v>
+        <v>-0.9812210202217102</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>0.05869376322709315</v>
       </c>
       <c r="B242" t="n">
-        <v>0.07072415202856064</v>
+        <v>0.06800322234630585</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>-0.9474475272643137</v>
       </c>
       <c r="B243" t="n">
-        <v>-0.8259662389755249</v>
+        <v>-0.862874448299408</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>1.075278475592948</v>
       </c>
       <c r="B244" t="n">
-        <v>1.006345272064209</v>
+        <v>1.046388387680054</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>-1.090806331478148</v>
       </c>
       <c r="B245" t="n">
-        <v>-0.9412247538566589</v>
+        <v>-0.9644597172737122</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>-0.8945072481492403</v>
       </c>
       <c r="B246" t="n">
-        <v>-0.901439905166626</v>
+        <v>-0.896949827671051</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>1.683496912023065</v>
       </c>
       <c r="B247" t="n">
-        <v>1.590735197067261</v>
+        <v>1.698762655258179</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>-0.6850857985039962</v>
       </c>
       <c r="B248" t="n">
-        <v>-0.6799934506416321</v>
+        <v>-0.6689207553863525</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>0.2356000694207066</v>
       </c>
       <c r="B249" t="n">
-        <v>0.2229594141244888</v>
+        <v>0.1961732655763626</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>2.224613600442937</v>
       </c>
       <c r="B250" t="n">
-        <v>2.114142179489136</v>
+        <v>2.125756740570068</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>1.704961150265342</v>
       </c>
       <c r="B251" t="n">
-        <v>1.600760102272034</v>
+        <v>1.653761625289917</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>-0.5743272165350668</v>
       </c>
       <c r="B252" t="n">
-        <v>-0.5969573855400085</v>
+        <v>-0.5349127054214478</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>-0.8078653914348605</v>
       </c>
       <c r="B253" t="n">
-        <v>-0.7662280797958374</v>
+        <v>-0.7678986787796021</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>0.1764687517755223</v>
       </c>
       <c r="B254" t="n">
-        <v>0.1694416254758835</v>
+        <v>0.1668031811714172</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>1.782181568170828</v>
       </c>
       <c r="B255" t="n">
-        <v>1.692339062690735</v>
+        <v>1.730459690093994</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>-0.9607369385284205</v>
       </c>
       <c r="B256" t="n">
-        <v>-0.9330471754074097</v>
+        <v>-0.9239709973335266</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>1.680782172235226</v>
       </c>
       <c r="B257" t="n">
-        <v>1.633057951927185</v>
+        <v>1.63128936290741</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>0.9904201608985549</v>
       </c>
       <c r="B258" t="n">
-        <v>0.868266224861145</v>
+        <v>0.9652937054634094</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>0.2298053735617039</v>
       </c>
       <c r="B259" t="n">
-        <v>0.2151342779397964</v>
+        <v>0.2129472196102142</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>-1.09912900879829</v>
       </c>
       <c r="B260" t="n">
-        <v>-0.9577476382255554</v>
+        <v>-0.9569712281227112</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>0.61894176712488</v>
       </c>
       <c r="B261" t="n">
-        <v>0.5758827328681946</v>
+        <v>0.6032124161720276</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>-0.4042718282925715</v>
       </c>
       <c r="B262" t="n">
-        <v>-0.341363936662674</v>
+        <v>-0.3521247804164886</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>-0.2848279465858243</v>
       </c>
       <c r="B263" t="n">
-        <v>-0.2458028346300125</v>
+        <v>-0.2460187077522278</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>-0.9286824656159837</v>
       </c>
       <c r="B264" t="n">
-        <v>-0.8365569114685059</v>
+        <v>-0.8613945841789246</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>-0.8362734080184764</v>
       </c>
       <c r="B265" t="n">
-        <v>-0.8204922676086426</v>
+        <v>-0.8215250372886658</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>-0.3976144127188398</v>
       </c>
       <c r="B266" t="n">
-        <v>-0.329404354095459</v>
+        <v>-0.3661610782146454</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>-0.8612580407190521</v>
       </c>
       <c r="B267" t="n">
-        <v>-0.7968140840530396</v>
+        <v>-0.8117005228996277</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>-0.8639852310620044</v>
       </c>
       <c r="B268" t="n">
-        <v>-0.8071865439414978</v>
+        <v>-0.800653874874115</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>-0.2822885521158316</v>
       </c>
       <c r="B269" t="n">
-        <v>-0.2570815682411194</v>
+        <v>-0.2328218519687653</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>-0.8174938207225141</v>
       </c>
       <c r="B270" t="n">
-        <v>-0.7521337866783142</v>
+        <v>-0.7742054462432861</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>1.091539419344106</v>
       </c>
       <c r="B271" t="n">
-        <v>1.050536036491394</v>
+        <v>1.099750995635986</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>-1.10844513666185</v>
       </c>
       <c r="B272" t="n">
-        <v>-0.9707196950912476</v>
+        <v>-0.9844775199890137</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>0.8675425198461729</v>
       </c>
       <c r="B273" t="n">
-        <v>0.7888180017471313</v>
+        <v>0.8769569396972656</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>0.5060982359475952</v>
       </c>
       <c r="B274" t="n">
-        <v>0.4574808180332184</v>
+        <v>0.4624996781349182</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>-1.075359342767525</v>
       </c>
       <c r="B275" t="n">
-        <v>-1.009173989295959</v>
+        <v>-1.007972836494446</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>-0.6342937589191047</v>
       </c>
       <c r="B276" t="n">
-        <v>-0.6868785619735718</v>
+        <v>-0.6843162178993225</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>-0.9732289954921434</v>
       </c>
       <c r="B277" t="n">
-        <v>-0.899221658706665</v>
+        <v>-0.962644636631012</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>1.889277093070785</v>
       </c>
       <c r="B278" t="n">
-        <v>1.694182753562927</v>
+        <v>1.842662215232849</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>-0.8624569254218413</v>
       </c>
       <c r="B279" t="n">
-        <v>-0.8429638743400574</v>
+        <v>-0.8804523348808289</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>-0.2841514664246659</v>
       </c>
       <c r="B280" t="n">
-        <v>-0.3071659505367279</v>
+        <v>-0.2946175932884216</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>-0.2181806438372174</v>
       </c>
       <c r="B281" t="n">
-        <v>-0.2428049594163895</v>
+        <v>-0.2340592741966248</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>-0.9213605016630773</v>
       </c>
       <c r="B282" t="n">
-        <v>-0.8790357708930969</v>
+        <v>-0.8753619790077209</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>-0.7280407324181668</v>
       </c>
       <c r="B283" t="n">
-        <v>-0.6667448282241821</v>
+        <v>-0.6915467381477356</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>-1.081007744603946</v>
       </c>
       <c r="B284" t="n">
-        <v>-0.9523096084594727</v>
+        <v>-0.9526404142379761</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>1.399995696999676</v>
       </c>
       <c r="B285" t="n">
-        <v>1.303267121315002</v>
+        <v>1.393315553665161</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>0.8496246147186801</v>
       </c>
       <c r="B286" t="n">
-        <v>0.7790606021881104</v>
+        <v>0.8629680275917053</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>1.729915694124394</v>
       </c>
       <c r="B287" t="n">
-        <v>1.622748970985413</v>
+        <v>1.705336093902588</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>0.9465226162076782</v>
       </c>
       <c r="B288" t="n">
-        <v>1.035087704658508</v>
+        <v>0.9749941229820251</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>-0.9626169723505357</v>
       </c>
       <c r="B289" t="n">
-        <v>-0.877683699131012</v>
+        <v>-0.8825241923332214</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>-0.8460263428572634</v>
       </c>
       <c r="B290" t="n">
-        <v>-0.8202800154685974</v>
+        <v>-0.8116410970687866</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>-0.4471920044070506</v>
       </c>
       <c r="B291" t="n">
-        <v>-0.425995945930481</v>
+        <v>-0.4053972065448761</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>0.2662087216206063</v>
       </c>
       <c r="B292" t="n">
-        <v>0.2506003975868225</v>
+        <v>0.2524116635322571</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>1.874892551729834</v>
       </c>
       <c r="B293" t="n">
-        <v>1.816370129585266</v>
+        <v>1.824955105781555</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>-0.8776969236537053</v>
       </c>
       <c r="B294" t="n">
-        <v>-0.8177652955055237</v>
+        <v>-0.8205312490463257</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>1.700074307383354</v>
       </c>
       <c r="B295" t="n">
-        <v>1.647088766098022</v>
+        <v>1.666708469390869</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>-0.9023671798376692</v>
       </c>
       <c r="B296" t="n">
-        <v>-0.8600659370422363</v>
+        <v>-0.847761332988739</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>-0.4432021202663532</v>
       </c>
       <c r="B297" t="n">
-        <v>-0.4277268648147583</v>
+        <v>-0.3701789975166321</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>0.1462891249539033</v>
       </c>
       <c r="B298" t="n">
-        <v>0.1451821178197861</v>
+        <v>0.1931021362543106</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>-0.596786980413282</v>
       </c>
       <c r="B299" t="n">
-        <v>-0.5771050453186035</v>
+        <v>-0.5742086172103882</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>-0.1069883675318396</v>
       </c>
       <c r="B300" t="n">
-        <v>-0.08381879329681396</v>
+        <v>-0.08510207384824753</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>-0.1334416469626604</v>
       </c>
       <c r="B301" t="n">
-        <v>-0.1401930600404739</v>
+        <v>-0.1550768464803696</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>2.121347658786593</v>
       </c>
       <c r="B302" t="n">
-        <v>1.972102284431458</v>
+        <v>2.016368627548218</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>0.3467487687831875</v>
       </c>
       <c r="B303" t="n">
-        <v>0.3349473476409912</v>
+        <v>0.3079667389392853</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>-0.1253290727600566</v>
       </c>
       <c r="B304" t="n">
-        <v>-0.1339822560548782</v>
+        <v>-0.08939878642559052</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>-0.6738974184152664</v>
       </c>
       <c r="B305" t="n">
-        <v>-0.6845856904983521</v>
+        <v>-0.6722972989082336</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>0.09283214780162605</v>
       </c>
       <c r="B306" t="n">
-        <v>0.09591351449489594</v>
+        <v>0.09135846048593521</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>-0.7469277057519816</v>
       </c>
       <c r="B307" t="n">
-        <v>-0.7678534388542175</v>
+        <v>-0.7528253793716431</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>-0.8954903232300648</v>
       </c>
       <c r="B308" t="n">
-        <v>-0.8759214878082275</v>
+        <v>-0.9080401062965393</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>-0.9416383057576788</v>
       </c>
       <c r="B309" t="n">
-        <v>-0.8648530840873718</v>
+        <v>-0.8884111046791077</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>0.2817044750054237</v>
       </c>
       <c r="B310" t="n">
-        <v>0.2770715951919556</v>
+        <v>0.2414872646331787</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>-1.07907272083008</v>
       </c>
       <c r="B311" t="n">
-        <v>-0.9822216629981995</v>
+        <v>-0.9890986680984497</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>-0.6717777114072194</v>
       </c>
       <c r="B312" t="n">
-        <v>-0.6868020296096802</v>
+        <v>-0.670407235622406</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>1.23561101783818</v>
       </c>
       <c r="B313" t="n">
-        <v>1.189491271972656</v>
+        <v>1.247822999954224</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>0.1396918870632196</v>
       </c>
       <c r="B314" t="n">
-        <v>0.1568956822156906</v>
+        <v>0.1733015477657318</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>-0.8097755140984995</v>
       </c>
       <c r="B315" t="n">
-        <v>-0.7663356065750122</v>
+        <v>-0.7626837491989136</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>0.7946569702126504</v>
       </c>
       <c r="B316" t="n">
-        <v>0.6554189920425415</v>
+        <v>0.7466710209846497</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>0.9756003689017658</v>
       </c>
       <c r="B317" t="n">
-        <v>0.8804316520690918</v>
+        <v>1.00387716293335</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>-0.4146913866030522</v>
       </c>
       <c r="B318" t="n">
-        <v>-0.3391929268836975</v>
+        <v>-0.3522078096866608</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>-0.07125838699531742</v>
       </c>
       <c r="B319" t="n">
-        <v>-0.1166592314839363</v>
+        <v>-0.1026359125971794</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>-0.8360129839073556</v>
       </c>
       <c r="B320" t="n">
-        <v>-0.857485294342041</v>
+        <v>-0.8690365552902222</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>0.01185736875633715</v>
       </c>
       <c r="B321" t="n">
-        <v>0.003732709214091301</v>
+        <v>0.03716159611940384</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>-0.53907346973163</v>
       </c>
       <c r="B322" t="n">
-        <v>-0.5614511966705322</v>
+        <v>-0.4897429645061493</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>0.08939371949782395</v>
       </c>
       <c r="B323" t="n">
-        <v>0.1313912570476532</v>
+        <v>0.1064737588167191</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>-0.757694323286247</v>
       </c>
       <c r="B324" t="n">
-        <v>-0.7502779960632324</v>
+        <v>-0.7577665448188782</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>-0.890566128682737</v>
       </c>
       <c r="B325" t="n">
-        <v>-0.8680418729782104</v>
+        <v>-0.8559704422950745</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>-0.8965439514565318</v>
       </c>
       <c r="B326" t="n">
-        <v>-0.894923210144043</v>
+        <v>-0.8784123659133911</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>-0.4398342451081933</v>
       </c>
       <c r="B327" t="n">
-        <v>-0.4215307235717773</v>
+        <v>-0.4450165331363678</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>-1.104644604713502</v>
       </c>
       <c r="B328" t="n">
-        <v>-0.9485217332839966</v>
+        <v>-0.9439288973808289</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>0.1293107179643383</v>
       </c>
       <c r="B329" t="n">
-        <v>0.1759937256574631</v>
+        <v>0.1611582934856415</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>-0.8601374907588512</v>
       </c>
       <c r="B330" t="n">
-        <v>-0.8548176288604736</v>
+        <v>-0.8410223126411438</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>-1.062155529069822</v>
       </c>
       <c r="B331" t="n">
-        <v>-1.006106495857239</v>
+        <v>-1.011366844177246</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>2.222412446053525</v>
       </c>
       <c r="B332" t="n">
-        <v>2.13770580291748</v>
+        <v>2.168389081954956</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>-0.1203109802762487</v>
       </c>
       <c r="B333" t="n">
-        <v>-0.0951475203037262</v>
+        <v>-0.1086079776287079</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>1.114489942603039</v>
       </c>
       <c r="B334" t="n">
-        <v>1.039958477020264</v>
+        <v>1.062146902084351</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>1.390208523134328</v>
       </c>
       <c r="B335" t="n">
-        <v>1.361595869064331</v>
+        <v>1.404470562934875</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>-0.8323317697788432</v>
       </c>
       <c r="B336" t="n">
-        <v>-0.82859206199646</v>
+        <v>-0.8247793912887573</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>0.301702141609975</v>
       </c>
       <c r="B337" t="n">
-        <v>0.2994314432144165</v>
+        <v>0.2939249277114868</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>-0.1918746959752379</v>
       </c>
       <c r="B338" t="n">
-        <v>-0.1399580389261246</v>
+        <v>-0.167205423116684</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>-0.9368064528274415</v>
       </c>
       <c r="B339" t="n">
-        <v>-0.8723572492599487</v>
+        <v>-0.8789278268814087</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>-0.8811981235062041</v>
       </c>
       <c r="B340" t="n">
-        <v>-0.8385719060897827</v>
+        <v>-0.8520898818969727</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>1.849821802689724</v>
       </c>
       <c r="B341" t="n">
-        <v>1.867015480995178</v>
+        <v>1.806525945663452</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>-0.6904239740088429</v>
       </c>
       <c r="B342" t="n">
-        <v>-0.691053032875061</v>
+        <v>-0.6845597624778748</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>1.200486964317174</v>
       </c>
       <c r="B343" t="n">
-        <v>1.248749971389771</v>
+        <v>1.273555040359497</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>0.1516988911506519</v>
       </c>
       <c r="B344" t="n">
-        <v>0.1198946163058281</v>
+        <v>0.1666827797889709</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>-0.9777734481085145</v>
       </c>
       <c r="B345" t="n">
-        <v>-0.8197280168533325</v>
+        <v>-0.841117799282074</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>1.565631656950064</v>
       </c>
       <c r="B346" t="n">
-        <v>1.459617853164673</v>
+        <v>1.522865533828735</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>1.474861403669351</v>
       </c>
       <c r="B347" t="n">
-        <v>1.547811627388</v>
+        <v>1.521874666213989</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>-0.287524529314123</v>
       </c>
       <c r="B348" t="n">
-        <v>-0.2872824668884277</v>
+        <v>-0.2877379953861237</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>0.4466945624093063</v>
       </c>
       <c r="B349" t="n">
-        <v>0.4341274499893188</v>
+        <v>0.4439692795276642</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>2.267950351380584</v>
       </c>
       <c r="B350" t="n">
-        <v>2.128541469573975</v>
+        <v>2.197445154190063</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>0.9714143885180335</v>
       </c>
       <c r="B351" t="n">
-        <v>0.9792021512985229</v>
+        <v>0.986139714717865</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>-0.8981630423943963</v>
       </c>
       <c r="B352" t="n">
-        <v>-0.8281189203262329</v>
+        <v>-0.859636127948761</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>-0.2806985124732314</v>
       </c>
       <c r="B353" t="n">
-        <v>-0.2637120485305786</v>
+        <v>-0.2477659583091736</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>-1.106860284750548</v>
       </c>
       <c r="B354" t="n">
-        <v>-0.989129900932312</v>
+        <v>-1.007846117019653</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>0.5631025837609164</v>
       </c>
       <c r="B355" t="n">
-        <v>0.5119968056678772</v>
+        <v>0.5613430142402649</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>1.98709799195756</v>
       </c>
       <c r="B356" t="n">
-        <v>1.917120575904846</v>
+        <v>1.953470826148987</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>0.1580512681241064</v>
       </c>
       <c r="B357" t="n">
-        <v>0.1941527426242828</v>
+        <v>0.1814253032207489</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>-0.7468659717495447</v>
       </c>
       <c r="B358" t="n">
-        <v>-0.7294808626174927</v>
+        <v>-0.7352514863014221</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>1.175777800148481</v>
       </c>
       <c r="B359" t="n">
-        <v>1.077833414077759</v>
+        <v>1.170133352279663</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>-0.9901467060255309</v>
       </c>
       <c r="B360" t="n">
-        <v>-0.9046428799629211</v>
+        <v>-0.9621288180351257</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>0.2642539844678111</v>
       </c>
       <c r="B361" t="n">
-        <v>0.2788719236850739</v>
+        <v>0.2852362990379333</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>-1.016792450287479</v>
       </c>
       <c r="B362" t="n">
-        <v>-0.9318000674247742</v>
+        <v>-0.9513009190559387</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>-0.9485436948874179</v>
       </c>
       <c r="B363" t="n">
-        <v>-0.8369209170341492</v>
+        <v>-0.9097982048988342</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>2.020818245389536</v>
       </c>
       <c r="B364" t="n">
-        <v>1.923815369606018</v>
+        <v>1.886515140533447</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>-0.7316560623592044</v>
       </c>
       <c r="B365" t="n">
-        <v>-0.6873506307601929</v>
+        <v>-0.6817764043807983</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>-0.1701069754520728</v>
       </c>
       <c r="B366" t="n">
-        <v>-0.1735950112342834</v>
+        <v>-0.197140246629715</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>-0.4186376938008529</v>
       </c>
       <c r="B367" t="n">
-        <v>-0.4040942192077637</v>
+        <v>-0.3667791187763214</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>-0.782087035845809</v>
       </c>
       <c r="B368" t="n">
-        <v>-0.7197036743164062</v>
+        <v>-0.7274958491325378</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>-1.092272384342745</v>
       </c>
       <c r="B369" t="n">
-        <v>-0.9660731554031372</v>
+        <v>-0.9812453389167786</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>-1.100688959599366</v>
       </c>
       <c r="B370" t="n">
-        <v>-0.9483243227005005</v>
+        <v>-0.9434719085693359</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>0.1571771354005237</v>
       </c>
       <c r="B371" t="n">
-        <v>0.1824150085449219</v>
+        <v>0.1598533987998962</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>-0.7914923926876819</v>
       </c>
       <c r="B372" t="n">
-        <v>-0.815521240234375</v>
+        <v>-0.8136443495750427</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>-0.8727141077427187</v>
       </c>
       <c r="B373" t="n">
-        <v>-0.8172789216041565</v>
+        <v>-0.8265408277511597</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>-0.9536219650542735</v>
       </c>
       <c r="B374" t="n">
-        <v>-0.9283841252326965</v>
+        <v>-0.9116995930671692</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>1.289727355638335</v>
       </c>
       <c r="B375" t="n">
-        <v>1.415268301963806</v>
+        <v>1.430945158004761</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>-0.8412017527508422</v>
       </c>
       <c r="B376" t="n">
-        <v>-0.8367971181869507</v>
+        <v>-0.853459894657135</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>1.015725914166429</v>
       </c>
       <c r="B377" t="n">
-        <v>0.9768179655075073</v>
+        <v>1.002236008644104</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>1.776465207054413</v>
       </c>
       <c r="B378" t="n">
-        <v>1.747915744781494</v>
+        <v>1.791614055633545</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>-0.9054704806996705</v>
       </c>
       <c r="B379" t="n">
-        <v>-0.8698152899742126</v>
+        <v>-0.8640549778938293</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>0.4716636319159906</v>
       </c>
       <c r="B380" t="n">
-        <v>0.4660473167896271</v>
+        <v>0.4992682635784149</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>-0.9641483906294771</v>
       </c>
       <c r="B381" t="n">
-        <v>-0.9200148582458496</v>
+        <v>-0.9060474038124084</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>-0.7284412252743128</v>
       </c>
       <c r="B382" t="n">
-        <v>-0.6734302043914795</v>
+        <v>-0.6725446581840515</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>-0.8666257862922931</v>
       </c>
       <c r="B383" t="n">
-        <v>-0.8161813020706177</v>
+        <v>-0.8331893086433411</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>-0.9915971956962357</v>
       </c>
       <c r="B384" t="n">
-        <v>-0.9051910042762756</v>
+        <v>-0.9097645878791809</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>2.218046451393778</v>
       </c>
       <c r="B385" t="n">
-        <v>1.966253399848938</v>
+        <v>2.028810024261475</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>-1.094872475268915</v>
       </c>
       <c r="B386" t="n">
-        <v>-1.008435249328613</v>
+        <v>-1.021924495697021</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>-0.005177584504367607</v>
       </c>
       <c r="B387" t="n">
-        <v>-0.000714251771569252</v>
+        <v>0.02170645631849766</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>1.159561470886479</v>
       </c>
       <c r="B388" t="n">
-        <v>1.075405240058899</v>
+        <v>1.186634659767151</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>0.06670310157688213</v>
       </c>
       <c r="B389" t="n">
-        <v>0.05005588382482529</v>
+        <v>0.04128504917025566</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>1.87553583041069</v>
       </c>
       <c r="B390" t="n">
-        <v>1.740333676338196</v>
+        <v>1.748545408248901</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>-0.7537127395156251</v>
       </c>
       <c r="B391" t="n">
-        <v>-0.6562466621398926</v>
+        <v>-0.6721801161766052</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>0.2524933976169971</v>
       </c>
       <c r="B392" t="n">
-        <v>0.2339428216218948</v>
+        <v>0.2138656675815582</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>1.709649821811776</v>
       </c>
       <c r="B393" t="n">
-        <v>1.68450665473938</v>
+        <v>1.71156644821167</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>0.1265876778064237</v>
       </c>
       <c r="B394" t="n">
-        <v>0.1040517166256905</v>
+        <v>0.1469692885875702</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>0.2943889968002739</v>
       </c>
       <c r="B395" t="n">
-        <v>0.2930953502655029</v>
+        <v>0.3242774307727814</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>0.127068061724547</v>
       </c>
       <c r="B396" t="n">
-        <v>0.09226864576339722</v>
+        <v>0.1214819401502609</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>-0.9272765904344351</v>
       </c>
       <c r="B397" t="n">
-        <v>-0.8676106333732605</v>
+        <v>-0.9050241112709045</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>-0.7991811292433022</v>
       </c>
       <c r="B398" t="n">
-        <v>-0.7570921182632446</v>
+        <v>-0.7630641460418701</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>0.135648050517031</v>
       </c>
       <c r="B399" t="n">
-        <v>0.199996218085289</v>
+        <v>0.163777083158493</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>0.2315282191255129</v>
       </c>
       <c r="B400" t="n">
-        <v>0.2188598215579987</v>
+        <v>0.2149533629417419</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>-0.8513209414192133</v>
       </c>
       <c r="B401" t="n">
-        <v>-0.7988958954811096</v>
+        <v>-0.8150321841239929</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>-0.8754636053302491</v>
       </c>
       <c r="B402" t="n">
-        <v>-0.8334415555000305</v>
+        <v>-0.8476232290267944</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>0.992539867906602</v>
       </c>
       <c r="B403" t="n">
-        <v>0.8722559213638306</v>
+        <v>1.040701389312744</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>1.115707503138499</v>
       </c>
       <c r="B404" t="n">
-        <v>1.173800826072693</v>
+        <v>1.19044029712677</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>-0.8905069885459483</v>
       </c>
       <c r="B405" t="n">
-        <v>-0.8626396059989929</v>
+        <v>-0.8643239140510559</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>-0.06646907346171733</v>
       </c>
       <c r="B406" t="n">
-        <v>-0.02165241353213787</v>
+        <v>-0.04465002939105034</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>0.9598820618442974</v>
       </c>
       <c r="B407" t="n">
-        <v>0.888774037361145</v>
+        <v>0.9152909517288208</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>-0.8028286231183825</v>
       </c>
       <c r="B408" t="n">
-        <v>-0.7471755146980286</v>
+        <v>-0.7723750472068787</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>-0.7715927742046482</v>
       </c>
       <c r="B409" t="n">
-        <v>-0.7101999521255493</v>
+        <v>-0.7635798454284668</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>1.144634811624967</v>
       </c>
       <c r="B410" t="n">
-        <v>1.101114869117737</v>
+        <v>1.192249059677124</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>-0.9488554775383812</v>
       </c>
       <c r="B411" t="n">
-        <v>-0.8233424425125122</v>
+        <v>-0.8872519135475159</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>-0.8247032109062706</v>
       </c>
       <c r="B412" t="n">
-        <v>-0.7175000905990601</v>
+        <v>-0.7381194829940796</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>-0.08393875860512977</v>
       </c>
       <c r="B413" t="n">
-        <v>-0.07773364335298538</v>
+        <v>-0.09775663912296295</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>0.9687556762282046</v>
       </c>
       <c r="B414" t="n">
-        <v>0.9439218640327454</v>
+        <v>0.9873389601707458</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>0.2770100969545629</v>
       </c>
       <c r="B415" t="n">
-        <v>0.2832261025905609</v>
+        <v>0.2769714295864105</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>-0.8726907629518812</v>
       </c>
       <c r="B416" t="n">
-        <v>-0.7979111075401306</v>
+        <v>-0.7718469500541687</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>-0.5695721420280283</v>
       </c>
       <c r="B417" t="n">
-        <v>-0.5058854222297668</v>
+        <v>-0.5331407189369202</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>-0.8020343814567772</v>
       </c>
       <c r="B418" t="n">
-        <v>-0.7780278921127319</v>
+        <v>-0.7912917137145996</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>-0.8630607773448385</v>
       </c>
       <c r="B419" t="n">
-        <v>-0.8286837935447693</v>
+        <v>-0.8105750679969788</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>2.150731487627218</v>
       </c>
       <c r="B420" t="n">
-        <v>2.065459728240967</v>
+        <v>2.058951616287231</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>0.7615545755781734</v>
       </c>
       <c r="B421" t="n">
-        <v>0.7392807602882385</v>
+        <v>0.8060574531555176</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>-0.2004868487017646</v>
       </c>
       <c r="B422" t="n">
-        <v>-0.1351470798254013</v>
+        <v>-0.2014394700527191</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>0.3430986810424584</v>
       </c>
       <c r="B423" t="n">
-        <v>0.3088289201259613</v>
+        <v>0.3338907361030579</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>0.1025907891448401</v>
       </c>
       <c r="B424" t="n">
-        <v>0.06661038845777512</v>
+        <v>0.1218747645616531</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>1.774399971224987</v>
       </c>
       <c r="B425" t="n">
-        <v>1.66770350933075</v>
+        <v>1.743453741073608</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>-0.235186027029528</v>
       </c>
       <c r="B426" t="n">
-        <v>-0.2594754099845886</v>
+        <v>-0.2401512265205383</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>0.2860730635308188</v>
       </c>
       <c r="B427" t="n">
-        <v>0.2443059533834457</v>
+        <v>0.2772018015384674</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>1.873048832026799</v>
       </c>
       <c r="B428" t="n">
-        <v>1.714582800865173</v>
+        <v>1.750796556472778</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>1.794373774265571</v>
       </c>
       <c r="B429" t="n">
-        <v>1.690865397453308</v>
+        <v>1.748290538787842</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>-0.9700764111828186</v>
       </c>
       <c r="B430" t="n">
-        <v>-0.899070143699646</v>
+        <v>-0.8992649912834167</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>-0.3846118829954697</v>
       </c>
       <c r="B431" t="n">
-        <v>-0.3017586171627045</v>
+        <v>-0.3316647112369537</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>2.34017498404684</v>
       </c>
       <c r="B432" t="n">
-        <v>2.129905939102173</v>
+        <v>2.187974214553833</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>1.915091244005787</v>
       </c>
       <c r="B433" t="n">
-        <v>1.63158655166626</v>
+        <v>1.771507263183594</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>-1.094866249991358</v>
       </c>
       <c r="B434" t="n">
-        <v>-0.9984585046768188</v>
+        <v>-1.003798484802246</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>0.2241963984831419</v>
       </c>
       <c r="B435" t="n">
-        <v>0.2151209264993668</v>
+        <v>0.2177698314189911</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>0.424094729786066</v>
       </c>
       <c r="B436" t="n">
-        <v>0.3105767965316772</v>
+        <v>0.3664751648902893</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>-0.9589632531978985</v>
       </c>
       <c r="B437" t="n">
-        <v>-0.8855764865875244</v>
+        <v>-0.8994688391685486</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>0.618371116682185</v>
       </c>
       <c r="B438" t="n">
-        <v>0.6838040351867676</v>
+        <v>0.5772818922996521</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>0.09613880773047871</v>
       </c>
       <c r="B439" t="n">
-        <v>0.1207685992121696</v>
+        <v>0.1242863386869431</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>-0.8825479711897426</v>
       </c>
       <c r="B440" t="n">
-        <v>-0.860135018825531</v>
+        <v>-0.8900942802429199</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>-1.084670282899788</v>
       </c>
       <c r="B441" t="n">
-        <v>-0.9887017011642456</v>
+        <v>-0.9940475225448608</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>-0.8029557225351647</v>
       </c>
       <c r="B442" t="n">
-        <v>-0.7705681920051575</v>
+        <v>-0.7811089754104614</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>-0.8966067230052281</v>
       </c>
       <c r="B443" t="n">
-        <v>-0.8732578754425049</v>
+        <v>-0.8437594175338745</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>-0.9512345711112896</v>
       </c>
       <c r="B444" t="n">
-        <v>-0.8415963649749756</v>
+        <v>-0.9069764018058777</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>0.8761463722026241</v>
       </c>
       <c r="B445" t="n">
-        <v>0.8772636651992798</v>
+        <v>0.9281185269355774</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>-1.080011700194878</v>
       </c>
       <c r="B446" t="n">
-        <v>-1.007094740867615</v>
+        <v>-1.004362821578979</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>-0.6780481222261779</v>
       </c>
       <c r="B447" t="n">
-        <v>-0.653323233127594</v>
+        <v>-0.6481716632843018</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>0.8868118289765936</v>
       </c>
       <c r="B448" t="n">
-        <v>0.8486157655715942</v>
+        <v>0.8868761658668518</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>-0.3964663677827634</v>
       </c>
       <c r="B449" t="n">
-        <v>-0.3817831873893738</v>
+        <v>-0.3494722843170166</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>-0.8229113685162084</v>
       </c>
       <c r="B450" t="n">
-        <v>-0.8169816732406616</v>
+        <v>-0.8117285966873169</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>-0.7461163445770954</v>
       </c>
       <c r="B451" t="n">
-        <v>-0.7279256582260132</v>
+        <v>-0.7413066029548645</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>-0.7174748800851043</v>
       </c>
       <c r="B452" t="n">
-        <v>-0.7035702466964722</v>
+        <v>-0.7289471626281738</v>
       </c>
     </row>
     <row r="453">
@@ -4058,7 +4058,7 @@
         <v>-1.024331261408609</v>
       </c>
       <c r="B453" t="n">
-        <v>-0.9146661758422852</v>
+        <v>-0.9375017285346985</v>
       </c>
     </row>
     <row r="454">
@@ -4066,7 +4066,7 @@
         <v>-1.098185879248454</v>
       </c>
       <c r="B454" t="n">
-        <v>-0.953532338142395</v>
+        <v>-0.9528211355209351</v>
       </c>
     </row>
     <row r="455">
@@ -4074,7 +4074,7 @@
         <v>-0.695675514401026</v>
       </c>
       <c r="B455" t="n">
-        <v>-0.6141995191574097</v>
+        <v>-0.6287524104118347</v>
       </c>
     </row>
     <row r="456">
@@ -4082,7 +4082,7 @@
         <v>-0.7579397029766058</v>
       </c>
       <c r="B456" t="n">
-        <v>-0.7681107521057129</v>
+        <v>-0.7981243133544922</v>
       </c>
     </row>
     <row r="457">
@@ -4090,7 +4090,7 @@
         <v>1.389398199505701</v>
       </c>
       <c r="B457" t="n">
-        <v>1.352487564086914</v>
+        <v>1.421605229377747</v>
       </c>
     </row>
     <row r="458">
@@ -4098,7 +4098,7 @@
         <v>-0.8381186840409001</v>
       </c>
       <c r="B458" t="n">
-        <v>-0.7994384765625</v>
+        <v>-0.8166868686676025</v>
       </c>
     </row>
     <row r="459">
@@ -4106,7 +4106,7 @@
         <v>0.5135291422577432</v>
       </c>
       <c r="B459" t="n">
-        <v>0.4502913653850555</v>
+        <v>0.4944556355476379</v>
       </c>
     </row>
     <row r="460">
@@ -4114,7 +4114,7 @@
         <v>-0.722637191498975</v>
       </c>
       <c r="B460" t="n">
-        <v>-0.6712788939476013</v>
+        <v>-0.6763380169868469</v>
       </c>
     </row>
     <row r="461">
@@ -4122,7 +4122,7 @@
         <v>-1.071393840963924</v>
       </c>
       <c r="B461" t="n">
-        <v>-0.9722374677658081</v>
+        <v>-0.99025559425354</v>
       </c>
     </row>
     <row r="462">
@@ -4130,7 +4130,7 @@
         <v>-1.004096515483775</v>
       </c>
       <c r="B462" t="n">
-        <v>-0.9226707220077515</v>
+        <v>-0.9470358490943909</v>
       </c>
     </row>
     <row r="463">
@@ -4138,7 +4138,7 @@
         <v>-0.3946086412052265</v>
       </c>
       <c r="B463" t="n">
-        <v>-0.3432632982730865</v>
+        <v>-0.3363007009029388</v>
       </c>
     </row>
     <row r="464">
@@ -4146,7 +4146,7 @@
         <v>0.08143470214161815</v>
       </c>
       <c r="B464" t="n">
-        <v>0.07645226269960403</v>
+        <v>0.07506240904331207</v>
       </c>
     </row>
     <row r="465">
@@ -4154,7 +4154,7 @@
         <v>-0.0924673888577711</v>
       </c>
       <c r="B465" t="n">
-        <v>-0.1055082902312279</v>
+        <v>-0.09182256460189819</v>
       </c>
     </row>
     <row r="466">
@@ -4162,7 +4162,7 @@
         <v>-1.069150147177873</v>
       </c>
       <c r="B466" t="n">
-        <v>-1.021798372268677</v>
+        <v>-1.001758456230164</v>
       </c>
     </row>
     <row r="467">
@@ -4170,7 +4170,7 @@
         <v>-1.085872799014485</v>
       </c>
       <c r="B467" t="n">
-        <v>-0.9639632701873779</v>
+        <v>-0.9946860671043396</v>
       </c>
     </row>
     <row r="468">
@@ -4178,7 +4178,7 @@
         <v>-0.7123385073277196</v>
       </c>
       <c r="B468" t="n">
-        <v>-0.6765249967575073</v>
+        <v>-0.6892541646957397</v>
       </c>
     </row>
     <row r="469">
@@ -4186,7 +4186,7 @@
         <v>-0.9475191179562156</v>
       </c>
       <c r="B469" t="n">
-        <v>-0.7970774173736572</v>
+        <v>-0.8614910840988159</v>
       </c>
     </row>
     <row r="470">
@@ -4194,7 +4194,7 @@
         <v>-0.6753774781543653</v>
       </c>
       <c r="B470" t="n">
-        <v>-0.607308030128479</v>
+        <v>-0.6173481345176697</v>
       </c>
     </row>
     <row r="471">
@@ -4202,7 +4202,7 @@
         <v>-0.9524557630586569</v>
       </c>
       <c r="B471" t="n">
-        <v>-0.8629394769668579</v>
+        <v>-0.8638843894004822</v>
       </c>
     </row>
     <row r="472">
@@ -4210,7 +4210,7 @@
         <v>0.7676703920044745</v>
       </c>
       <c r="B472" t="n">
-        <v>0.7931310534477234</v>
+        <v>0.8034409880638123</v>
       </c>
     </row>
     <row r="473">
@@ -4218,7 +4218,7 @@
         <v>-0.6908094224442269</v>
       </c>
       <c r="B473" t="n">
-        <v>-0.6372685432434082</v>
+        <v>-0.6631650328636169</v>
       </c>
     </row>
     <row r="474">
@@ -4226,7 +4226,7 @@
         <v>0.9379192826243564</v>
       </c>
       <c r="B474" t="n">
-        <v>0.9071210026741028</v>
+        <v>0.9558534026145935</v>
       </c>
     </row>
     <row r="475">
@@ -4234,7 +4234,7 @@
         <v>-0.7505139843977547</v>
       </c>
       <c r="B475" t="n">
-        <v>-0.7184053659439087</v>
+        <v>-0.7270521521568298</v>
       </c>
     </row>
     <row r="476">
@@ -4242,7 +4242,7 @@
         <v>-0.7546662445280554</v>
       </c>
       <c r="B476" t="n">
-        <v>-0.753348708152771</v>
+        <v>-0.7475931644439697</v>
       </c>
     </row>
     <row r="477">
@@ -4250,7 +4250,7 @@
         <v>0.06907752619162302</v>
       </c>
       <c r="B477" t="n">
-        <v>0.05170285701751709</v>
+        <v>0.07609239965677261</v>
       </c>
     </row>
     <row r="478">
@@ -4258,7 +4258,7 @@
         <v>-0.9061521485921261</v>
       </c>
       <c r="B478" t="n">
-        <v>-0.8160038590431213</v>
+        <v>-0.8595734238624573</v>
       </c>
     </row>
     <row r="479">
@@ -4266,7 +4266,7 @@
         <v>-0.8114750148714711</v>
       </c>
       <c r="B479" t="n">
-        <v>-0.751477837562561</v>
+        <v>-0.8118426203727722</v>
       </c>
     </row>
     <row r="480">
@@ -4274,7 +4274,7 @@
         <v>-1.07606020526578</v>
       </c>
       <c r="B480" t="n">
-        <v>-0.9465857744216919</v>
+        <v>-0.9519127011299133</v>
       </c>
     </row>
     <row r="481">
@@ -4282,7 +4282,7 @@
         <v>1.673931773057237</v>
       </c>
       <c r="B481" t="n">
-        <v>1.564008831977844</v>
+        <v>1.647676467895508</v>
       </c>
     </row>
     <row r="482">
@@ -4290,7 +4290,7 @@
         <v>0.9540126626546146</v>
       </c>
       <c r="B482" t="n">
-        <v>0.812974214553833</v>
+        <v>0.8939425349235535</v>
       </c>
     </row>
     <row r="483">
@@ -4298,7 +4298,7 @@
         <v>-0.9185487512999801</v>
       </c>
       <c r="B483" t="n">
-        <v>-0.8358319997787476</v>
+        <v>-0.8726376891136169</v>
       </c>
     </row>
     <row r="484">
@@ -4306,7 +4306,7 @@
         <v>1.092629361689654</v>
       </c>
       <c r="B484" t="n">
-        <v>1.079590678215027</v>
+        <v>1.155941367149353</v>
       </c>
     </row>
     <row r="485">
@@ -4314,7 +4314,7 @@
         <v>1.168141459678963</v>
       </c>
       <c r="B485" t="n">
-        <v>1.195268988609314</v>
+        <v>1.234310507774353</v>
       </c>
     </row>
     <row r="486">
@@ -4322,7 +4322,7 @@
         <v>-0.7780670628635877</v>
       </c>
       <c r="B486" t="n">
-        <v>-0.7721949815750122</v>
+        <v>-0.771974503993988</v>
       </c>
     </row>
     <row r="487">
@@ -4330,7 +4330,7 @@
         <v>0.5720042118938282</v>
       </c>
       <c r="B487" t="n">
-        <v>0.5808449983596802</v>
+        <v>0.6288161873817444</v>
       </c>
     </row>
     <row r="488">
@@ -4338,7 +4338,7 @@
         <v>-0.7268096837813348</v>
       </c>
       <c r="B488" t="n">
-        <v>-0.7085592746734619</v>
+        <v>-0.6760635375976562</v>
       </c>
     </row>
     <row r="489">
@@ -4346,7 +4346,7 @@
         <v>-0.4589795674606102</v>
       </c>
       <c r="B489" t="n">
-        <v>-0.3314748704433441</v>
+        <v>-0.2963315546512604</v>
       </c>
     </row>
     <row r="490">
@@ -4354,7 +4354,7 @@
         <v>2.042583372047053</v>
       </c>
       <c r="B490" t="n">
-        <v>2.008256435394287</v>
+        <v>1.93749213218689</v>
       </c>
     </row>
     <row r="491">
@@ -4362,7 +4362,7 @@
         <v>-1.088292875664642</v>
       </c>
       <c r="B491" t="n">
-        <v>-0.9770004749298096</v>
+        <v>-0.9849159121513367</v>
       </c>
     </row>
     <row r="492">
@@ -4370,7 +4370,7 @@
         <v>-0.9153790474773744</v>
       </c>
       <c r="B492" t="n">
-        <v>-0.836119532585144</v>
+        <v>-0.8567343354225159</v>
       </c>
     </row>
     <row r="493">
@@ -4378,7 +4378,7 @@
         <v>-0.2822382311222484</v>
       </c>
       <c r="B493" t="n">
-        <v>-0.2827950417995453</v>
+        <v>-0.282394677400589</v>
       </c>
     </row>
     <row r="494">
@@ -4386,7 +4386,7 @@
         <v>1.977137547866884</v>
       </c>
       <c r="B494" t="n">
-        <v>1.763543009757996</v>
+        <v>1.880938410758972</v>
       </c>
     </row>
     <row r="495">
@@ -4394,7 +4394,7 @@
         <v>-0.9887932269300845</v>
       </c>
       <c r="B495" t="n">
-        <v>-0.9145682454109192</v>
+        <v>-0.9685422778129578</v>
       </c>
     </row>
     <row r="496">
@@ -4402,7 +4402,7 @@
         <v>2.241070640437131</v>
       </c>
       <c r="B496" t="n">
-        <v>2.150116443634033</v>
+        <v>2.17145848274231</v>
       </c>
     </row>
     <row r="497">
@@ -4410,7 +4410,7 @@
         <v>-0.9628965910674562</v>
       </c>
       <c r="B497" t="n">
-        <v>-0.8798843622207642</v>
+        <v>-0.9086276292800903</v>
       </c>
     </row>
     <row r="498">
@@ -4418,7 +4418,7 @@
         <v>-0.7259516330247734</v>
       </c>
       <c r="B498" t="n">
-        <v>-0.67519611120224</v>
+        <v>-0.6770028471946716</v>
       </c>
     </row>
     <row r="499">
@@ -4426,7 +4426,7 @@
         <v>0.8605396013680462</v>
       </c>
       <c r="B499" t="n">
-        <v>0.8061280250549316</v>
+        <v>0.8936066031455994</v>
       </c>
     </row>
     <row r="500">
@@ -4434,7 +4434,7 @@
         <v>-0.1134294547104768</v>
       </c>
       <c r="B500" t="n">
-        <v>-0.1265535354614258</v>
+        <v>-0.1448211669921875</v>
       </c>
     </row>
     <row r="501">
@@ -4442,7 +4442,7 @@
         <v>1.135271475406602</v>
       </c>
       <c r="B501" t="n">
-        <v>1.115018486976624</v>
+        <v>1.16941249370575</v>
       </c>
     </row>
     <row r="502">
@@ -4450,7 +4450,7 @@
         <v>0.6789695247382251</v>
       </c>
       <c r="B502" t="n">
-        <v>0.5719238519668579</v>
+        <v>0.6311064958572388</v>
       </c>
     </row>
     <row r="503">
@@ -4458,7 +4458,7 @@
         <v>-0.9653249680876883</v>
       </c>
       <c r="B503" t="n">
-        <v>-0.9122366905212402</v>
+        <v>-0.9293665885925293</v>
       </c>
     </row>
     <row r="504">
@@ -4466,7 +4466,7 @@
         <v>2.25634020873739</v>
       </c>
       <c r="B504" t="n">
-        <v>2.134960889816284</v>
+        <v>2.169562816619873</v>
       </c>
     </row>
     <row r="505">
@@ -4474,7 +4474,7 @@
         <v>0.07840973602220491</v>
       </c>
       <c r="B505" t="n">
-        <v>0.1593321561813354</v>
+        <v>0.1131927520036697</v>
       </c>
     </row>
     <row r="506">
@@ -4482,7 +4482,7 @@
         <v>-0.9475502443439988</v>
       </c>
       <c r="B506" t="n">
-        <v>-0.9228302240371704</v>
+        <v>-0.9300441145896912</v>
       </c>
     </row>
     <row r="507">
@@ -4490,7 +4490,7 @@
         <v>0.9376832408503328</v>
       </c>
       <c r="B507" t="n">
-        <v>0.9146154522895813</v>
+        <v>0.9858506321907043</v>
       </c>
     </row>
     <row r="508">
@@ -4498,7 +4498,7 @@
         <v>-0.6219703032225415</v>
       </c>
       <c r="B508" t="n">
-        <v>-0.5931093692779541</v>
+        <v>-0.5938664674758911</v>
       </c>
     </row>
     <row r="509">
@@ -4506,7 +4506,7 @@
         <v>2.207069730741975</v>
       </c>
       <c r="B509" t="n">
-        <v>2.135951519012451</v>
+        <v>2.105969667434692</v>
       </c>
     </row>
     <row r="510">
@@ -4514,7 +4514,7 @@
         <v>-0.41667880646302</v>
       </c>
       <c r="B510" t="n">
-        <v>-0.348446786403656</v>
+        <v>-0.3623089790344238</v>
       </c>
     </row>
     <row r="511">
@@ -4522,7 +4522,7 @@
         <v>-0.8794477829665195</v>
       </c>
       <c r="B511" t="n">
-        <v>-0.8574209213256836</v>
+        <v>-0.8455347418785095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Self Attention Mechanism for better accuracy
</commit_message>
<xml_diff>
--- a/Stored_data/predictions_test.xlsx
+++ b/Stored_data/predictions_test.xlsx
@@ -450,7 +450,7 @@
         <v>12780.96</v>
       </c>
       <c r="B2" t="n">
-        <v>13777.2314453125</v>
+        <v>11891.1044921875</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>7283.54</v>
       </c>
       <c r="B3" t="n">
-        <v>8860.271484375</v>
+        <v>7360.3544921875</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>7948.01</v>
       </c>
       <c r="B4" t="n">
-        <v>8668.7958984375</v>
+        <v>7948.3515625</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>7009.84</v>
       </c>
       <c r="B5" t="n">
-        <v>7905.271484375</v>
+        <v>7227.56396484375</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>27454.47</v>
       </c>
       <c r="B6" t="n">
-        <v>23585.947265625</v>
+        <v>26368.28125</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>9529.93</v>
       </c>
       <c r="B7" t="n">
-        <v>9080.4697265625</v>
+        <v>8422.0966796875</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>7338.64</v>
       </c>
       <c r="B8" t="n">
-        <v>8242.8671875</v>
+        <v>7298.56103515625</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>57338</v>
       </c>
       <c r="B9" t="n">
-        <v>55927</v>
+        <v>58413.3671875</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>19422.61</v>
       </c>
       <c r="B10" t="n">
-        <v>19530.978515625</v>
+        <v>18689.810546875</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>34669.13</v>
       </c>
       <c r="B11" t="n">
-        <v>33852.1875</v>
+        <v>33811.62109375</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>64262.7</v>
       </c>
       <c r="B12" t="n">
-        <v>60523.1640625</v>
+        <v>63943.12109375</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>8810.790000000003</v>
       </c>
       <c r="B13" t="n">
-        <v>9845.626953125</v>
+        <v>9307.30078125</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>58202.01</v>
       </c>
       <c r="B14" t="n">
-        <v>57773.453125</v>
+        <v>58184.44921875</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>10340.31</v>
       </c>
       <c r="B15" t="n">
-        <v>10234.8681640625</v>
+        <v>10760.02734375</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>37449.73</v>
       </c>
       <c r="B16" t="n">
-        <v>37563.1640625</v>
+        <v>38427.3515625</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>3715.3</v>
       </c>
       <c r="B17" t="n">
-        <v>5364.18603515625</v>
+        <v>3567.103759765625</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>6609.78</v>
       </c>
       <c r="B18" t="n">
-        <v>7631.52490234375</v>
+        <v>6068.8115234375</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>7934.52</v>
       </c>
       <c r="B19" t="n">
-        <v>9111.7197265625</v>
+        <v>7487.83154296875</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>7508.52</v>
       </c>
       <c r="B20" t="n">
-        <v>9757.759765625</v>
+        <v>7938.42578125</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>60752.71000000001</v>
       </c>
       <c r="B21" t="n">
-        <v>60478.984375</v>
+        <v>61505.6796875</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>6250.81</v>
       </c>
       <c r="B22" t="n">
-        <v>8655.5283203125</v>
+        <v>6548.302734375</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>8187.17</v>
       </c>
       <c r="B23" t="n">
-        <v>9629.8935546875</v>
+        <v>8074.67822265625</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>11256.49</v>
       </c>
       <c r="B24" t="n">
-        <v>11957.193359375</v>
+        <v>11413.294921875</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>31801.04</v>
       </c>
       <c r="B25" t="n">
-        <v>29935.544921875</v>
+        <v>31072.72265625</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>47120.87</v>
       </c>
       <c r="B26" t="n">
-        <v>47208.203125</v>
+        <v>47011.6484375</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>33504.69</v>
       </c>
       <c r="B27" t="n">
-        <v>33875.54296875</v>
+        <v>34068.09375</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>9687.879999999999</v>
       </c>
       <c r="B28" t="n">
-        <v>11281.416015625</v>
+        <v>9738.4765625</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>7240.06</v>
       </c>
       <c r="B29" t="n">
-        <v>8172.85595703125</v>
+        <v>6860.58203125</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>24441.38</v>
       </c>
       <c r="B30" t="n">
-        <v>23165.162109375</v>
+        <v>23737.818359375</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>16812.08</v>
       </c>
       <c r="B31" t="n">
-        <v>18947.77734375</v>
+        <v>16940.80859375</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>46653.99</v>
       </c>
       <c r="B32" t="n">
-        <v>46789.2109375</v>
+        <v>45511.03515625</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>38420.81</v>
       </c>
       <c r="B33" t="n">
-        <v>39647.8828125</v>
+        <v>39211.6171875</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>24712.47</v>
       </c>
       <c r="B34" t="n">
-        <v>25706.833984375</v>
+        <v>24083.8203125</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>7316.14</v>
       </c>
       <c r="B35" t="n">
-        <v>7656.6318359375</v>
+        <v>7627.2099609375</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>7824.8</v>
       </c>
       <c r="B36" t="n">
-        <v>9652.951171875</v>
+        <v>8468.376953125</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>8655.02</v>
       </c>
       <c r="B37" t="n">
-        <v>8970.8935546875</v>
+        <v>7974.640625</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>28171.87</v>
       </c>
       <c r="B38" t="n">
-        <v>27325.00390625</v>
+        <v>27305.609375</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>53787.63</v>
       </c>
       <c r="B39" t="n">
-        <v>53294.51953125</v>
+        <v>54178.34765625</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>7115.04</v>
       </c>
       <c r="B40" t="n">
-        <v>7949.064453125</v>
+        <v>5791.43310546875</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>7120.74</v>
       </c>
       <c r="B41" t="n">
-        <v>8948.732421875</v>
+        <v>6949.76318359375</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>6144.009999999999</v>
       </c>
       <c r="B42" t="n">
-        <v>7562.76611328125</v>
+        <v>6178.015625</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>7991.74</v>
       </c>
       <c r="B43" t="n">
-        <v>7652.54052734375</v>
+        <v>7883.4375</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>8170</v>
       </c>
       <c r="B44" t="n">
-        <v>10956.8525390625</v>
+        <v>8879.55078125</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>47111.52</v>
       </c>
       <c r="B45" t="n">
-        <v>45457.0078125</v>
+        <v>47078.578125</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>21783.54</v>
       </c>
       <c r="B46" t="n">
-        <v>19584.16015625</v>
+        <v>20842.5625</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>8359.940000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>9456.95703125</v>
+        <v>8127.71533203125</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>44145.11</v>
       </c>
       <c r="B48" t="n">
-        <v>43450.59765625</v>
+        <v>42681.64453125</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>62819.91</v>
       </c>
       <c r="B49" t="n">
-        <v>62148.21484375</v>
+        <v>61553.125</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>29581.99</v>
       </c>
       <c r="B50" t="n">
-        <v>29304.32421875</v>
+        <v>28972.818359375</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>29430.27</v>
       </c>
       <c r="B51" t="n">
-        <v>29284.994140625</v>
+        <v>29778.369140625</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>6734.1</v>
       </c>
       <c r="B52" t="n">
-        <v>7744.99658203125</v>
+        <v>6707.2626953125</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>42380.87</v>
       </c>
       <c r="B53" t="n">
-        <v>41743.21875</v>
+        <v>42247.5234375</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>60058.87</v>
       </c>
       <c r="B54" t="n">
-        <v>57515.72265625</v>
+        <v>62072.61328125</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>70631.08</v>
       </c>
       <c r="B55" t="n">
-        <v>66746.03125</v>
+        <v>69582.15625</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>63152.01</v>
       </c>
       <c r="B56" t="n">
-        <v>61194.1015625</v>
+        <v>63620.13671875</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>3823</v>
       </c>
       <c r="B57" t="n">
-        <v>5631.56396484375</v>
+        <v>3762.67626953125</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>10666.39</v>
       </c>
       <c r="B58" t="n">
-        <v>11498.6787109375</v>
+        <v>10720.279296875</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>62896.48</v>
       </c>
       <c r="B59" t="n">
-        <v>58815.69921875</v>
+        <v>61811.09375</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>34262.88</v>
       </c>
       <c r="B60" t="n">
-        <v>35153.84765625</v>
+        <v>33636.2734375</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>33786.55</v>
       </c>
       <c r="B61" t="n">
-        <v>33634.44921875</v>
+        <v>33736.3828125</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>43137.95</v>
       </c>
       <c r="B62" t="n">
-        <v>44941.97265625</v>
+        <v>42901.87109375</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>6868.699999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>9716.853515625</v>
+        <v>6888.52685546875</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>10890.01</v>
       </c>
       <c r="B64" t="n">
-        <v>11069.1953125</v>
+        <v>11074.6005859375</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>3680.06</v>
       </c>
       <c r="B65" t="n">
-        <v>5799.10107421875</v>
+        <v>2832.24658203125</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>61286.75</v>
       </c>
       <c r="B66" t="n">
-        <v>58914.484375</v>
+        <v>61702.86328125</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>23742.3</v>
       </c>
       <c r="B67" t="n">
-        <v>24655.92578125</v>
+        <v>22278.197265625</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>29211.06</v>
       </c>
       <c r="B68" t="n">
-        <v>28474.498046875</v>
+        <v>28321.296875</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>3792.01</v>
       </c>
       <c r="B69" t="n">
-        <v>6327.36767578125</v>
+        <v>3598.173095703125</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>68124.19</v>
       </c>
       <c r="B70" t="n">
-        <v>63285.33203125</v>
+        <v>68643.078125</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>48343.28</v>
       </c>
       <c r="B71" t="n">
-        <v>46443.46484375</v>
+        <v>48521.63671875</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>19951.86</v>
       </c>
       <c r="B72" t="n">
-        <v>18863.8125</v>
+        <v>19508.3671875</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>8055.98</v>
       </c>
       <c r="B73" t="n">
-        <v>7515.5107421875</v>
+        <v>7771.85546875</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>26516.99</v>
       </c>
       <c r="B74" t="n">
-        <v>25413.009765625</v>
+        <v>26038.59375</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>9170.280000000001</v>
       </c>
       <c r="B75" t="n">
-        <v>9599.7294921875</v>
+        <v>8831.9921875</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>10624.93</v>
       </c>
       <c r="B76" t="n">
-        <v>11862.4228515625</v>
+        <v>11087.7431640625</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>9381.27</v>
       </c>
       <c r="B77" t="n">
-        <v>9950.9140625</v>
+        <v>9344.259765625</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>29770.42</v>
       </c>
       <c r="B78" t="n">
-        <v>29407.28515625</v>
+        <v>28752.220703125</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>40480.01</v>
       </c>
       <c r="B79" t="n">
-        <v>40239.4453125</v>
+        <v>40738.515625</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>45584.99</v>
       </c>
       <c r="B80" t="n">
-        <v>45788.921875</v>
+        <v>45901.69140625</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>8110.34</v>
       </c>
       <c r="B81" t="n">
-        <v>8379.310546875</v>
+        <v>8380.6982421875</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>62432.1</v>
       </c>
       <c r="B82" t="n">
-        <v>54916.19921875</v>
+        <v>59127.703125</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>29542.15</v>
       </c>
       <c r="B83" t="n">
-        <v>29937.001953125</v>
+        <v>32334.86328125</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>10303.12</v>
       </c>
       <c r="B84" t="n">
-        <v>9772.2568359375</v>
+        <v>10390.0458984375</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>56950.56</v>
       </c>
       <c r="B85" t="n">
-        <v>52920.83203125</v>
+        <v>57342.2109375</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>37371.38</v>
       </c>
       <c r="B86" t="n">
-        <v>37090.07421875</v>
+        <v>36253.1171875</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>61987.28</v>
       </c>
       <c r="B87" t="n">
-        <v>62666.18359375</v>
+        <v>61747.8671875</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>8197.27</v>
       </c>
       <c r="B88" t="n">
-        <v>7890.13134765625</v>
+        <v>8018.44189453125</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>6723.05</v>
       </c>
       <c r="B89" t="n">
-        <v>8303.2158203125</v>
+        <v>5811.6796875</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>6410.000000000001</v>
       </c>
       <c r="B90" t="n">
-        <v>8394.5595703125</v>
+        <v>6150.89501953125</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>9513.209999999999</v>
       </c>
       <c r="B91" t="n">
-        <v>10018.16015625</v>
+        <v>8938.9482421875</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>6618.96</v>
       </c>
       <c r="B92" t="n">
-        <v>7614.52099609375</v>
+        <v>6406.40576171875</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>6796.1</v>
       </c>
       <c r="B93" t="n">
-        <v>8125.021484375</v>
+        <v>7273.7958984375</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>7019.98</v>
       </c>
       <c r="B94" t="n">
-        <v>7883.53955078125</v>
+        <v>5823.2177734375</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>9160.780000000001</v>
       </c>
       <c r="B95" t="n">
-        <v>9090.8994140625</v>
+        <v>8980.2626953125</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>53555</v>
       </c>
       <c r="B96" t="n">
-        <v>51258.08203125</v>
+        <v>53759.93359375</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>57301.86</v>
       </c>
       <c r="B97" t="n">
-        <v>56904.50390625</v>
+        <v>59286.16796875</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>7510.11</v>
       </c>
       <c r="B98" t="n">
-        <v>8565.5791015625</v>
+        <v>7324.4716796875</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>41574.25</v>
       </c>
       <c r="B99" t="n">
-        <v>39031.1484375</v>
+        <v>39344.1796875</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>67116.52</v>
       </c>
       <c r="B100" t="n">
-        <v>64783.5</v>
+        <v>66675.390625</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>22346.57</v>
       </c>
       <c r="B101" t="n">
-        <v>18919.7578125</v>
+        <v>21695.505859375</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>66504.33</v>
       </c>
       <c r="B102" t="n">
-        <v>63642.87109375</v>
+        <v>67507.328125</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>22430.24</v>
       </c>
       <c r="B103" t="n">
-        <v>19754.53125</v>
+        <v>22003.994140625</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>13636.17</v>
       </c>
       <c r="B104" t="n">
-        <v>14078.4169921875</v>
+        <v>13291.458984375</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>37237.6</v>
       </c>
       <c r="B105" t="n">
-        <v>34440.57421875</v>
+        <v>36574.46484375</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>32945.17</v>
       </c>
       <c r="B106" t="n">
-        <v>31469.859375</v>
+        <v>32821.88671875</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>9227</v>
       </c>
       <c r="B107" t="n">
-        <v>9663.3408203125</v>
+        <v>9485.7841796875</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>50441.92</v>
       </c>
       <c r="B108" t="n">
-        <v>48923.796875</v>
+        <v>50285.30859375</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>7541.89</v>
       </c>
       <c r="B109" t="n">
-        <v>9522.529296875</v>
+        <v>7731.5478515625</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>33380.81</v>
       </c>
       <c r="B110" t="n">
-        <v>32534.935546875</v>
+        <v>36395.3984375</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>62312.08</v>
       </c>
       <c r="B111" t="n">
-        <v>60258.19921875</v>
+        <v>63133.6171875</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>45510.34</v>
       </c>
       <c r="B112" t="n">
-        <v>46013.0234375</v>
+        <v>46761.06640625</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>65173.99</v>
       </c>
       <c r="B113" t="n">
-        <v>61548.3515625</v>
+        <v>64768.75390625</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>19421.9</v>
       </c>
       <c r="B114" t="n">
-        <v>19466.083984375</v>
+        <v>19466.634765625</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>8471.73</v>
       </c>
       <c r="B115" t="n">
-        <v>9353.5595703125</v>
+        <v>8287.501953125</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>38207.05</v>
       </c>
       <c r="B116" t="n">
-        <v>39875.94921875</v>
+        <v>40623.12109375</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>8614.43</v>
       </c>
       <c r="B117" t="n">
-        <v>9419.892578125</v>
+        <v>8150.14111328125</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>56180</v>
       </c>
       <c r="B118" t="n">
-        <v>56451.28125</v>
+        <v>57795.6015625</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>7854.25</v>
       </c>
       <c r="B119" t="n">
-        <v>9556.5986328125</v>
+        <v>7903.74560546875</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>27250.97</v>
       </c>
       <c r="B120" t="n">
-        <v>23566.353515625</v>
+        <v>27156.453125</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>7575.01</v>
       </c>
       <c r="B121" t="n">
-        <v>8265.7919921875</v>
+        <v>7644.2861328125</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>27242.59</v>
       </c>
       <c r="B122" t="n">
-        <v>27188.14453125</v>
+        <v>26770.443359375</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>47287.6</v>
       </c>
       <c r="B123" t="n">
-        <v>47594.16015625</v>
+        <v>48542.05859375</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>17719.85</v>
       </c>
       <c r="B124" t="n">
-        <v>16620.95703125</v>
+        <v>17672.314453125</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>19292.84</v>
       </c>
       <c r="B125" t="n">
-        <v>17579.1953125</v>
+        <v>18317.123046875</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>8173</v>
       </c>
       <c r="B126" t="n">
-        <v>8458.6865234375</v>
+        <v>7706.35302734375</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>36568.1</v>
       </c>
       <c r="B127" t="n">
-        <v>36033.25390625</v>
+        <v>35959.5625</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>52124.11</v>
       </c>
       <c r="B128" t="n">
-        <v>51064.94921875</v>
+        <v>50903.28125</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>3601.31</v>
       </c>
       <c r="B129" t="n">
-        <v>5721.68896484375</v>
+        <v>3251.07373046875</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>42217.87</v>
       </c>
       <c r="B130" t="n">
-        <v>43285.5546875</v>
+        <v>43415.22265625</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>7056</v>
       </c>
       <c r="B131" t="n">
-        <v>8515.0068359375</v>
+        <v>7342.78662109375</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>27162.14</v>
       </c>
       <c r="B132" t="n">
-        <v>26424.125</v>
+        <v>26911.455078125</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>33552.79</v>
       </c>
       <c r="B133" t="n">
-        <v>34578.0390625</v>
+        <v>37565.26953125</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>30466.93</v>
       </c>
       <c r="B134" t="n">
-        <v>29570.408203125</v>
+        <v>30055.5859375</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>65175.32</v>
       </c>
       <c r="B135" t="n">
-        <v>62928.1953125</v>
+        <v>65928.015625</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>58427.35</v>
       </c>
       <c r="B136" t="n">
-        <v>56810.4375</v>
+        <v>59276.8515625</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>9721</v>
       </c>
       <c r="B137" t="n">
-        <v>9170.595703125</v>
+        <v>9938.5458984375</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>26493.39</v>
       </c>
       <c r="B138" t="n">
-        <v>27055.41796875</v>
+        <v>25125.603515625</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>65936.00999999999</v>
       </c>
       <c r="B139" t="n">
-        <v>62919.6171875</v>
+        <v>67866</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>19329.72</v>
       </c>
       <c r="B140" t="n">
-        <v>18826.1875</v>
+        <v>19172.814453125</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>19417.96</v>
       </c>
       <c r="B141" t="n">
-        <v>17838.416015625</v>
+        <v>19549.265625</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>57221.72</v>
       </c>
       <c r="B142" t="n">
-        <v>54442.171875</v>
+        <v>55900.7109375</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>25840.1</v>
       </c>
       <c r="B143" t="n">
-        <v>26391.220703125</v>
+        <v>24689.306640625</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>20401.31</v>
       </c>
       <c r="B144" t="n">
-        <v>21806.3515625</v>
+        <v>22093.927734375</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>8785.25</v>
       </c>
       <c r="B145" t="n">
-        <v>10351.9951171875</v>
+        <v>9284.2451171875</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>52303.65</v>
       </c>
       <c r="B146" t="n">
-        <v>50519.48046875</v>
+        <v>53958.2890625</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>9012</v>
       </c>
       <c r="B147" t="n">
-        <v>10765.810546875</v>
+        <v>9261.015625</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>13326.61</v>
       </c>
       <c r="B148" t="n">
-        <v>15383.4052734375</v>
+        <v>15777.546875</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>10842.85</v>
       </c>
       <c r="B149" t="n">
-        <v>11603.86328125</v>
+        <v>11069.6875</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>15328.41</v>
       </c>
       <c r="B150" t="n">
-        <v>14908.8388671875</v>
+        <v>14996.259765625</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>27494.51</v>
       </c>
       <c r="B151" t="n">
-        <v>27688.34375</v>
+        <v>27076.8515625</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>29026.16</v>
       </c>
       <c r="B152" t="n">
-        <v>28268.478515625</v>
+        <v>27887.974609375</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>9224.52</v>
       </c>
       <c r="B153" t="n">
-        <v>11191.7216796875</v>
+        <v>9851.34375</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>29331.69</v>
       </c>
       <c r="B154" t="n">
-        <v>30358.615234375</v>
+        <v>29993.294921875</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>4295.84</v>
       </c>
       <c r="B155" t="n">
-        <v>4685.29833984375</v>
+        <v>4110.89306640625</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>5415</v>
       </c>
       <c r="B156" t="n">
-        <v>6051.58984375</v>
+        <v>4722.2333984375</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>20627.48</v>
       </c>
       <c r="B157" t="n">
-        <v>19830.9296875</v>
+        <v>20494.998046875</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>9419</v>
       </c>
       <c r="B158" t="n">
-        <v>9390.08203125</v>
+        <v>9134.693359375</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>44695.95</v>
       </c>
       <c r="B159" t="n">
-        <v>45175.796875</v>
+        <v>46519.0078125</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>23312.42</v>
       </c>
       <c r="B160" t="n">
-        <v>23234.302734375</v>
+        <v>22126.84375</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>47800</v>
       </c>
       <c r="B161" t="n">
-        <v>47327.09375</v>
+        <v>47063.94140625</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>7027.55</v>
       </c>
       <c r="B162" t="n">
-        <v>8837.0859375</v>
+        <v>6856.62939453125</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>25925.55</v>
       </c>
       <c r="B163" t="n">
-        <v>25782.4453125</v>
+        <v>25864.033203125</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>17085.05</v>
       </c>
       <c r="B164" t="n">
-        <v>18337.62109375</v>
+        <v>17125.244140625</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>7795.51</v>
       </c>
       <c r="B165" t="n">
-        <v>9206.1611328125</v>
+        <v>7778.9287109375</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>9574.209999999999</v>
       </c>
       <c r="B166" t="n">
-        <v>10159.1142578125</v>
+        <v>10106.7880859375</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>3631.05</v>
       </c>
       <c r="B167" t="n">
-        <v>5909.7890625</v>
+        <v>2976.59326171875</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>20742.56</v>
       </c>
       <c r="B168" t="n">
-        <v>22755.173828125</v>
+        <v>20347.560546875</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>10331.54</v>
       </c>
       <c r="B169" t="n">
-        <v>10582.7119140625</v>
+        <v>10378.18359375</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>38150.02</v>
       </c>
       <c r="B170" t="n">
-        <v>36877.41796875</v>
+        <v>37116.30078125</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>9131.34</v>
       </c>
       <c r="B171" t="n">
-        <v>10293.5927734375</v>
+        <v>8861.1865234375</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>5308.25</v>
       </c>
       <c r="B172" t="n">
-        <v>6527.12646484375</v>
+        <v>4922.36572265625</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>3594.87</v>
       </c>
       <c r="B173" t="n">
-        <v>5297.57177734375</v>
+        <v>3131.335205078125</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>9292.24</v>
       </c>
       <c r="B174" t="n">
-        <v>9461.6630859375</v>
+        <v>9156.0078125</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>7390.89</v>
       </c>
       <c r="B175" t="n">
-        <v>9211.0390625</v>
+        <v>7696.18505859375</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>7488.21</v>
       </c>
       <c r="B176" t="n">
-        <v>8500.0185546875</v>
+        <v>7392.58984375</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>30692.44</v>
       </c>
       <c r="B177" t="n">
-        <v>30326.76171875</v>
+        <v>29668.072265625</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>26180.05</v>
       </c>
       <c r="B178" t="n">
-        <v>26081.611328125</v>
+        <v>25756.423828125</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>9518.16</v>
       </c>
       <c r="B179" t="n">
-        <v>9298.0947265625</v>
+        <v>9148.5263671875</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>9231.610000000001</v>
       </c>
       <c r="B180" t="n">
-        <v>9574.7744140625</v>
+        <v>9144.197265625</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>39942.38</v>
       </c>
       <c r="B181" t="n">
-        <v>39776.34765625</v>
+        <v>40286.359375</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>51568.22</v>
       </c>
       <c r="B182" t="n">
-        <v>53392.84375</v>
+        <v>52714.2734375</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>63113.97</v>
       </c>
       <c r="B183" t="n">
-        <v>63489.75390625</v>
+        <v>62494.35546875</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>39422</v>
       </c>
       <c r="B184" t="n">
-        <v>39099.47265625</v>
+        <v>39821.19140625</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>30617.03</v>
       </c>
       <c r="B185" t="n">
-        <v>30697.8515625</v>
+        <v>30226.681640625</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>56022.01000000001</v>
       </c>
       <c r="B186" t="n">
-        <v>53857.73046875</v>
+        <v>57867.62890625</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>24305.24</v>
       </c>
       <c r="B187" t="n">
-        <v>23155.07421875</v>
+        <v>23883.998046875</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>6197.92</v>
       </c>
       <c r="B188" t="n">
-        <v>7027.12451171875</v>
+        <v>6191.95458984375</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>8041.46</v>
       </c>
       <c r="B189" t="n">
-        <v>9303.9619140625</v>
+        <v>8099.2587890625</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>33892.02</v>
       </c>
       <c r="B190" t="n">
-        <v>32190.533203125</v>
+        <v>32579.056640625</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>9910</v>
       </c>
       <c r="B191" t="n">
-        <v>10631.4111328125</v>
+        <v>10021.3505859375</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>32178.33</v>
       </c>
       <c r="B192" t="n">
-        <v>33144.65625</v>
+        <v>31804.646484375</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>7894.56</v>
       </c>
       <c r="B193" t="n">
-        <v>8717.3046875</v>
+        <v>7678.71337890625</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>61188.39</v>
       </c>
       <c r="B194" t="n">
-        <v>56943.1953125</v>
+        <v>59113.1171875</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>50820</v>
       </c>
       <c r="B195" t="n">
-        <v>48130.84375</v>
+        <v>49174.8515625</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>23009.65</v>
       </c>
       <c r="B196" t="n">
-        <v>22461.193359375</v>
+        <v>21292.78515625</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>20175.83</v>
       </c>
       <c r="B197" t="n">
-        <v>19976.451171875</v>
+        <v>20424.794921875</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>49676.2</v>
       </c>
       <c r="B198" t="n">
-        <v>50038.83984375</v>
+        <v>50123.8671875</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>28715.32</v>
       </c>
       <c r="B199" t="n">
-        <v>30641.91796875</v>
+        <v>30829.64453125</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>47067.99</v>
       </c>
       <c r="B200" t="n">
-        <v>47676.70703125</v>
+        <v>47658.1171875</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>64122.23</v>
       </c>
       <c r="B201" t="n">
-        <v>60343.6015625</v>
+        <v>64517.99609375</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>32254.2</v>
       </c>
       <c r="B202" t="n">
-        <v>32808.96875</v>
+        <v>32359.38671875</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>30200.42</v>
       </c>
       <c r="B203" t="n">
-        <v>29043.283203125</v>
+        <v>28829.134765625</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>8169.87</v>
       </c>
       <c r="B204" t="n">
-        <v>8886.3740234375</v>
+        <v>6969.427734375</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>59346.64</v>
       </c>
       <c r="B205" t="n">
-        <v>56189.53125</v>
+        <v>60498.21875</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>14400</v>
       </c>
       <c r="B206" t="n">
-        <v>15248.3056640625</v>
+        <v>15221.9169921875</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>8278</v>
       </c>
       <c r="B207" t="n">
-        <v>8905.1162109375</v>
+        <v>7888.8896484375</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>58950.01</v>
       </c>
       <c r="B208" t="n">
-        <v>57216.421875</v>
+        <v>57975.46875</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>6744.719999999999</v>
       </c>
       <c r="B209" t="n">
-        <v>8214.4658203125</v>
+        <v>6826.54052734375</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>7527.47</v>
       </c>
       <c r="B210" t="n">
-        <v>8785.416015625</v>
+        <v>7440.333984375</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>10372.25</v>
       </c>
       <c r="B211" t="n">
-        <v>9078.5673828125</v>
+        <v>10235.55859375</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>12968.52</v>
       </c>
       <c r="B212" t="n">
-        <v>13280.8134765625</v>
+        <v>12293.8955078125</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>6506.98</v>
       </c>
       <c r="B213" t="n">
-        <v>8592.7041015625</v>
+        <v>6306.36083984375</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>8400</v>
       </c>
       <c r="B214" t="n">
-        <v>9077.435546875</v>
+        <v>8656.3427734375</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>28629.8</v>
       </c>
       <c r="B215" t="n">
-        <v>28509.0390625</v>
+        <v>30533.83984375</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>21195.6</v>
       </c>
       <c r="B216" t="n">
-        <v>21004.384765625</v>
+        <v>19673.673828125</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>21299.37</v>
       </c>
       <c r="B217" t="n">
-        <v>21148.09375</v>
+        <v>20064.642578125</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>51728.85</v>
       </c>
       <c r="B218" t="n">
-        <v>52883.7890625</v>
+        <v>52962.63671875</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>69499.85000000001</v>
       </c>
       <c r="B219" t="n">
-        <v>62901.5625</v>
+        <v>69487.9140625</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>21491.19</v>
       </c>
       <c r="B220" t="n">
-        <v>22071.744140625</v>
+        <v>20882.890625</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>6214.57</v>
       </c>
       <c r="B221" t="n">
-        <v>6924.8818359375</v>
+        <v>6253.84375</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>10241.46</v>
       </c>
       <c r="B222" t="n">
-        <v>11853.978515625</v>
+        <v>10543.1904296875</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>42508.93</v>
       </c>
       <c r="B223" t="n">
-        <v>43255.2734375</v>
+        <v>42336.99609375</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>43839.99</v>
       </c>
       <c r="B224" t="n">
-        <v>42211.21875</v>
+        <v>43423.83984375</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>34494.89</v>
       </c>
       <c r="B225" t="n">
-        <v>33371.40625</v>
+        <v>34584.48046875</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>8856.980000000001</v>
       </c>
       <c r="B226" t="n">
-        <v>8982.42578125</v>
+        <v>8085.88525390625</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>26017.37</v>
       </c>
       <c r="B227" t="n">
-        <v>25785.41796875</v>
+        <v>25586.025390625</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>52137.67</v>
       </c>
       <c r="B228" t="n">
-        <v>52894.09765625</v>
+        <v>51457.98828125</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>3665.3</v>
       </c>
       <c r="B229" t="n">
-        <v>5753.85498046875</v>
+        <v>3181.830078125</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>16824.67</v>
       </c>
       <c r="B230" t="n">
-        <v>17863.28125</v>
+        <v>16243.390625</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>9162.209999999999</v>
       </c>
       <c r="B231" t="n">
-        <v>10549.9072265625</v>
+        <v>9359.728515625</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>3745.79</v>
       </c>
       <c r="B232" t="n">
-        <v>6729.98095703125</v>
+        <v>3486.45849609375</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>16428.78</v>
       </c>
       <c r="B233" t="n">
-        <v>16718.619140625</v>
+        <v>16536.98828125</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>25841.21</v>
       </c>
       <c r="B234" t="n">
-        <v>26227.94921875</v>
+        <v>25919.57421875</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>21826.87</v>
       </c>
       <c r="B235" t="n">
-        <v>20805.8125</v>
+        <v>19681.79296875</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>6353.01</v>
       </c>
       <c r="B236" t="n">
-        <v>6711.8359375</v>
+        <v>6298.03466796875</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>6479.84</v>
       </c>
       <c r="B237" t="n">
-        <v>7337.373046875</v>
+        <v>5847.353515625</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>55605.2</v>
       </c>
       <c r="B238" t="n">
-        <v>54515.609375</v>
+        <v>57956.5859375</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>9266</v>
       </c>
       <c r="B239" t="n">
-        <v>9400.6328125</v>
+        <v>9123.7822265625</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>20798.16</v>
       </c>
       <c r="B240" t="n">
-        <v>20980.158203125</v>
+        <v>20041.814453125</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>22987.79</v>
       </c>
       <c r="B241" t="n">
-        <v>23235.791015625</v>
+        <v>23173.67578125</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>18036.53</v>
       </c>
       <c r="B242" t="n">
-        <v>18157.7734375</v>
+        <v>18379.1171875</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>5017.37</v>
       </c>
       <c r="B243" t="n">
-        <v>6376.38037109375</v>
+        <v>4913.203125</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>8133.64</v>
       </c>
       <c r="B244" t="n">
-        <v>9737.529296875</v>
+        <v>7994.3876953125</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>7521.01</v>
       </c>
       <c r="B245" t="n">
-        <v>7206.19921875</v>
+        <v>7323.3623046875</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>63470.08</v>
       </c>
       <c r="B246" t="n">
-        <v>59572.8828125</v>
+        <v>64067.640625</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>10164.71</v>
       </c>
       <c r="B247" t="n">
-        <v>11762.509765625</v>
+        <v>9454.5908203125</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>8778.57</v>
       </c>
       <c r="B248" t="n">
-        <v>7901.01904296875</v>
+        <v>7813.98193359375</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>43082.94</v>
       </c>
       <c r="B249" t="n">
-        <v>43549.37890625</v>
+        <v>43306.0859375</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>44170.99</v>
       </c>
       <c r="B250" t="n">
-        <v>42469.82421875</v>
+        <v>41496.2890625</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>6720.06</v>
       </c>
       <c r="B251" t="n">
-        <v>7294.5927734375</v>
+        <v>6590.9541015625</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>9525.59</v>
       </c>
       <c r="B252" t="n">
-        <v>10849.0537109375</v>
+        <v>9547.0029296875</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>10840.48</v>
       </c>
       <c r="B253" t="n">
-        <v>11642.380859375</v>
+        <v>10643.1865234375</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>68809.89999999999</v>
       </c>
       <c r="B254" t="n">
-        <v>65199.52734375</v>
+        <v>69230.2734375</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>46431.5</v>
       </c>
       <c r="B255" t="n">
-        <v>43751.56640625</v>
+        <v>45596.5859375</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>18970.79</v>
       </c>
       <c r="B256" t="n">
-        <v>19564.275390625</v>
+        <v>21301.642578125</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>59123.99</v>
       </c>
       <c r="B257" t="n">
-        <v>58089.7265625</v>
+        <v>59077.91015625</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>8650</v>
       </c>
       <c r="B258" t="n">
-        <v>7896.38134765625</v>
+        <v>8425.908203125</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>7851.51</v>
       </c>
       <c r="B259" t="n">
-        <v>8925.6904296875</v>
+        <v>7994.353515625</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>4027.81</v>
       </c>
       <c r="B260" t="n">
-        <v>6521.171875</v>
+        <v>3789.40869140625</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>22432.58</v>
       </c>
       <c r="B261" t="n">
-        <v>22041.68359375</v>
+        <v>20858.837890625</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>11681.68</v>
       </c>
       <c r="B262" t="n">
-        <v>11205.603515625</v>
+        <v>11473.068359375</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>36742.22</v>
       </c>
       <c r="B263" t="n">
-        <v>37516.01953125</v>
+        <v>36797.5703125</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>42364.13</v>
       </c>
       <c r="B264" t="n">
-        <v>41322.53515625</v>
+        <v>43515.796875</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>30312.01</v>
       </c>
       <c r="B265" t="n">
-        <v>29982.140625</v>
+        <v>29614.6875</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>7658.84</v>
       </c>
       <c r="B266" t="n">
-        <v>8132.4189453125</v>
+        <v>7086.755859375</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>13699.34</v>
       </c>
       <c r="B267" t="n">
-        <v>13989.662109375</v>
+        <v>14883.685546875</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>7461.29</v>
       </c>
       <c r="B268" t="n">
-        <v>7348.93212890625</v>
+        <v>7312.77734375</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>28838.16</v>
       </c>
       <c r="B269" t="n">
-        <v>28069.017578125</v>
+        <v>27945.9453125</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>65376</v>
       </c>
       <c r="B270" t="n">
-        <v>62362.8203125</v>
+        <v>67462.6484375</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>11360.2</v>
       </c>
       <c r="B271" t="n">
-        <v>12279.76171875</v>
+        <v>11111.498046875</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>3987.81</v>
       </c>
       <c r="B272" t="n">
-        <v>6263.57470703125</v>
+        <v>3470.13232421875</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>11219.81</v>
       </c>
       <c r="B273" t="n">
-        <v>11485.7744140625</v>
+        <v>11025.87890625</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>26568.08</v>
       </c>
       <c r="B274" t="n">
-        <v>26865.501953125</v>
+        <v>26095.96484375</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>16850.36</v>
       </c>
       <c r="B275" t="n">
-        <v>18796.314453125</v>
+        <v>16756.5546875</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>23268.01</v>
       </c>
       <c r="B276" t="n">
-        <v>23508.08984375</v>
+        <v>23607.490234375</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>20591.13</v>
       </c>
       <c r="B277" t="n">
-        <v>20773.787109375</v>
+        <v>19272.564453125</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>57487.73</v>
       </c>
       <c r="B278" t="n">
-        <v>56967.375</v>
+        <v>59385.06640625</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>56247.18</v>
       </c>
       <c r="B279" t="n">
-        <v>54891.25</v>
+        <v>58228.5546875</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>19160.01</v>
       </c>
       <c r="B280" t="n">
-        <v>19885.51171875</v>
+        <v>18570.630859375</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>9197.02</v>
       </c>
       <c r="B281" t="n">
-        <v>9370.3037109375</v>
+        <v>9208.68359375</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>11761.41</v>
       </c>
       <c r="B282" t="n">
-        <v>11328.9931640625</v>
+        <v>11357.396484375</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>21310.9</v>
       </c>
       <c r="B283" t="n">
-        <v>22169.970703125</v>
+        <v>22738.091796875</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>51288.42</v>
       </c>
       <c r="B284" t="n">
-        <v>53542.83984375</v>
+        <v>53359.0703125</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>6965.71</v>
       </c>
       <c r="B285" t="n">
-        <v>7198.1220703125</v>
+        <v>7411.87890625</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>62486.65</v>
       </c>
       <c r="B286" t="n">
-        <v>61347.0234375</v>
+        <v>61314.11328125</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>5170.27</v>
       </c>
       <c r="B287" t="n">
-        <v>6453.4833984375</v>
+        <v>4648.9228515625</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>8168.39</v>
       </c>
       <c r="B288" t="n">
-        <v>9321.349609375</v>
+        <v>7830.98876953125</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>27219.61</v>
       </c>
       <c r="B289" t="n">
-        <v>26130.1640625</v>
+        <v>26115.498046875</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>9301.530000000001</v>
       </c>
       <c r="B290" t="n">
-        <v>9730.9541015625</v>
+        <v>8900.2978515625</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>6010.01</v>
       </c>
       <c r="B291" t="n">
-        <v>8109.01611328125</v>
+        <v>5754.48291015625</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>3545.37</v>
       </c>
       <c r="B292" t="n">
-        <v>6355.2509765625</v>
+        <v>3407.128662109375</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>8439</v>
       </c>
       <c r="B293" t="n">
-        <v>9180.208984375</v>
+        <v>8877.1513671875</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>63987.92000000001</v>
       </c>
       <c r="B294" t="n">
-        <v>61039.26171875</v>
+        <v>64852.09375</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>62224</v>
       </c>
       <c r="B295" t="n">
-        <v>60800.8046875</v>
+        <v>61645.4765625</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>6708</v>
       </c>
       <c r="B296" t="n">
-        <v>8552.4375</v>
+        <v>5816.6357421875</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>8733.27</v>
       </c>
       <c r="B297" t="n">
-        <v>8749.302734375</v>
+        <v>8649.1103515625</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>65300.63</v>
       </c>
       <c r="B298" t="n">
-        <v>66351.1640625</v>
+        <v>68337.34375</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>3403.55</v>
       </c>
       <c r="B299" t="n">
-        <v>5814.630859375</v>
+        <v>3237.740478515625</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>9666.299999999999</v>
       </c>
       <c r="B300" t="n">
-        <v>10444.7529296875</v>
+        <v>9902.0205078125</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>28028.53</v>
       </c>
       <c r="B301" t="n">
-        <v>26897.716796875</v>
+        <v>26881.9453125</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>10374.99</v>
       </c>
       <c r="B302" t="n">
-        <v>9390.13671875</v>
+        <v>10089.6865234375</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>3969.74</v>
       </c>
       <c r="B303" t="n">
-        <v>6296.90576171875</v>
+        <v>3185.351318359375</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>22197.96</v>
       </c>
       <c r="B304" t="n">
-        <v>21445.515625</v>
+        <v>21644.9296875</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>8462</v>
       </c>
       <c r="B305" t="n">
-        <v>9413.666015625</v>
+        <v>8136.93505859375</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>16150.03</v>
       </c>
       <c r="B306" t="n">
-        <v>16276.9482421875</v>
+        <v>15370.4462890625</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>50053.9</v>
       </c>
       <c r="B307" t="n">
-        <v>47587.37109375</v>
+        <v>49920.734375</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>20862.47</v>
       </c>
       <c r="B308" t="n">
-        <v>20080.30078125</v>
+        <v>20891.77734375</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>3862.2</v>
       </c>
       <c r="B309" t="n">
-        <v>4379.236328125</v>
+        <v>4307.67138671875</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>46914.16</v>
       </c>
       <c r="B310" t="n">
-        <v>45902.55859375</v>
+        <v>48161.04296875</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>7375.96</v>
       </c>
       <c r="B311" t="n">
-        <v>7128.45068359375</v>
+        <v>7300.45263671875</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>25728.2</v>
       </c>
       <c r="B312" t="n">
-        <v>26771.517578125</v>
+        <v>26294.439453125</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>38795.69</v>
       </c>
       <c r="B313" t="n">
-        <v>39259.953125</v>
+        <v>40455.32421875</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>16291.86</v>
       </c>
       <c r="B314" t="n">
-        <v>15680.640625</v>
+        <v>15285.208984375</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>23554.85</v>
       </c>
       <c r="B315" t="n">
-        <v>20897.880859375</v>
+        <v>22605.001953125</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>46446.1</v>
       </c>
       <c r="B316" t="n">
-        <v>47096.05078125</v>
+        <v>46791.37890625</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>10174.18</v>
       </c>
       <c r="B317" t="n">
-        <v>11805.9609375</v>
+        <v>10889.2119140625</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>22667.21</v>
       </c>
       <c r="B318" t="n">
-        <v>23218.24609375</v>
+        <v>21072.591796875</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>10776.59</v>
       </c>
       <c r="B319" t="n">
-        <v>11756.0009765625</v>
+        <v>10531.1669921875</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>47153.69</v>
       </c>
       <c r="B320" t="n">
-        <v>48721.5859375</v>
+        <v>48850.921875</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>3932.44</v>
       </c>
       <c r="B321" t="n">
-        <v>6452.0478515625</v>
+        <v>4444.22998046875</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>58050</v>
       </c>
       <c r="B322" t="n">
-        <v>56118.51171875</v>
+        <v>58653.98046875</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>11754.59</v>
       </c>
       <c r="B323" t="n">
-        <v>11724.150390625</v>
+        <v>11924.8857421875</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>6468.99</v>
       </c>
       <c r="B324" t="n">
-        <v>8110.064453125</v>
+        <v>5808.7998046875</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>27628.27</v>
       </c>
       <c r="B325" t="n">
-        <v>28164.095703125</v>
+        <v>27985.75390625</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>45511</v>
       </c>
       <c r="B326" t="n">
-        <v>47069.6015625</v>
+        <v>46398.06640625</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>12543.41</v>
       </c>
       <c r="B327" t="n">
-        <v>12589.455078125</v>
+        <v>11708.5478515625</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>3743.56</v>
       </c>
       <c r="B328" t="n">
-        <v>5353.50927734375</v>
+        <v>3688.27294921875</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>43082.31</v>
       </c>
       <c r="B329" t="n">
-        <v>44327.69140625</v>
+        <v>43498.21484375</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>11071.35</v>
       </c>
       <c r="B330" t="n">
-        <v>11773.9501953125</v>
+        <v>10959.1357421875</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>57339.89</v>
       </c>
       <c r="B331" t="n">
-        <v>56985.58984375</v>
+        <v>59790.28125</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>3567.91</v>
       </c>
       <c r="B332" t="n">
-        <v>6861.4794921875</v>
+        <v>3562.650634765625</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>5655.94</v>
       </c>
       <c r="B333" t="n">
-        <v>7225.10595703125</v>
+        <v>5181.51220703125</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>69469.99000000001</v>
       </c>
       <c r="B334" t="n">
-        <v>67888.1328125</v>
+        <v>68919</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>9465.139999999999</v>
       </c>
       <c r="B335" t="n">
-        <v>11011.6572265625</v>
+        <v>9610.2861328125</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>29109.15</v>
       </c>
       <c r="B336" t="n">
-        <v>30116.8359375</v>
+        <v>33106.89453125</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>14378.9</v>
       </c>
       <c r="B337" t="n">
-        <v>14771.6689453125</v>
+        <v>14507.9951171875</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>11780</v>
       </c>
       <c r="B338" t="n">
-        <v>11441.650390625</v>
+        <v>11770.759765625</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>26852.48</v>
       </c>
       <c r="B339" t="n">
-        <v>26370.73046875</v>
+        <v>27212.197265625</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>7603.44</v>
       </c>
       <c r="B340" t="n">
-        <v>8542.34375</v>
+        <v>6912.7080078125</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>6298.01</v>
       </c>
       <c r="B341" t="n">
-        <v>8152.3544921875</v>
+        <v>6035.51220703125</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>11744.91</v>
       </c>
       <c r="B342" t="n">
-        <v>11439.955078125</v>
+        <v>11129.3359375</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>27033.84</v>
       </c>
       <c r="B343" t="n">
-        <v>26532.150390625</v>
+        <v>26819.650390625</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>70799.06000000001</v>
       </c>
       <c r="B344" t="n">
-        <v>66225.796875</v>
+        <v>69152.0625</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>8189.99</v>
       </c>
       <c r="B345" t="n">
-        <v>9171.05078125</v>
+        <v>8322.755859375</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>42849.78</v>
       </c>
       <c r="B346" t="n">
-        <v>41755.84375</v>
+        <v>43205.91796875</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>34258.14</v>
       </c>
       <c r="B347" t="n">
-        <v>33288.41015625</v>
+        <v>33687.45703125</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>21529.12</v>
       </c>
       <c r="B348" t="n">
-        <v>22094.564453125</v>
+        <v>21274.818359375</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>23232.76</v>
       </c>
       <c r="B349" t="n">
-        <v>22596.9296875</v>
+        <v>22812.83203125</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>48440.65</v>
       </c>
       <c r="B350" t="n">
-        <v>47447.55078125</v>
+        <v>49598.10546875</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>34051.24</v>
       </c>
       <c r="B351" t="n">
-        <v>34884.8671875</v>
+        <v>35303.8984375</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>19289.91</v>
       </c>
       <c r="B352" t="n">
-        <v>19612.060546875</v>
+        <v>18545.642578125</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>41461.83</v>
       </c>
       <c r="B353" t="n">
-        <v>42389.40625</v>
+        <v>41969.5625</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>11820.86</v>
       </c>
       <c r="B354" t="n">
-        <v>12433.697265625</v>
+        <v>11342.0615234375</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>6712.1</v>
       </c>
       <c r="B355" t="n">
-        <v>7865.3095703125</v>
+        <v>6132.3671875</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>7784.02</v>
       </c>
       <c r="B356" t="n">
-        <v>9565.8076171875</v>
+        <v>8535.1552734375</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>40515.7</v>
       </c>
       <c r="B357" t="n">
-        <v>41562.515625</v>
+        <v>41747.73046875</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>19327.44</v>
       </c>
       <c r="B358" t="n">
-        <v>18934.708984375</v>
+        <v>18978.423828125</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>16070.45</v>
       </c>
       <c r="B359" t="n">
-        <v>15860.6044921875</v>
+        <v>15622.970703125</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>3583.13</v>
       </c>
       <c r="B360" t="n">
-        <v>6069.9560546875</v>
+        <v>3224.470703125</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>30366.15</v>
       </c>
       <c r="B361" t="n">
-        <v>32364.767578125</v>
+        <v>32341.77734375</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>22622.98</v>
       </c>
       <c r="B362" t="n">
-        <v>22669.919921875</v>
+        <v>22145.359375</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>37818.87</v>
       </c>
       <c r="B363" t="n">
-        <v>36615.25390625</v>
+        <v>38063.16015625</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>5219.9</v>
       </c>
       <c r="B364" t="n">
-        <v>7374.05712890625</v>
+        <v>4677.78759765625</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>11388.54</v>
       </c>
       <c r="B365" t="n">
-        <v>11638.4853515625</v>
+        <v>11105.1923828125</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>8292.440000000001</v>
       </c>
       <c r="B366" t="n">
-        <v>9204.48828125</v>
+        <v>8166.2509765625</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>23060.94</v>
       </c>
       <c r="B367" t="n">
-        <v>23203.625</v>
+        <v>21303.638671875</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>44399</v>
       </c>
       <c r="B368" t="n">
-        <v>45751.3203125</v>
+        <v>45900.48828125</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>7457</v>
       </c>
       <c r="B369" t="n">
-        <v>8121.833984375</v>
+        <v>7574.509765625</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>39457.87</v>
       </c>
       <c r="B370" t="n">
-        <v>37787.23828125</v>
+        <v>38568.2578125</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>58712.59</v>
       </c>
       <c r="B371" t="n">
-        <v>57474.484375</v>
+        <v>60558.1640625</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>24998.78</v>
       </c>
       <c r="B372" t="n">
-        <v>24842.1484375</v>
+        <v>24538.1796875</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>43902.66</v>
       </c>
       <c r="B373" t="n">
-        <v>41737.59765625</v>
+        <v>43078.62890625</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>11526.91</v>
       </c>
       <c r="B374" t="n">
-        <v>11620.763671875</v>
+        <v>11503.8759765625</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>7302.01</v>
       </c>
       <c r="B375" t="n">
-        <v>9002.333984375</v>
+        <v>6730.59033203125</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>23152.19</v>
       </c>
       <c r="B376" t="n">
-        <v>22737.015625</v>
+        <v>22926.99609375</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>28500.78</v>
       </c>
       <c r="B377" t="n">
-        <v>27796.154296875</v>
+        <v>28137.34765625</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>5683.9</v>
       </c>
       <c r="B378" t="n">
-        <v>8152.09912109375</v>
+        <v>5768.056640625</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>36552.97</v>
       </c>
       <c r="B379" t="n">
-        <v>36896.16015625</v>
+        <v>37120.1171875</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>55857.81</v>
       </c>
       <c r="B380" t="n">
-        <v>55564.28125</v>
+        <v>57874.1015625</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>26281.66</v>
       </c>
       <c r="B381" t="n">
-        <v>26381.828125</v>
+        <v>25906.587890625</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>8115.82</v>
       </c>
       <c r="B382" t="n">
-        <v>8539.9462890625</v>
+        <v>7848.4541015625</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>6841.37</v>
       </c>
       <c r="B383" t="n">
-        <v>10015.927734375</v>
+        <v>6861.1416015625</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>27510.93</v>
       </c>
       <c r="B384" t="n">
-        <v>27975.521484375</v>
+        <v>27328.0234375</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>11293.22</v>
       </c>
       <c r="B385" t="n">
-        <v>11780.734375</v>
+        <v>10731.9873046875</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>9694.51</v>
       </c>
       <c r="B386" t="n">
-        <v>10267.65625</v>
+        <v>10350.9287109375</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>20591.84</v>
       </c>
       <c r="B387" t="n">
-        <v>20032.572265625</v>
+        <v>19791.62890625</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>9242.620000000003</v>
       </c>
       <c r="B388" t="n">
-        <v>9944.2666015625</v>
+        <v>9307.845703125</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>64628</v>
       </c>
       <c r="B389" t="n">
-        <v>63154.265625</v>
+        <v>65627.2734375</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>6162.37</v>
       </c>
       <c r="B390" t="n">
-        <v>6812.96875</v>
+        <v>5686.07080078125</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>23810.79</v>
       </c>
       <c r="B391" t="n">
-        <v>23202.328125</v>
+        <v>23075.505859375</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>6387.96</v>
       </c>
       <c r="B392" t="n">
-        <v>8004.88037109375</v>
+        <v>6249.42919921875</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>4041.32</v>
       </c>
       <c r="B393" t="n">
-        <v>5169.0283203125</v>
+        <v>4029.89013671875</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>6485.85</v>
       </c>
       <c r="B394" t="n">
-        <v>8114.998046875</v>
+        <v>5843.41357421875</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>28415.29</v>
       </c>
       <c r="B395" t="n">
-        <v>28176.689453125</v>
+        <v>27885.078125</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>10126.65</v>
       </c>
       <c r="B396" t="n">
-        <v>11998.9404296875</v>
+        <v>10550.341796875</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>20954.92</v>
       </c>
       <c r="B397" t="n">
-        <v>21909.56640625</v>
+        <v>19117.423828125</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>66915.2</v>
       </c>
       <c r="B398" t="n">
-        <v>62439.9375</v>
+        <v>67110.9453125</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>6185.05</v>
       </c>
       <c r="B399" t="n">
-        <v>8388.0400390625</v>
+        <v>6587.9443359375</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>41492.39</v>
       </c>
       <c r="B400" t="n">
-        <v>41838.44921875</v>
+        <v>41242.3359375</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>8064.92</v>
       </c>
       <c r="B401" t="n">
-        <v>7716.4833984375</v>
+        <v>7846.74462890625</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>62959.53</v>
       </c>
       <c r="B402" t="n">
-        <v>56461.19140625</v>
+        <v>62009.59765625</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>26821.28</v>
       </c>
       <c r="B403" t="n">
-        <v>26683.416015625</v>
+        <v>26615.609375</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>4117.76</v>
       </c>
       <c r="B404" t="n">
-        <v>6104.6923828125</v>
+        <v>3636.288330078125</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>43794.37</v>
       </c>
       <c r="B405" t="n">
-        <v>43321.5234375</v>
+        <v>43987.65234375</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>5922.41</v>
       </c>
       <c r="B406" t="n">
-        <v>8300.3671875</v>
+        <v>5282.35693359375</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>42511.1</v>
       </c>
       <c r="B407" t="n">
-        <v>43434.46484375</v>
+        <v>42340.62109375</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>55777.63</v>
       </c>
       <c r="B408" t="n">
-        <v>53603.17578125</v>
+        <v>55125.09375</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>10925.57</v>
       </c>
       <c r="B409" t="n">
-        <v>11387.0146484375</v>
+        <v>10432.79296875</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>7864.5</v>
       </c>
       <c r="B410" t="n">
-        <v>8671.2119140625</v>
+        <v>6961.96875</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>11369.02</v>
       </c>
       <c r="B411" t="n">
-        <v>11808.2841796875</v>
+        <v>10979.5546875</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>5236.900000000001</v>
       </c>
       <c r="B412" t="n">
-        <v>6757.10205078125</v>
+        <v>4756.89404296875</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>20468.81</v>
       </c>
       <c r="B413" t="n">
-        <v>21742.302734375</v>
+        <v>21906.4296875</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>25805.05</v>
       </c>
       <c r="B414" t="n">
-        <v>26534.6171875</v>
+        <v>25671.5078125</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>6895.8</v>
       </c>
       <c r="B415" t="n">
-        <v>7836.21533203125</v>
+        <v>7251.34228515625</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>9364.999999999998</v>
       </c>
       <c r="B416" t="n">
-        <v>9837.4970703125</v>
+        <v>9013.537109375</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>24842.2</v>
       </c>
       <c r="B417" t="n">
-        <v>24439.10546875</v>
+        <v>23690.970703125</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>5361.3</v>
       </c>
       <c r="B418" t="n">
-        <v>7586.3212890625</v>
+        <v>5762.14404296875</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>25598.49</v>
       </c>
       <c r="B419" t="n">
-        <v>25332.818359375</v>
+        <v>25746.990234375</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>61498.33</v>
       </c>
       <c r="B420" t="n">
-        <v>62043.796875</v>
+        <v>63429.9609375</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>44042.99</v>
       </c>
       <c r="B421" t="n">
-        <v>43488.37109375</v>
+        <v>44641.6171875</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>9315.84</v>
       </c>
       <c r="B422" t="n">
-        <v>10405.8046875</v>
+        <v>9564.5576171875</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>7604.58</v>
       </c>
       <c r="B423" t="n">
-        <v>8379.0576171875</v>
+        <v>7844.68212890625</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>49224.94</v>
       </c>
       <c r="B424" t="n">
-        <v>47071.9921875</v>
+        <v>49704.90234375</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>34525.89</v>
       </c>
       <c r="B425" t="n">
-        <v>33490.71875</v>
+        <v>33091.078125</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>46834.48</v>
       </c>
       <c r="B426" t="n">
-        <v>45643.5</v>
+        <v>47301.59765625</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>68352.17</v>
       </c>
       <c r="B427" t="n">
-        <v>64566.14453125</v>
+        <v>68647.6328125</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>9896.799999999999</v>
       </c>
       <c r="B428" t="n">
-        <v>10780.9375</v>
+        <v>9143.5322265625</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>56714.62</v>
       </c>
       <c r="B429" t="n">
-        <v>54791.3046875</v>
+        <v>58063.359375</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>3875.21</v>
       </c>
       <c r="B430" t="n">
-        <v>4653.93896484375</v>
+        <v>4241.41552734375</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>8873.030000000001</v>
       </c>
       <c r="B431" t="n">
-        <v>11893.484375</v>
+        <v>9542.783203125</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>39280.33</v>
       </c>
       <c r="B432" t="n">
-        <v>39213.5078125</v>
+        <v>40407.50390625</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>9058.26</v>
       </c>
       <c r="B433" t="n">
-        <v>10095.2890625</v>
+        <v>9167.6572265625</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>35546.11000000001</v>
       </c>
       <c r="B434" t="n">
-        <v>36531.765625</v>
+        <v>37895.56640625</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>22916.45</v>
       </c>
       <c r="B435" t="n">
-        <v>22448.072265625</v>
+        <v>21614.224609375</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>63606.74</v>
       </c>
       <c r="B436" t="n">
-        <v>61375.58984375</v>
+        <v>64875.50390625</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>9310</v>
       </c>
       <c r="B437" t="n">
-        <v>8953.166015625</v>
+        <v>8882.7587890625</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>57541.06</v>
       </c>
       <c r="B438" t="n">
-        <v>55302.1953125</v>
+        <v>58605.84765625</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>22583.72</v>
       </c>
       <c r="B439" t="n">
-        <v>21422.85546875</v>
+        <v>22619.298828125</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>3224.17</v>
       </c>
       <c r="B440" t="n">
-        <v>6201.43212890625</v>
+        <v>3394.729248046875</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>8491.02</v>
       </c>
       <c r="B441" t="n">
-        <v>9333.78125</v>
+        <v>8216.73828125</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>5024.95</v>
       </c>
       <c r="B442" t="n">
-        <v>6165.9296875</v>
+        <v>4958.18701171875</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>16738.21</v>
       </c>
       <c r="B443" t="n">
-        <v>17745.9453125</v>
+        <v>16555.49609375</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>43789.51</v>
       </c>
       <c r="B444" t="n">
-        <v>43003.46875</v>
+        <v>41827.2890625</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>46580.51000000001</v>
       </c>
       <c r="B445" t="n">
-        <v>45040.85546875</v>
+        <v>46817.828125</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>3434.1</v>
       </c>
       <c r="B446" t="n">
-        <v>5668.013671875</v>
+        <v>2674.382080078125</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>64774.26</v>
       </c>
       <c r="B447" t="n">
-        <v>62275.30859375</v>
+        <v>65703.390625</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>47100.89</v>
       </c>
       <c r="B448" t="n">
-        <v>47726.3515625</v>
+        <v>49765.05859375</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>6070.780000000001</v>
       </c>
       <c r="B449" t="n">
-        <v>7010.5703125</v>
+        <v>6158.9765625</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>3819.93</v>
       </c>
       <c r="B450" t="n">
-        <v>5588.93701171875</v>
+        <v>3731.389892578125</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>63866</v>
       </c>
       <c r="B451" t="n">
-        <v>60684.4453125</v>
+        <v>64429.59765625</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>3434.15</v>
       </c>
       <c r="B452" t="n">
-        <v>5766.4365234375</v>
+        <v>2805.12158203125</v>
       </c>
     </row>
     <row r="453">
@@ -4058,7 +4058,7 @@
         <v>30304.65</v>
       </c>
       <c r="B453" t="n">
-        <v>29911.13671875</v>
+        <v>30395.3359375</v>
       </c>
     </row>
     <row r="454">
@@ -4066,7 +4066,7 @@
         <v>26844.35</v>
       </c>
       <c r="B454" t="n">
-        <v>25835.095703125</v>
+        <v>26401.837890625</v>
       </c>
     </row>
     <row r="455">
@@ -4074,7 +4074,7 @@
         <v>46374.87</v>
       </c>
       <c r="B455" t="n">
-        <v>40917.5078125</v>
+        <v>43005.37890625</v>
       </c>
     </row>
     <row r="456">
@@ -4082,7 +4082,7 @@
         <v>6285</v>
       </c>
       <c r="B456" t="n">
-        <v>6953.09521484375</v>
+        <v>6371.25146484375</v>
       </c>
     </row>
     <row r="457">
@@ -4090,7 +4090,7 @@
         <v>55953.45</v>
       </c>
       <c r="B457" t="n">
-        <v>55982.1015625</v>
+        <v>59080.28515625</v>
       </c>
     </row>
     <row r="458">
@@ -4098,7 +4098,7 @@
         <v>68549.99000000001</v>
       </c>
       <c r="B458" t="n">
-        <v>65617.6171875</v>
+        <v>68488.9765625</v>
       </c>
     </row>
     <row r="459">
@@ -4106,7 +4106,7 @@
         <v>68398.39</v>
       </c>
       <c r="B459" t="n">
-        <v>64249.4296875</v>
+        <v>68768.3671875</v>
       </c>
     </row>
     <row r="460">
@@ -4114,7 +4114,7 @@
         <v>44349.6</v>
       </c>
       <c r="B460" t="n">
-        <v>44223.44921875</v>
+        <v>44790.80078125</v>
       </c>
     </row>
     <row r="461">
@@ -4122,7 +4122,7 @@
         <v>30086.74</v>
       </c>
       <c r="B461" t="n">
-        <v>30490.55859375</v>
+        <v>28835.322265625</v>
       </c>
     </row>
     <row r="462">
@@ -4130,7 +4130,7 @@
         <v>7487</v>
       </c>
       <c r="B462" t="n">
-        <v>8069.501953125</v>
+        <v>7216.19384765625</v>
       </c>
     </row>
     <row r="463">
@@ -4138,7 +4138,7 @@
         <v>6433.98</v>
       </c>
       <c r="B463" t="n">
-        <v>8211.935546875</v>
+        <v>5961.53759765625</v>
       </c>
     </row>
     <row r="464">
@@ -4146,7 +4146,7 @@
         <v>49699.59</v>
       </c>
       <c r="B464" t="n">
-        <v>50446.1796875</v>
+        <v>49525.1640625</v>
       </c>
     </row>
     <row r="465">
@@ -4154,7 +4154,7 @@
         <v>3951.64</v>
       </c>
       <c r="B465" t="n">
-        <v>5886.626953125</v>
+        <v>3468.145263671875</v>
       </c>
     </row>
     <row r="466">
@@ -4162,7 +4162,7 @@
         <v>11699.99</v>
       </c>
       <c r="B466" t="n">
-        <v>12195.0087890625</v>
+        <v>12451.7119140625</v>
       </c>
     </row>
     <row r="467">
@@ -4170,7 +4170,7 @@
         <v>41382.59</v>
       </c>
       <c r="B467" t="n">
-        <v>40990.27734375</v>
+        <v>40779.51953125</v>
       </c>
     </row>
     <row r="468">
@@ -4178,7 +4178,7 @@
         <v>16542.4</v>
       </c>
       <c r="B468" t="n">
-        <v>18362.361328125</v>
+        <v>16658.087890625</v>
       </c>
     </row>
     <row r="469">
@@ -4186,7 +4186,7 @@
         <v>25934.25</v>
       </c>
       <c r="B469" t="n">
-        <v>25619.240234375</v>
+        <v>25859.072265625</v>
       </c>
     </row>
     <row r="470">
@@ -4194,7 +4194,7 @@
         <v>29201.35</v>
       </c>
       <c r="B470" t="n">
-        <v>29017.498046875</v>
+        <v>31381.505859375</v>
       </c>
     </row>
     <row r="471">
@@ -4202,7 +4202,7 @@
         <v>10728.6</v>
       </c>
       <c r="B471" t="n">
-        <v>11592.05078125</v>
+        <v>10586.1416015625</v>
       </c>
     </row>
     <row r="472">
@@ -4210,7 +4210,7 @@
         <v>8555</v>
       </c>
       <c r="B472" t="n">
-        <v>8847.4228515625</v>
+        <v>7927.13671875</v>
       </c>
     </row>
     <row r="473">
@@ -4218,7 +4218,7 @@
         <v>25759.95</v>
       </c>
       <c r="B473" t="n">
-        <v>26231.701171875</v>
+        <v>25137.45703125</v>
       </c>
     </row>
     <row r="474">
@@ -4226,7 +4226,7 @@
         <v>63201.05</v>
       </c>
       <c r="B474" t="n">
-        <v>58638.109375</v>
+        <v>62310.6484375</v>
       </c>
     </row>
     <row r="475">
@@ -4234,7 +4234,7 @@
         <v>29864.04</v>
       </c>
       <c r="B475" t="n">
-        <v>30480.01171875</v>
+        <v>31252.369140625</v>
       </c>
     </row>
     <row r="476">
@@ -4242,7 +4242,7 @@
         <v>30319.23</v>
       </c>
       <c r="B476" t="n">
-        <v>30925.265625</v>
+        <v>31863.876953125</v>
       </c>
     </row>
     <row r="477">
@@ -4250,7 +4250,7 @@
         <v>10159.98</v>
       </c>
       <c r="B477" t="n">
-        <v>8594.0009765625</v>
+        <v>9716.587890625</v>
       </c>
     </row>
     <row r="478">
@@ -4258,7 +4258,7 @@
         <v>3839.26</v>
       </c>
       <c r="B478" t="n">
-        <v>6706.06689453125</v>
+        <v>3651.466796875</v>
       </c>
     </row>
     <row r="479">
@@ -4266,7 +4266,7 @@
         <v>24631.95</v>
       </c>
       <c r="B479" t="n">
-        <v>23563.6796875</v>
+        <v>22904.46875</v>
       </c>
     </row>
     <row r="480">
@@ -4274,7 +4274,7 @@
         <v>57970.9</v>
       </c>
       <c r="B480" t="n">
-        <v>56145.80859375</v>
+        <v>58389.078125</v>
       </c>
     </row>
     <row r="481">
@@ -4282,7 +4282,7 @@
         <v>7257.45</v>
       </c>
       <c r="B481" t="n">
-        <v>8124.28369140625</v>
+        <v>7452.9287109375</v>
       </c>
     </row>
     <row r="482">
@@ -4290,7 +4290,7 @@
         <v>50399.66</v>
       </c>
       <c r="B482" t="n">
-        <v>49135.765625</v>
+        <v>49831.6875</v>
       </c>
     </row>
     <row r="483">
@@ -4298,7 +4298,7 @@
         <v>3861.84</v>
       </c>
       <c r="B483" t="n">
-        <v>5648.201171875</v>
+        <v>3493.441162109375</v>
       </c>
     </row>
     <row r="484">
@@ -4306,7 +4306,7 @@
         <v>3553.06</v>
       </c>
       <c r="B484" t="n">
-        <v>6159.05078125</v>
+        <v>3142.62841796875</v>
       </c>
     </row>
     <row r="485">
@@ -4314,7 +4314,7 @@
         <v>37359.86</v>
       </c>
       <c r="B485" t="n">
-        <v>36371.38671875</v>
+        <v>36307.3125</v>
       </c>
     </row>
     <row r="486">
@@ -4322,7 +4322,7 @@
         <v>10142.57</v>
       </c>
       <c r="B486" t="n">
-        <v>10127.4794921875</v>
+        <v>10818.7197265625</v>
       </c>
     </row>
     <row r="487">
@@ -4330,7 +4330,7 @@
         <v>7964.87</v>
       </c>
       <c r="B487" t="n">
-        <v>9117.884765625</v>
+        <v>8061.10498046875</v>
       </c>
     </row>
     <row r="488">
@@ -4338,7 +4338,7 @@
         <v>7693.1</v>
       </c>
       <c r="B488" t="n">
-        <v>9265.7255859375</v>
+        <v>7411.0625</v>
       </c>
     </row>
     <row r="489">
@@ -4346,7 +4346,7 @@
         <v>4161.01</v>
       </c>
       <c r="B489" t="n">
-        <v>5641.29931640625</v>
+        <v>3800.04150390625</v>
       </c>
     </row>
     <row r="490">
@@ -4354,7 +4354,7 @@
         <v>3476.81</v>
       </c>
       <c r="B490" t="n">
-        <v>6097.89697265625</v>
+        <v>3184.420654296875</v>
       </c>
     </row>
     <row r="491">
@@ -4362,7 +4362,7 @@
         <v>3838.66</v>
       </c>
       <c r="B491" t="n">
-        <v>5412.46337890625</v>
+        <v>3486.130615234375</v>
       </c>
     </row>
     <row r="492">
@@ -4370,7 +4370,7 @@
         <v>11039</v>
       </c>
       <c r="B492" t="n">
-        <v>10841.951171875</v>
+        <v>10656.50390625</v>
       </c>
     </row>
     <row r="493">
@@ -4378,7 +4378,7 @@
         <v>6505.6</v>
       </c>
       <c r="B493" t="n">
-        <v>8921.58203125</v>
+        <v>6489.978515625</v>
       </c>
     </row>
     <row r="494">
@@ -4386,7 +4386,7 @@
         <v>27598.75</v>
       </c>
       <c r="B494" t="n">
-        <v>27893.45703125</v>
+        <v>27777.34765625</v>
       </c>
     </row>
     <row r="495">
@@ -4394,7 +4394,7 @@
         <v>8725.98</v>
       </c>
       <c r="B495" t="n">
-        <v>8721.30078125</v>
+        <v>7872.060546875</v>
       </c>
     </row>
     <row r="496">
@@ -4402,7 +4402,7 @@
         <v>29031.33</v>
       </c>
       <c r="B496" t="n">
-        <v>28735.900390625</v>
+        <v>31153.556640625</v>
       </c>
     </row>
     <row r="497">
@@ -4410,7 +4410,7 @@
         <v>11454</v>
       </c>
       <c r="B497" t="n">
-        <v>11392.3798828125</v>
+        <v>10564.42578125</v>
       </c>
     </row>
     <row r="498">
@@ -4418,7 +4418,7 @@
         <v>63892.04</v>
       </c>
       <c r="B498" t="n">
-        <v>61480.00390625</v>
+        <v>63126.52734375</v>
       </c>
     </row>
     <row r="499">
@@ -4426,7 +4426,7 @@
         <v>35796.31</v>
       </c>
       <c r="B499" t="n">
-        <v>36658.5546875</v>
+        <v>38178.9765625</v>
       </c>
     </row>
     <row r="500">
@@ -4434,7 +4434,7 @@
         <v>30083.75</v>
       </c>
       <c r="B500" t="n">
-        <v>29861.9296875</v>
+        <v>29581.57421875</v>
       </c>
     </row>
     <row r="501">
@@ -4442,7 +4442,7 @@
         <v>3665.18</v>
       </c>
       <c r="B501" t="n">
-        <v>5613.67529296875</v>
+        <v>2725.744873046875</v>
       </c>
     </row>
     <row r="502">
@@ -4450,7 +4450,7 @@
         <v>7303</v>
       </c>
       <c r="B502" t="n">
-        <v>9025.3818359375</v>
+        <v>6071.14501953125</v>
       </c>
     </row>
     <row r="503">
@@ -4458,7 +4458,7 @@
         <v>9128.02</v>
       </c>
       <c r="B503" t="n">
-        <v>10069.1474609375</v>
+        <v>8300.5712890625</v>
       </c>
     </row>
     <row r="504">
@@ -4466,7 +4466,7 @@
         <v>10446.25</v>
       </c>
       <c r="B504" t="n">
-        <v>11991.32421875</v>
+        <v>10445.19921875</v>
       </c>
     </row>
     <row r="505">
@@ -4474,7 +4474,7 @@
         <v>46025.24</v>
       </c>
       <c r="B505" t="n">
-        <v>45539.19921875</v>
+        <v>46355.37890625</v>
       </c>
     </row>
     <row r="506">
@@ -4482,7 +4482,7 @@
         <v>38466.9</v>
       </c>
       <c r="B506" t="n">
-        <v>38255.64453125</v>
+        <v>38411.28125</v>
       </c>
     </row>
     <row r="507">
@@ -4490,7 +4490,7 @@
         <v>7064.04</v>
       </c>
       <c r="B507" t="n">
-        <v>8601.416015625</v>
+        <v>5957.85888671875</v>
       </c>
     </row>
     <row r="508">
@@ -4498,7 +4498,7 @@
         <v>7210</v>
       </c>
       <c r="B508" t="n">
-        <v>8112.27978515625</v>
+        <v>7295.41845703125</v>
       </c>
     </row>
     <row r="509">
@@ -4506,7 +4506,7 @@
         <v>61528.33</v>
       </c>
       <c r="B509" t="n">
-        <v>57981.40234375</v>
+        <v>62712.8125</v>
       </c>
     </row>
     <row r="510">
@@ -4514,7 +4514,7 @@
         <v>23191.2</v>
       </c>
       <c r="B510" t="n">
-        <v>23114.08984375</v>
+        <v>22806.345703125</v>
       </c>
     </row>
     <row r="511">
@@ -4522,7 +4522,7 @@
         <v>26575.96</v>
       </c>
       <c r="B511" t="n">
-        <v>26782.142578125</v>
+        <v>26045.287109375</v>
       </c>
     </row>
     <row r="512">
@@ -4530,7 +4530,7 @@
         <v>10760.05</v>
       </c>
       <c r="B512" t="n">
-        <v>11419.130859375</v>
+        <v>11071.9931640625</v>
       </c>
     </row>
     <row r="513">
@@ -4538,7 +4538,7 @@
         <v>66001.41</v>
       </c>
       <c r="B513" t="n">
-        <v>62237.83203125</v>
+        <v>66598.8359375</v>
       </c>
     </row>
     <row r="514">
@@ -4546,7 +4546,7 @@
         <v>6208.36</v>
       </c>
       <c r="B514" t="n">
-        <v>7606.171875</v>
+        <v>5649.4619140625</v>
       </c>
     </row>
     <row r="515">
@@ -4554,7 +4554,7 @@
         <v>56900.75</v>
       </c>
       <c r="B515" t="n">
-        <v>54514.02734375</v>
+        <v>56843.67578125</v>
       </c>
     </row>
     <row r="516">
@@ -4562,7 +4562,7 @@
         <v>5709.99</v>
       </c>
       <c r="B516" t="n">
-        <v>7680.1376953125</v>
+        <v>5272.162109375</v>
       </c>
     </row>
     <row r="517">
@@ -4570,7 +4570,7 @@
         <v>69582.17999999999</v>
       </c>
       <c r="B517" t="n">
-        <v>66881.7265625</v>
+        <v>69063.9609375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added future predictions from lstm model
</commit_message>
<xml_diff>
--- a/Stored_data/predictions_test.xlsx
+++ b/Stored_data/predictions_test.xlsx
@@ -450,7 +450,7 @@
         <v>12780.96</v>
       </c>
       <c r="B2" t="n">
-        <v>11891.1044921875</v>
+        <v>12352.564453125</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>7283.54</v>
       </c>
       <c r="B3" t="n">
-        <v>7360.3544921875</v>
+        <v>6229.8505859375</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>7948.01</v>
       </c>
       <c r="B4" t="n">
-        <v>7948.3515625</v>
+        <v>7509.443359375</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>7009.84</v>
       </c>
       <c r="B5" t="n">
-        <v>7227.56396484375</v>
+        <v>7646.74609375</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>27454.47</v>
       </c>
       <c r="B6" t="n">
-        <v>26368.28125</v>
+        <v>27199.630859375</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>9529.93</v>
       </c>
       <c r="B7" t="n">
-        <v>8422.0966796875</v>
+        <v>7800.3388671875</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>7338.64</v>
       </c>
       <c r="B8" t="n">
-        <v>7298.56103515625</v>
+        <v>7205.873046875</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>57338</v>
       </c>
       <c r="B9" t="n">
-        <v>58413.3671875</v>
+        <v>57363.296875</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>19422.61</v>
       </c>
       <c r="B10" t="n">
-        <v>18689.810546875</v>
+        <v>18599.337890625</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>34669.13</v>
       </c>
       <c r="B11" t="n">
-        <v>33811.62109375</v>
+        <v>32976.65625</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>64262.7</v>
       </c>
       <c r="B12" t="n">
-        <v>63943.12109375</v>
+        <v>63301.11328125</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>8810.790000000003</v>
       </c>
       <c r="B13" t="n">
-        <v>9307.30078125</v>
+        <v>8772.8466796875</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>58202.01</v>
       </c>
       <c r="B14" t="n">
-        <v>58184.44921875</v>
+        <v>58233.359375</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>10340.31</v>
       </c>
       <c r="B15" t="n">
-        <v>10760.02734375</v>
+        <v>10445.2578125</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>37449.73</v>
       </c>
       <c r="B16" t="n">
-        <v>38427.3515625</v>
+        <v>36999.67578125</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>3715.3</v>
       </c>
       <c r="B17" t="n">
-        <v>3567.103759765625</v>
+        <v>4002.35791015625</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>6609.78</v>
       </c>
       <c r="B18" t="n">
-        <v>6068.8115234375</v>
+        <v>6362.017578125</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>7934.52</v>
       </c>
       <c r="B19" t="n">
-        <v>7487.83154296875</v>
+        <v>7388.341796875</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>7508.52</v>
       </c>
       <c r="B20" t="n">
-        <v>7938.42578125</v>
+        <v>8070.56005859375</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>60752.71000000001</v>
       </c>
       <c r="B21" t="n">
-        <v>61505.6796875</v>
+        <v>60387.3359375</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>6250.81</v>
       </c>
       <c r="B22" t="n">
-        <v>6548.302734375</v>
+        <v>6919.34033203125</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>8187.17</v>
       </c>
       <c r="B23" t="n">
-        <v>8074.67822265625</v>
+        <v>8423.650390625</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>11256.49</v>
       </c>
       <c r="B24" t="n">
-        <v>11413.294921875</v>
+        <v>11376.224609375</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>31801.04</v>
       </c>
       <c r="B25" t="n">
-        <v>31072.72265625</v>
+        <v>28353.689453125</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>47120.87</v>
       </c>
       <c r="B26" t="n">
-        <v>47011.6484375</v>
+        <v>45413.06640625</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>33504.69</v>
       </c>
       <c r="B27" t="n">
-        <v>34068.09375</v>
+        <v>33480.5625</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>9687.879999999999</v>
       </c>
       <c r="B28" t="n">
-        <v>9738.4765625</v>
+        <v>9787.9619140625</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>7240.06</v>
       </c>
       <c r="B29" t="n">
-        <v>6860.58203125</v>
+        <v>7418.90966796875</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>24441.38</v>
       </c>
       <c r="B30" t="n">
-        <v>23737.818359375</v>
+        <v>22593.4765625</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>16812.08</v>
       </c>
       <c r="B31" t="n">
-        <v>16940.80859375</v>
+        <v>16668.421875</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>46653.99</v>
       </c>
       <c r="B32" t="n">
-        <v>45511.03515625</v>
+        <v>45378.89453125</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>38420.81</v>
       </c>
       <c r="B33" t="n">
-        <v>39211.6171875</v>
+        <v>38012.31640625</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>24712.47</v>
       </c>
       <c r="B34" t="n">
-        <v>24083.8203125</v>
+        <v>24841.369140625</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>7316.14</v>
       </c>
       <c r="B35" t="n">
-        <v>7627.2099609375</v>
+        <v>7780.00341796875</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>7824.8</v>
       </c>
       <c r="B36" t="n">
-        <v>8468.376953125</v>
+        <v>8112.1220703125</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>8655.02</v>
       </c>
       <c r="B37" t="n">
-        <v>7974.640625</v>
+        <v>7355.783203125</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>28171.87</v>
       </c>
       <c r="B38" t="n">
-        <v>27305.609375</v>
+        <v>27323.6328125</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>53787.63</v>
       </c>
       <c r="B39" t="n">
-        <v>54178.34765625</v>
+        <v>53374.55078125</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>7115.04</v>
       </c>
       <c r="B40" t="n">
-        <v>5791.43310546875</v>
+        <v>6493.67626953125</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>7120.74</v>
       </c>
       <c r="B41" t="n">
-        <v>6949.76318359375</v>
+        <v>6651.5634765625</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>6144.009999999999</v>
       </c>
       <c r="B42" t="n">
-        <v>6178.015625</v>
+        <v>6751.4921875</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>7991.74</v>
       </c>
       <c r="B43" t="n">
-        <v>7883.4375</v>
+        <v>7746.171875</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>8170</v>
       </c>
       <c r="B44" t="n">
-        <v>8879.55078125</v>
+        <v>8450.224609375</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>47111.52</v>
       </c>
       <c r="B45" t="n">
-        <v>47078.578125</v>
+        <v>45191.76953125</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>21783.54</v>
       </c>
       <c r="B46" t="n">
-        <v>20842.5625</v>
+        <v>21901.052734375</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>8359.940000000001</v>
       </c>
       <c r="B47" t="n">
-        <v>8127.71533203125</v>
+        <v>7910.82470703125</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>44145.11</v>
       </c>
       <c r="B48" t="n">
-        <v>42681.64453125</v>
+        <v>43024.4453125</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>62819.91</v>
       </c>
       <c r="B49" t="n">
-        <v>61553.125</v>
+        <v>61022.89453125</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>29581.99</v>
       </c>
       <c r="B50" t="n">
-        <v>28972.818359375</v>
+        <v>29217.41015625</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>29430.27</v>
       </c>
       <c r="B51" t="n">
-        <v>29778.369140625</v>
+        <v>29270.80078125</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>6734.1</v>
       </c>
       <c r="B52" t="n">
-        <v>6707.2626953125</v>
+        <v>5900.154296875</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>42380.87</v>
       </c>
       <c r="B53" t="n">
-        <v>42247.5234375</v>
+        <v>39883.0234375</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>60058.87</v>
       </c>
       <c r="B54" t="n">
-        <v>62072.61328125</v>
+        <v>61647.7265625</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>70631.08</v>
       </c>
       <c r="B55" t="n">
-        <v>69582.15625</v>
+        <v>69471</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>63152.01</v>
       </c>
       <c r="B56" t="n">
-        <v>63620.13671875</v>
+        <v>63204.8203125</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>3823</v>
       </c>
       <c r="B57" t="n">
-        <v>3762.67626953125</v>
+        <v>4066.844482421875</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>10666.39</v>
       </c>
       <c r="B58" t="n">
-        <v>10720.279296875</v>
+        <v>10066.7177734375</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>62896.48</v>
       </c>
       <c r="B59" t="n">
-        <v>61811.09375</v>
+        <v>61922.8203125</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>34262.88</v>
       </c>
       <c r="B60" t="n">
-        <v>33636.2734375</v>
+        <v>33999.6015625</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>33786.55</v>
       </c>
       <c r="B61" t="n">
-        <v>33736.3828125</v>
+        <v>33018.328125</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>43137.95</v>
       </c>
       <c r="B62" t="n">
-        <v>42901.87109375</v>
+        <v>42635.453125</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>6868.699999999999</v>
       </c>
       <c r="B63" t="n">
-        <v>6888.52685546875</v>
+        <v>6246.486328125</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>10890.01</v>
       </c>
       <c r="B64" t="n">
-        <v>11074.6005859375</v>
+        <v>11024.830078125</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>3680.06</v>
       </c>
       <c r="B65" t="n">
-        <v>2832.24658203125</v>
+        <v>3470.919921875</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>61286.75</v>
       </c>
       <c r="B66" t="n">
-        <v>61702.86328125</v>
+        <v>60343.20703125</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>23742.3</v>
       </c>
       <c r="B67" t="n">
-        <v>22278.197265625</v>
+        <v>22332.853515625</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>29211.06</v>
       </c>
       <c r="B68" t="n">
-        <v>28321.296875</v>
+        <v>28600.4453125</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>3792.01</v>
       </c>
       <c r="B69" t="n">
-        <v>3598.173095703125</v>
+        <v>3478.960693359375</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>68124.19</v>
       </c>
       <c r="B70" t="n">
-        <v>68643.078125</v>
+        <v>67850.4140625</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>48343.28</v>
       </c>
       <c r="B71" t="n">
-        <v>48521.63671875</v>
+        <v>47492.74609375</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>19951.86</v>
       </c>
       <c r="B72" t="n">
-        <v>19508.3671875</v>
+        <v>19355.455078125</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>8055.98</v>
       </c>
       <c r="B73" t="n">
-        <v>7771.85546875</v>
+        <v>8487.74609375</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>26516.99</v>
       </c>
       <c r="B74" t="n">
-        <v>26038.59375</v>
+        <v>26086.568359375</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>9170.280000000001</v>
       </c>
       <c r="B75" t="n">
-        <v>8831.9921875</v>
+        <v>8712.140625</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>10624.93</v>
       </c>
       <c r="B76" t="n">
-        <v>11087.7431640625</v>
+        <v>11251.7333984375</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>9381.27</v>
       </c>
       <c r="B77" t="n">
-        <v>9344.259765625</v>
+        <v>8844.1318359375</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>29770.42</v>
       </c>
       <c r="B78" t="n">
-        <v>28752.220703125</v>
+        <v>28974.447265625</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>40480.01</v>
       </c>
       <c r="B79" t="n">
-        <v>40738.515625</v>
+        <v>39697.1171875</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>45584.99</v>
       </c>
       <c r="B80" t="n">
-        <v>45901.69140625</v>
+        <v>43447.99609375</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>8110.34</v>
       </c>
       <c r="B81" t="n">
-        <v>8380.6982421875</v>
+        <v>8935.9609375</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>62432.1</v>
       </c>
       <c r="B82" t="n">
-        <v>59127.703125</v>
+        <v>58977.5703125</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>29542.15</v>
       </c>
       <c r="B83" t="n">
-        <v>32334.86328125</v>
+        <v>29766.8984375</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>10303.12</v>
       </c>
       <c r="B84" t="n">
-        <v>10390.0458984375</v>
+        <v>9664.50390625</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>56950.56</v>
       </c>
       <c r="B85" t="n">
-        <v>57342.2109375</v>
+        <v>55772.4375</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>37371.38</v>
       </c>
       <c r="B86" t="n">
-        <v>36253.1171875</v>
+        <v>37685.08984375</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>61987.28</v>
       </c>
       <c r="B87" t="n">
-        <v>61747.8671875</v>
+        <v>62061.1875</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>8197.27</v>
       </c>
       <c r="B88" t="n">
-        <v>8018.44189453125</v>
+        <v>7581.28857421875</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>6723.05</v>
       </c>
       <c r="B89" t="n">
-        <v>5811.6796875</v>
+        <v>6471.357421875</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>6410.000000000001</v>
       </c>
       <c r="B90" t="n">
-        <v>6150.89501953125</v>
+        <v>5775.814453125</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>9513.209999999999</v>
       </c>
       <c r="B91" t="n">
-        <v>8938.9482421875</v>
+        <v>9626.6611328125</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>6618.96</v>
       </c>
       <c r="B92" t="n">
-        <v>6406.40576171875</v>
+        <v>6661.63623046875</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>6796.1</v>
       </c>
       <c r="B93" t="n">
-        <v>7273.7958984375</v>
+        <v>6074.28515625</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>7019.98</v>
       </c>
       <c r="B94" t="n">
-        <v>5823.2177734375</v>
+        <v>6485.82421875</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>9160.780000000001</v>
       </c>
       <c r="B95" t="n">
-        <v>8980.2626953125</v>
+        <v>8835.8681640625</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>53555</v>
       </c>
       <c r="B96" t="n">
-        <v>53759.93359375</v>
+        <v>53485.2734375</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>57301.86</v>
       </c>
       <c r="B97" t="n">
-        <v>59286.16796875</v>
+        <v>57432.9375</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>7510.11</v>
       </c>
       <c r="B98" t="n">
-        <v>7324.4716796875</v>
+        <v>7387.99951171875</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>41574.25</v>
       </c>
       <c r="B99" t="n">
-        <v>39344.1796875</v>
+        <v>37500.56640625</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>67116.52</v>
       </c>
       <c r="B100" t="n">
-        <v>66675.390625</v>
+        <v>66539.7890625</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>22346.57</v>
       </c>
       <c r="B101" t="n">
-        <v>21695.505859375</v>
+        <v>22484.6328125</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>66504.33</v>
       </c>
       <c r="B102" t="n">
-        <v>67507.328125</v>
+        <v>67118.2578125</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>22430.24</v>
       </c>
       <c r="B103" t="n">
-        <v>22003.994140625</v>
+        <v>22571.484375</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>13636.17</v>
       </c>
       <c r="B104" t="n">
-        <v>13291.458984375</v>
+        <v>13924.267578125</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>37237.6</v>
       </c>
       <c r="B105" t="n">
-        <v>36574.46484375</v>
+        <v>35002.8203125</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>32945.17</v>
       </c>
       <c r="B106" t="n">
-        <v>32821.88671875</v>
+        <v>33839.71875</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>9227</v>
       </c>
       <c r="B107" t="n">
-        <v>9485.7841796875</v>
+        <v>8836.8720703125</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>50441.92</v>
       </c>
       <c r="B108" t="n">
-        <v>50285.30859375</v>
+        <v>48659.3046875</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>7541.89</v>
       </c>
       <c r="B109" t="n">
-        <v>7731.5478515625</v>
+        <v>8205.4482421875</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>33380.81</v>
       </c>
       <c r="B110" t="n">
-        <v>36395.3984375</v>
+        <v>35354.63671875</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>62312.08</v>
       </c>
       <c r="B111" t="n">
-        <v>63133.6171875</v>
+        <v>61915.35546875</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>45510.34</v>
       </c>
       <c r="B112" t="n">
-        <v>46761.06640625</v>
+        <v>45628.24609375</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>65173.99</v>
       </c>
       <c r="B113" t="n">
-        <v>64768.75390625</v>
+        <v>63748.7890625</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>19421.9</v>
       </c>
       <c r="B114" t="n">
-        <v>19466.634765625</v>
+        <v>19660.306640625</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>8471.73</v>
       </c>
       <c r="B115" t="n">
-        <v>8287.501953125</v>
+        <v>8558.9599609375</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>38207.05</v>
       </c>
       <c r="B116" t="n">
-        <v>40623.12109375</v>
+        <v>38415.65234375</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>8614.43</v>
       </c>
       <c r="B117" t="n">
-        <v>8150.14111328125</v>
+        <v>8629.900390625</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>56180</v>
       </c>
       <c r="B118" t="n">
-        <v>57795.6015625</v>
+        <v>56539.52734375</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>7854.25</v>
       </c>
       <c r="B119" t="n">
-        <v>7903.74560546875</v>
+        <v>7579.4736328125</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>27250.97</v>
       </c>
       <c r="B120" t="n">
-        <v>27156.453125</v>
+        <v>28212.97265625</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>7575.01</v>
       </c>
       <c r="B121" t="n">
-        <v>7644.2861328125</v>
+        <v>7799.65478515625</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>27242.59</v>
       </c>
       <c r="B122" t="n">
-        <v>26770.443359375</v>
+        <v>27086.55859375</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>47287.6</v>
       </c>
       <c r="B123" t="n">
-        <v>48542.05859375</v>
+        <v>46981.5859375</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>17719.85</v>
       </c>
       <c r="B124" t="n">
-        <v>17672.314453125</v>
+        <v>17345.71484375</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>19292.84</v>
       </c>
       <c r="B125" t="n">
-        <v>18317.123046875</v>
+        <v>18648.544921875</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>8173</v>
       </c>
       <c r="B126" t="n">
-        <v>7706.35302734375</v>
+        <v>6368.60888671875</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>36568.1</v>
       </c>
       <c r="B127" t="n">
-        <v>35959.5625</v>
+        <v>36414.859375</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>52124.11</v>
       </c>
       <c r="B128" t="n">
-        <v>50903.28125</v>
+        <v>50284.953125</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>3601.31</v>
       </c>
       <c r="B129" t="n">
-        <v>3251.07373046875</v>
+        <v>3632.303466796875</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>42217.87</v>
       </c>
       <c r="B130" t="n">
-        <v>43415.22265625</v>
+        <v>41341.08984375</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>7056</v>
       </c>
       <c r="B131" t="n">
-        <v>7342.78662109375</v>
+        <v>6248.32568359375</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>27162.14</v>
       </c>
       <c r="B132" t="n">
-        <v>26911.455078125</v>
+        <v>27035.484375</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>33552.79</v>
       </c>
       <c r="B133" t="n">
-        <v>37565.26953125</v>
+        <v>36575.421875</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>30466.93</v>
       </c>
       <c r="B134" t="n">
-        <v>30055.5859375</v>
+        <v>29534.16796875</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>65175.32</v>
       </c>
       <c r="B135" t="n">
-        <v>65928.015625</v>
+        <v>65855.265625</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>58427.35</v>
       </c>
       <c r="B136" t="n">
-        <v>59276.8515625</v>
+        <v>59771.984375</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>9721</v>
       </c>
       <c r="B137" t="n">
-        <v>9938.5458984375</v>
+        <v>9499.6279296875</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>26493.39</v>
       </c>
       <c r="B138" t="n">
-        <v>25125.603515625</v>
+        <v>26133.298828125</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>65936.00999999999</v>
       </c>
       <c r="B139" t="n">
-        <v>67866</v>
+        <v>66328.7109375</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>19329.72</v>
       </c>
       <c r="B140" t="n">
-        <v>19172.814453125</v>
+        <v>19389.59375</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>19417.96</v>
       </c>
       <c r="B141" t="n">
-        <v>19549.265625</v>
+        <v>18904.52734375</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>57221.72</v>
       </c>
       <c r="B142" t="n">
-        <v>55900.7109375</v>
+        <v>56095.5703125</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>25840.1</v>
       </c>
       <c r="B143" t="n">
-        <v>24689.306640625</v>
+        <v>25145.30078125</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>20401.31</v>
       </c>
       <c r="B144" t="n">
-        <v>22093.927734375</v>
+        <v>21531.94921875</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>8785.25</v>
       </c>
       <c r="B145" t="n">
-        <v>9284.2451171875</v>
+        <v>9332.3125</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>52303.65</v>
       </c>
       <c r="B146" t="n">
-        <v>53958.2890625</v>
+        <v>53655.03125</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>9012</v>
       </c>
       <c r="B147" t="n">
-        <v>9261.015625</v>
+        <v>8562.8330078125</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>13326.61</v>
       </c>
       <c r="B148" t="n">
-        <v>15777.546875</v>
+        <v>15558.591796875</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>10842.85</v>
       </c>
       <c r="B149" t="n">
-        <v>11069.6875</v>
+        <v>11187.9052734375</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>15328.41</v>
       </c>
       <c r="B150" t="n">
-        <v>14996.259765625</v>
+        <v>15427.8818359375</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>27494.51</v>
       </c>
       <c r="B151" t="n">
-        <v>27076.8515625</v>
+        <v>27553.685546875</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>29026.16</v>
       </c>
       <c r="B152" t="n">
-        <v>27887.974609375</v>
+        <v>28298.423828125</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>9224.52</v>
       </c>
       <c r="B153" t="n">
-        <v>9851.34375</v>
+        <v>9427.267578125</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>29331.69</v>
       </c>
       <c r="B154" t="n">
-        <v>29993.294921875</v>
+        <v>31428.0390625</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>4295.84</v>
       </c>
       <c r="B155" t="n">
-        <v>4110.89306640625</v>
+        <v>3350.287109375</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>5415</v>
       </c>
       <c r="B156" t="n">
-        <v>4722.2333984375</v>
+        <v>5360.0869140625</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>20627.48</v>
       </c>
       <c r="B157" t="n">
-        <v>20494.998046875</v>
+        <v>20095.591796875</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>9419</v>
       </c>
       <c r="B158" t="n">
-        <v>9134.693359375</v>
+        <v>8768.994140625</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>44695.95</v>
       </c>
       <c r="B159" t="n">
-        <v>46519.0078125</v>
+        <v>44368.14453125</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>23312.42</v>
       </c>
       <c r="B160" t="n">
-        <v>22126.84375</v>
+        <v>21998.15625</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>47800</v>
       </c>
       <c r="B161" t="n">
-        <v>47063.94140625</v>
+        <v>44699.2421875</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>7027.55</v>
       </c>
       <c r="B162" t="n">
-        <v>6856.62939453125</v>
+        <v>6460.78662109375</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>25925.55</v>
       </c>
       <c r="B163" t="n">
-        <v>25864.033203125</v>
+        <v>26034.068359375</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>17085.05</v>
       </c>
       <c r="B164" t="n">
-        <v>17125.244140625</v>
+        <v>16972.69140625</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>7795.51</v>
       </c>
       <c r="B165" t="n">
-        <v>7778.9287109375</v>
+        <v>6970.66943359375</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>9574.209999999999</v>
       </c>
       <c r="B166" t="n">
-        <v>10106.7880859375</v>
+        <v>9774.625</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>3631.05</v>
       </c>
       <c r="B167" t="n">
-        <v>2976.59326171875</v>
+        <v>3590.880126953125</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>20742.56</v>
       </c>
       <c r="B168" t="n">
-        <v>20347.560546875</v>
+        <v>19651.8984375</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>10331.54</v>
       </c>
       <c r="B169" t="n">
-        <v>10378.18359375</v>
+        <v>10083.8740234375</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>38150.02</v>
       </c>
       <c r="B170" t="n">
-        <v>37116.30078125</v>
+        <v>39823.734375</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>9131.34</v>
       </c>
       <c r="B171" t="n">
-        <v>8861.1865234375</v>
+        <v>8482.740234375</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>5308.25</v>
       </c>
       <c r="B172" t="n">
-        <v>4922.36572265625</v>
+        <v>5442.9638671875</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>3594.87</v>
       </c>
       <c r="B173" t="n">
-        <v>3131.335205078125</v>
+        <v>3826.64404296875</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>9292.24</v>
       </c>
       <c r="B174" t="n">
-        <v>9156.0078125</v>
+        <v>9888.828125</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>7390.89</v>
       </c>
       <c r="B175" t="n">
-        <v>7696.18505859375</v>
+        <v>8178.259765625</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>7488.21</v>
       </c>
       <c r="B176" t="n">
-        <v>7392.58984375</v>
+        <v>7489.0908203125</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>30692.44</v>
       </c>
       <c r="B177" t="n">
-        <v>29668.072265625</v>
+        <v>30281.80859375</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>26180.05</v>
       </c>
       <c r="B178" t="n">
-        <v>25756.423828125</v>
+        <v>25737.5546875</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>9518.16</v>
       </c>
       <c r="B179" t="n">
-        <v>9148.5263671875</v>
+        <v>8929.12890625</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>9231.610000000001</v>
       </c>
       <c r="B180" t="n">
-        <v>9144.197265625</v>
+        <v>8588.220703125</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>39942.38</v>
       </c>
       <c r="B181" t="n">
-        <v>40286.359375</v>
+        <v>39247.5390625</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>51568.22</v>
       </c>
       <c r="B182" t="n">
-        <v>52714.2734375</v>
+        <v>52599.1640625</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>63113.97</v>
       </c>
       <c r="B183" t="n">
-        <v>62494.35546875</v>
+        <v>62618.9453125</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>39422</v>
       </c>
       <c r="B184" t="n">
-        <v>39821.19140625</v>
+        <v>39165.82421875</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>30617.03</v>
       </c>
       <c r="B185" t="n">
-        <v>30226.681640625</v>
+        <v>30897.208984375</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>56022.01000000001</v>
       </c>
       <c r="B186" t="n">
-        <v>57867.62890625</v>
+        <v>57340.12109375</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>24305.24</v>
       </c>
       <c r="B187" t="n">
-        <v>23883.998046875</v>
+        <v>22707.6640625</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>6197.92</v>
       </c>
       <c r="B188" t="n">
-        <v>6191.95458984375</v>
+        <v>6158.50732421875</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>8041.46</v>
       </c>
       <c r="B189" t="n">
-        <v>8099.2587890625</v>
+        <v>8404.021484375</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>33892.02</v>
       </c>
       <c r="B190" t="n">
-        <v>32579.056640625</v>
+        <v>33027.48828125</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>9910</v>
       </c>
       <c r="B191" t="n">
-        <v>10021.3505859375</v>
+        <v>9068.3271484375</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>32178.33</v>
       </c>
       <c r="B192" t="n">
-        <v>31804.646484375</v>
+        <v>33522.484375</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>7894.56</v>
       </c>
       <c r="B193" t="n">
-        <v>7678.71337890625</v>
+        <v>7614.21728515625</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>61188.39</v>
       </c>
       <c r="B194" t="n">
-        <v>59113.1171875</v>
+        <v>59437.875</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>50820</v>
       </c>
       <c r="B195" t="n">
-        <v>49174.8515625</v>
+        <v>48233.6796875</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>23009.65</v>
       </c>
       <c r="B196" t="n">
-        <v>21292.78515625</v>
+        <v>21863.9609375</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>20175.83</v>
       </c>
       <c r="B197" t="n">
-        <v>20424.794921875</v>
+        <v>19644.271484375</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>49676.2</v>
       </c>
       <c r="B198" t="n">
-        <v>50123.8671875</v>
+        <v>47967.8984375</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>28715.32</v>
       </c>
       <c r="B199" t="n">
-        <v>30829.64453125</v>
+        <v>29499.947265625</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>47067.99</v>
       </c>
       <c r="B200" t="n">
-        <v>47658.1171875</v>
+        <v>46019.65234375</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>64122.23</v>
       </c>
       <c r="B201" t="n">
-        <v>64517.99609375</v>
+        <v>64429.9921875</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>32254.2</v>
       </c>
       <c r="B202" t="n">
-        <v>32359.38671875</v>
+        <v>33424.60546875</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>30200.42</v>
       </c>
       <c r="B203" t="n">
-        <v>28829.134765625</v>
+        <v>28127.67578125</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>8169.87</v>
       </c>
       <c r="B204" t="n">
-        <v>6969.427734375</v>
+        <v>7543.783203125</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>59346.64</v>
       </c>
       <c r="B205" t="n">
-        <v>60498.21875</v>
+        <v>60575.45703125</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>14400</v>
       </c>
       <c r="B206" t="n">
-        <v>15221.9169921875</v>
+        <v>14212.6259765625</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>8278</v>
       </c>
       <c r="B207" t="n">
-        <v>7888.8896484375</v>
+        <v>6573.59814453125</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>58950.01</v>
       </c>
       <c r="B208" t="n">
-        <v>57975.46875</v>
+        <v>59064.40625</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>6744.719999999999</v>
       </c>
       <c r="B209" t="n">
-        <v>6826.54052734375</v>
+        <v>6092.8671875</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>7527.47</v>
       </c>
       <c r="B210" t="n">
-        <v>7440.333984375</v>
+        <v>7631.841796875</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>10372.25</v>
       </c>
       <c r="B211" t="n">
-        <v>10235.55859375</v>
+        <v>9651.439453125</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>12968.52</v>
       </c>
       <c r="B212" t="n">
-        <v>12293.8955078125</v>
+        <v>12795.8017578125</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>6506.98</v>
       </c>
       <c r="B213" t="n">
-        <v>6306.36083984375</v>
+        <v>6984.189453125</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>8400</v>
       </c>
       <c r="B214" t="n">
-        <v>8656.3427734375</v>
+        <v>9055.83203125</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>28629.8</v>
       </c>
       <c r="B215" t="n">
-        <v>30533.83984375</v>
+        <v>28123.71484375</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>21195.6</v>
       </c>
       <c r="B216" t="n">
-        <v>19673.673828125</v>
+        <v>19321.01953125</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>21299.37</v>
       </c>
       <c r="B217" t="n">
-        <v>20064.642578125</v>
+        <v>19763.177734375</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>51728.85</v>
       </c>
       <c r="B218" t="n">
-        <v>52962.63671875</v>
+        <v>52674.1875</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>69499.85000000001</v>
       </c>
       <c r="B219" t="n">
-        <v>69487.9140625</v>
+        <v>69910.4453125</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>21491.19</v>
       </c>
       <c r="B220" t="n">
-        <v>20882.890625</v>
+        <v>20301.99609375</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>6214.57</v>
       </c>
       <c r="B221" t="n">
-        <v>6253.84375</v>
+        <v>6621.744140625</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>10241.46</v>
       </c>
       <c r="B222" t="n">
-        <v>10543.1904296875</v>
+        <v>10232.2275390625</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>42508.93</v>
       </c>
       <c r="B223" t="n">
-        <v>42336.99609375</v>
+        <v>42696.52734375</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>43839.99</v>
       </c>
       <c r="B224" t="n">
-        <v>43423.83984375</v>
+        <v>40786.3359375</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>34494.89</v>
       </c>
       <c r="B225" t="n">
-        <v>34584.48046875</v>
+        <v>33806.50390625</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>8856.980000000001</v>
       </c>
       <c r="B226" t="n">
-        <v>8085.88525390625</v>
+        <v>6809.37109375</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>26017.37</v>
       </c>
       <c r="B227" t="n">
-        <v>25586.025390625</v>
+        <v>25693.369140625</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>52137.67</v>
       </c>
       <c r="B228" t="n">
-        <v>51457.98828125</v>
+        <v>50757.42578125</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>3665.3</v>
       </c>
       <c r="B229" t="n">
-        <v>3181.830078125</v>
+        <v>3941.7587890625</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>16824.67</v>
       </c>
       <c r="B230" t="n">
-        <v>16243.390625</v>
+        <v>16098.005859375</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>9162.209999999999</v>
       </c>
       <c r="B231" t="n">
-        <v>9359.728515625</v>
+        <v>8675.16015625</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>3745.79</v>
       </c>
       <c r="B232" t="n">
-        <v>3486.45849609375</v>
+        <v>3238.206787109375</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>16428.78</v>
       </c>
       <c r="B233" t="n">
-        <v>16536.98828125</v>
+        <v>16247.322265625</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>25841.21</v>
       </c>
       <c r="B234" t="n">
-        <v>25919.57421875</v>
+        <v>26141.833984375</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>21826.87</v>
       </c>
       <c r="B235" t="n">
-        <v>19681.79296875</v>
+        <v>19954.78125</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>6353.01</v>
       </c>
       <c r="B236" t="n">
-        <v>6298.03466796875</v>
+        <v>6640.9658203125</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>6479.84</v>
       </c>
       <c r="B237" t="n">
-        <v>5847.353515625</v>
+        <v>5365.69677734375</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>55605.2</v>
       </c>
       <c r="B238" t="n">
-        <v>57956.5859375</v>
+        <v>58406.6796875</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>9266</v>
       </c>
       <c r="B239" t="n">
-        <v>9123.7822265625</v>
+        <v>8491.71875</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>20798.16</v>
       </c>
       <c r="B240" t="n">
-        <v>20041.814453125</v>
+        <v>19689.8515625</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>22987.79</v>
       </c>
       <c r="B241" t="n">
-        <v>23173.67578125</v>
+        <v>22543.8984375</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>18036.53</v>
       </c>
       <c r="B242" t="n">
-        <v>18379.1171875</v>
+        <v>18960.6015625</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>5017.37</v>
       </c>
       <c r="B243" t="n">
-        <v>4913.203125</v>
+        <v>5494.41748046875</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>8133.64</v>
       </c>
       <c r="B244" t="n">
-        <v>7994.3876953125</v>
+        <v>8360.029296875</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>7521.01</v>
       </c>
       <c r="B245" t="n">
-        <v>7323.3623046875</v>
+        <v>7318.92724609375</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>63470.08</v>
       </c>
       <c r="B246" t="n">
-        <v>64067.640625</v>
+        <v>62259.1875</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>10164.71</v>
       </c>
       <c r="B247" t="n">
-        <v>9454.5908203125</v>
+        <v>9727.2666015625</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>8778.57</v>
       </c>
       <c r="B248" t="n">
-        <v>7813.98193359375</v>
+        <v>7888.41064453125</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>43082.94</v>
       </c>
       <c r="B249" t="n">
-        <v>43306.0859375</v>
+        <v>42161.1640625</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>44170.99</v>
       </c>
       <c r="B250" t="n">
-        <v>41496.2890625</v>
+        <v>41434.56640625</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>6720.06</v>
       </c>
       <c r="B251" t="n">
-        <v>6590.9541015625</v>
+        <v>7141.53369140625</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>9525.59</v>
       </c>
       <c r="B252" t="n">
-        <v>9547.0029296875</v>
+        <v>8957.16796875</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>10840.48</v>
       </c>
       <c r="B253" t="n">
-        <v>10643.1865234375</v>
+        <v>10254.77734375</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>68809.89999999999</v>
       </c>
       <c r="B254" t="n">
-        <v>69230.2734375</v>
+        <v>67343.0703125</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>46431.5</v>
       </c>
       <c r="B255" t="n">
-        <v>45596.5859375</v>
+        <v>43693.6484375</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>18970.79</v>
       </c>
       <c r="B256" t="n">
-        <v>21301.642578125</v>
+        <v>20865.076171875</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>59123.99</v>
       </c>
       <c r="B257" t="n">
-        <v>59077.91015625</v>
+        <v>57623.84765625</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>8650</v>
       </c>
       <c r="B258" t="n">
-        <v>8425.908203125</v>
+        <v>8730.556640625</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>7851.51</v>
       </c>
       <c r="B259" t="n">
-        <v>7994.353515625</v>
+        <v>8451.693359375</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>4027.81</v>
       </c>
       <c r="B260" t="n">
-        <v>3789.40869140625</v>
+        <v>4600.708984375</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>22432.58</v>
       </c>
       <c r="B261" t="n">
-        <v>20858.837890625</v>
+        <v>20561.1484375</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>11681.68</v>
       </c>
       <c r="B262" t="n">
-        <v>11473.068359375</v>
+        <v>11355.521484375</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>36742.22</v>
       </c>
       <c r="B263" t="n">
-        <v>36797.5703125</v>
+        <v>37965.828125</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>42364.13</v>
       </c>
       <c r="B264" t="n">
-        <v>43515.796875</v>
+        <v>42111.203125</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>30312.01</v>
       </c>
       <c r="B265" t="n">
-        <v>29614.6875</v>
+        <v>30523.845703125</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>7658.84</v>
       </c>
       <c r="B266" t="n">
-        <v>7086.755859375</v>
+        <v>7072.1015625</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>13699.34</v>
       </c>
       <c r="B267" t="n">
-        <v>14883.685546875</v>
+        <v>14420.8310546875</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>7461.29</v>
       </c>
       <c r="B268" t="n">
-        <v>7312.77734375</v>
+        <v>7420.28857421875</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>28838.16</v>
       </c>
       <c r="B269" t="n">
-        <v>27945.9453125</v>
+        <v>28262.609375</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>65376</v>
       </c>
       <c r="B270" t="n">
-        <v>67462.6484375</v>
+        <v>65653.296875</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>11360.2</v>
       </c>
       <c r="B271" t="n">
-        <v>11111.498046875</v>
+        <v>11055.375</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>3987.81</v>
       </c>
       <c r="B272" t="n">
-        <v>3470.13232421875</v>
+        <v>4391.123046875</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>11219.81</v>
       </c>
       <c r="B273" t="n">
-        <v>11025.87890625</v>
+        <v>10872.744140625</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>26568.08</v>
       </c>
       <c r="B274" t="n">
-        <v>26095.96484375</v>
+        <v>26499.748046875</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>16850.36</v>
       </c>
       <c r="B275" t="n">
-        <v>16756.5546875</v>
+        <v>16612.109375</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>23268.01</v>
       </c>
       <c r="B276" t="n">
-        <v>23607.490234375</v>
+        <v>22672.974609375</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>20591.13</v>
       </c>
       <c r="B277" t="n">
-        <v>19272.564453125</v>
+        <v>18969.421875</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>57487.73</v>
       </c>
       <c r="B278" t="n">
-        <v>59385.06640625</v>
+        <v>57646.94140625</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>56247.18</v>
       </c>
       <c r="B279" t="n">
-        <v>58228.5546875</v>
+        <v>57342.37890625</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>19160.01</v>
       </c>
       <c r="B280" t="n">
-        <v>18570.630859375</v>
+        <v>18485.697265625</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>9197.02</v>
       </c>
       <c r="B281" t="n">
-        <v>9208.68359375</v>
+        <v>9888.9052734375</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>11761.41</v>
       </c>
       <c r="B282" t="n">
-        <v>11357.396484375</v>
+        <v>11240.4482421875</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>21310.9</v>
       </c>
       <c r="B283" t="n">
-        <v>22738.091796875</v>
+        <v>21712.84375</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>51288.42</v>
       </c>
       <c r="B284" t="n">
-        <v>53359.0703125</v>
+        <v>53052.99609375</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>6965.71</v>
       </c>
       <c r="B285" t="n">
-        <v>7411.87890625</v>
+        <v>7941.49755859375</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>62486.65</v>
       </c>
       <c r="B286" t="n">
-        <v>61314.11328125</v>
+        <v>61527.12109375</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>5170.27</v>
       </c>
       <c r="B287" t="n">
-        <v>4648.9228515625</v>
+        <v>5154.7509765625</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>8168.39</v>
       </c>
       <c r="B288" t="n">
-        <v>7830.98876953125</v>
+        <v>7528.5869140625</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>27219.61</v>
       </c>
       <c r="B289" t="n">
-        <v>26115.498046875</v>
+        <v>26217.48046875</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>9301.530000000001</v>
       </c>
       <c r="B290" t="n">
-        <v>8900.2978515625</v>
+        <v>9564.181640625</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>6010.01</v>
       </c>
       <c r="B291" t="n">
-        <v>5754.48291015625</v>
+        <v>6326.76513671875</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>3545.37</v>
       </c>
       <c r="B292" t="n">
-        <v>3407.128662109375</v>
+        <v>2791.511962890625</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>8439</v>
       </c>
       <c r="B293" t="n">
-        <v>8877.1513671875</v>
+        <v>9404.7626953125</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>63987.92000000001</v>
       </c>
       <c r="B294" t="n">
-        <v>64852.09375</v>
+        <v>62949.671875</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>62224</v>
       </c>
       <c r="B295" t="n">
-        <v>61645.4765625</v>
+        <v>61347.6953125</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>6708</v>
       </c>
       <c r="B296" t="n">
-        <v>5816.6357421875</v>
+        <v>6496.87109375</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>8733.27</v>
       </c>
       <c r="B297" t="n">
-        <v>8649.1103515625</v>
+        <v>8863.341796875</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>65300.63</v>
       </c>
       <c r="B298" t="n">
-        <v>68337.34375</v>
+        <v>68410.703125</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>3403.55</v>
       </c>
       <c r="B299" t="n">
-        <v>3237.740478515625</v>
+        <v>2556.9541015625</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>9666.299999999999</v>
       </c>
       <c r="B300" t="n">
-        <v>9902.0205078125</v>
+        <v>9277.552734375</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>28028.53</v>
       </c>
       <c r="B301" t="n">
-        <v>26881.9453125</v>
+        <v>26730.486328125</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>10374.99</v>
       </c>
       <c r="B302" t="n">
-        <v>10089.6865234375</v>
+        <v>9892.0615234375</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>3969.74</v>
       </c>
       <c r="B303" t="n">
-        <v>3185.351318359375</v>
+        <v>3571.150634765625</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>22197.96</v>
       </c>
       <c r="B304" t="n">
-        <v>21644.9296875</v>
+        <v>22222.337890625</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>8462</v>
       </c>
       <c r="B305" t="n">
-        <v>8136.93505859375</v>
+        <v>8514.08203125</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>16150.03</v>
       </c>
       <c r="B306" t="n">
-        <v>15370.4462890625</v>
+        <v>14368.59375</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>50053.9</v>
       </c>
       <c r="B307" t="n">
-        <v>49920.734375</v>
+        <v>49137.41015625</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>20862.47</v>
       </c>
       <c r="B308" t="n">
-        <v>20891.77734375</v>
+        <v>20210.390625</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>3862.2</v>
       </c>
       <c r="B309" t="n">
-        <v>4307.67138671875</v>
+        <v>3455.676513671875</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>46914.16</v>
       </c>
       <c r="B310" t="n">
-        <v>48161.04296875</v>
+        <v>47053.58203125</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>7375.96</v>
       </c>
       <c r="B311" t="n">
-        <v>7300.45263671875</v>
+        <v>7336.33056640625</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>25728.2</v>
       </c>
       <c r="B312" t="n">
-        <v>26294.439453125</v>
+        <v>26645.134765625</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>38795.69</v>
       </c>
       <c r="B313" t="n">
-        <v>40455.32421875</v>
+        <v>40136.50390625</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>16291.86</v>
       </c>
       <c r="B314" t="n">
-        <v>15285.208984375</v>
+        <v>15717.0966796875</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>23554.85</v>
       </c>
       <c r="B315" t="n">
-        <v>22605.001953125</v>
+        <v>23078.966796875</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>46446.1</v>
       </c>
       <c r="B316" t="n">
-        <v>46791.37890625</v>
+        <v>45172.234375</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>10174.18</v>
       </c>
       <c r="B317" t="n">
-        <v>10889.2119140625</v>
+        <v>10696.2431640625</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>22667.21</v>
       </c>
       <c r="B318" t="n">
-        <v>21072.591796875</v>
+        <v>21838.505859375</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>10776.59</v>
       </c>
       <c r="B319" t="n">
-        <v>10531.1669921875</v>
+        <v>10162.6650390625</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>47153.69</v>
       </c>
       <c r="B320" t="n">
-        <v>48850.921875</v>
+        <v>47346.7734375</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>3932.44</v>
       </c>
       <c r="B321" t="n">
-        <v>4444.22998046875</v>
+        <v>3557.844970703125</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>58050</v>
       </c>
       <c r="B322" t="n">
-        <v>58653.98046875</v>
+        <v>56470.171875</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>11754.59</v>
       </c>
       <c r="B323" t="n">
-        <v>11924.8857421875</v>
+        <v>11563.490234375</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>6468.99</v>
       </c>
       <c r="B324" t="n">
-        <v>5808.7998046875</v>
+        <v>5417.04931640625</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>27628.27</v>
       </c>
       <c r="B325" t="n">
-        <v>27985.75390625</v>
+        <v>28342.9375</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>45511</v>
       </c>
       <c r="B326" t="n">
-        <v>46398.06640625</v>
+        <v>44077.95703125</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>12543.41</v>
       </c>
       <c r="B327" t="n">
-        <v>11708.5478515625</v>
+        <v>11554.9560546875</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>3743.56</v>
       </c>
       <c r="B328" t="n">
-        <v>3688.27294921875</v>
+        <v>3754.77392578125</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>43082.31</v>
       </c>
       <c r="B329" t="n">
-        <v>43498.21484375</v>
+        <v>41976.890625</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>11071.35</v>
       </c>
       <c r="B330" t="n">
-        <v>10959.1357421875</v>
+        <v>10814.349609375</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>57339.89</v>
       </c>
       <c r="B331" t="n">
-        <v>59790.28125</v>
+        <v>57980.9609375</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>3567.91</v>
       </c>
       <c r="B332" t="n">
-        <v>3562.650634765625</v>
+        <v>3520.496826171875</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>5655.94</v>
       </c>
       <c r="B333" t="n">
-        <v>5181.51220703125</v>
+        <v>4769.67919921875</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>69469.99000000001</v>
       </c>
       <c r="B334" t="n">
-        <v>68919</v>
+        <v>69170.421875</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>9465.139999999999</v>
       </c>
       <c r="B335" t="n">
-        <v>9610.2861328125</v>
+        <v>8986.8173828125</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>29109.15</v>
       </c>
       <c r="B336" t="n">
-        <v>33106.89453125</v>
+        <v>30615.46875</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>14378.9</v>
       </c>
       <c r="B337" t="n">
-        <v>14507.9951171875</v>
+        <v>13792.4111328125</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>11780</v>
       </c>
       <c r="B338" t="n">
-        <v>11770.759765625</v>
+        <v>11543.810546875</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>26852.48</v>
       </c>
       <c r="B339" t="n">
-        <v>27212.197265625</v>
+        <v>27584.6484375</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>7603.44</v>
       </c>
       <c r="B340" t="n">
-        <v>6912.7080078125</v>
+        <v>6870.5302734375</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>6298.01</v>
       </c>
       <c r="B341" t="n">
-        <v>6035.51220703125</v>
+        <v>6529.81396484375</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>11744.91</v>
       </c>
       <c r="B342" t="n">
-        <v>11129.3359375</v>
+        <v>10951.890625</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>27033.84</v>
       </c>
       <c r="B343" t="n">
-        <v>26819.650390625</v>
+        <v>27004.560546875</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>70799.06000000001</v>
       </c>
       <c r="B344" t="n">
-        <v>69152.0625</v>
+        <v>68113.7734375</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>8189.99</v>
       </c>
       <c r="B345" t="n">
-        <v>8322.755859375</v>
+        <v>7917.1171875</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>42849.78</v>
       </c>
       <c r="B346" t="n">
-        <v>43205.91796875</v>
+        <v>41330.70703125</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>34258.14</v>
       </c>
       <c r="B347" t="n">
-        <v>33687.45703125</v>
+        <v>32355.271484375</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>21529.12</v>
       </c>
       <c r="B348" t="n">
-        <v>21274.818359375</v>
+        <v>20689.640625</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>23232.76</v>
       </c>
       <c r="B349" t="n">
-        <v>22812.83203125</v>
+        <v>23535.80859375</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>48440.65</v>
       </c>
       <c r="B350" t="n">
-        <v>49598.10546875</v>
+        <v>47529.62109375</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>34051.24</v>
       </c>
       <c r="B351" t="n">
-        <v>35303.8984375</v>
+        <v>37346.4921875</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>19289.91</v>
       </c>
       <c r="B352" t="n">
-        <v>18545.642578125</v>
+        <v>18698.89453125</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>41461.83</v>
       </c>
       <c r="B353" t="n">
-        <v>41969.5625</v>
+        <v>39484.26171875</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>11820.86</v>
       </c>
       <c r="B354" t="n">
-        <v>11342.0615234375</v>
+        <v>11225.5380859375</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>6712.1</v>
       </c>
       <c r="B355" t="n">
-        <v>6132.3671875</v>
+        <v>6542.7998046875</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>7784.02</v>
       </c>
       <c r="B356" t="n">
-        <v>8535.1552734375</v>
+        <v>7930.99072265625</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>40515.7</v>
       </c>
       <c r="B357" t="n">
-        <v>41747.73046875</v>
+        <v>40294.0078125</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>19327.44</v>
       </c>
       <c r="B358" t="n">
-        <v>18978.423828125</v>
+        <v>18587.15625</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>16070.45</v>
       </c>
       <c r="B359" t="n">
-        <v>15622.970703125</v>
+        <v>15839.1533203125</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>3583.13</v>
       </c>
       <c r="B360" t="n">
-        <v>3224.470703125</v>
+        <v>3502.338623046875</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>30366.15</v>
       </c>
       <c r="B361" t="n">
-        <v>32341.77734375</v>
+        <v>33387.52734375</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>22622.98</v>
       </c>
       <c r="B362" t="n">
-        <v>22145.359375</v>
+        <v>22058.150390625</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>37818.87</v>
       </c>
       <c r="B363" t="n">
-        <v>38063.16015625</v>
+        <v>38402.06640625</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>5219.9</v>
       </c>
       <c r="B364" t="n">
-        <v>4677.78759765625</v>
+        <v>5290.626953125</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>11388.54</v>
       </c>
       <c r="B365" t="n">
-        <v>11105.1923828125</v>
+        <v>11088.720703125</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>8292.440000000001</v>
       </c>
       <c r="B366" t="n">
-        <v>8166.2509765625</v>
+        <v>7883.99462890625</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>23060.94</v>
       </c>
       <c r="B367" t="n">
-        <v>21303.638671875</v>
+        <v>21952.74609375</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>44399</v>
       </c>
       <c r="B368" t="n">
-        <v>45900.48828125</v>
+        <v>43901.34765625</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>7457</v>
       </c>
       <c r="B369" t="n">
-        <v>7574.509765625</v>
+        <v>7713.4443359375</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>39457.87</v>
       </c>
       <c r="B370" t="n">
-        <v>38568.2578125</v>
+        <v>36850.4296875</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>58712.59</v>
       </c>
       <c r="B371" t="n">
-        <v>60558.1640625</v>
+        <v>60697.3203125</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>24998.78</v>
       </c>
       <c r="B372" t="n">
-        <v>24538.1796875</v>
+        <v>24942.763671875</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>43902.66</v>
       </c>
       <c r="B373" t="n">
-        <v>43078.62890625</v>
+        <v>41924.0859375</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>11526.91</v>
       </c>
       <c r="B374" t="n">
-        <v>11503.8759765625</v>
+        <v>11046.783203125</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>7302.01</v>
       </c>
       <c r="B375" t="n">
-        <v>6730.59033203125</v>
+        <v>6854.09228515625</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>23152.19</v>
       </c>
       <c r="B376" t="n">
-        <v>22926.99609375</v>
+        <v>22159.138671875</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>28500.78</v>
       </c>
       <c r="B377" t="n">
-        <v>28137.34765625</v>
+        <v>28172.3203125</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>5683.9</v>
       </c>
       <c r="B378" t="n">
-        <v>5768.056640625</v>
+        <v>6220.11865234375</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>36552.97</v>
       </c>
       <c r="B379" t="n">
-        <v>37120.1171875</v>
+        <v>36181.8984375</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>55857.81</v>
       </c>
       <c r="B380" t="n">
-        <v>57874.1015625</v>
+        <v>56047.7109375</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>26281.66</v>
       </c>
       <c r="B381" t="n">
-        <v>25906.587890625</v>
+        <v>27041.716796875</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>8115.82</v>
       </c>
       <c r="B382" t="n">
-        <v>7848.4541015625</v>
+        <v>8540.3642578125</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>6841.37</v>
       </c>
       <c r="B383" t="n">
-        <v>6861.1416015625</v>
+        <v>6687.30224609375</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>27510.93</v>
       </c>
       <c r="B384" t="n">
-        <v>27328.0234375</v>
+        <v>27514.029296875</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>11293.22</v>
       </c>
       <c r="B385" t="n">
-        <v>10731.9873046875</v>
+        <v>10462.2431640625</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>9694.51</v>
       </c>
       <c r="B386" t="n">
-        <v>10350.9287109375</v>
+        <v>9123.1767578125</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>20591.84</v>
       </c>
       <c r="B387" t="n">
-        <v>19791.62890625</v>
+        <v>19785.84375</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>9242.620000000003</v>
       </c>
       <c r="B388" t="n">
-        <v>9307.845703125</v>
+        <v>9033.7998046875</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>64628</v>
       </c>
       <c r="B389" t="n">
-        <v>65627.2734375</v>
+        <v>64063.640625</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>6162.37</v>
       </c>
       <c r="B390" t="n">
-        <v>5686.07080078125</v>
+        <v>5365.8984375</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>23810.79</v>
       </c>
       <c r="B391" t="n">
-        <v>23075.505859375</v>
+        <v>23888.384765625</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>6387.96</v>
       </c>
       <c r="B392" t="n">
-        <v>6249.42919921875</v>
+        <v>6793.10595703125</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>4041.32</v>
       </c>
       <c r="B393" t="n">
-        <v>4029.89013671875</v>
+        <v>3258.55224609375</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>6485.85</v>
       </c>
       <c r="B394" t="n">
-        <v>5843.41357421875</v>
+        <v>5470.31689453125</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>28415.29</v>
       </c>
       <c r="B395" t="n">
-        <v>27885.078125</v>
+        <v>28542.375</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>10126.65</v>
       </c>
       <c r="B396" t="n">
-        <v>10550.341796875</v>
+        <v>10324.6533203125</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>20954.92</v>
       </c>
       <c r="B397" t="n">
-        <v>19117.423828125</v>
+        <v>19562.15234375</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>66915.2</v>
       </c>
       <c r="B398" t="n">
-        <v>67110.9453125</v>
+        <v>65022.75390625</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>6185.05</v>
       </c>
       <c r="B399" t="n">
-        <v>6587.9443359375</v>
+        <v>6956.58935546875</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>41492.39</v>
       </c>
       <c r="B400" t="n">
-        <v>41242.3359375</v>
+        <v>41041.671875</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>8064.92</v>
       </c>
       <c r="B401" t="n">
-        <v>7846.74462890625</v>
+        <v>6413.6015625</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>62959.53</v>
       </c>
       <c r="B402" t="n">
-        <v>62009.59765625</v>
+        <v>61920.96484375</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>26821.28</v>
       </c>
       <c r="B403" t="n">
-        <v>26615.609375</v>
+        <v>26837.251953125</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>4117.76</v>
       </c>
       <c r="B404" t="n">
-        <v>3636.288330078125</v>
+        <v>3655.611572265625</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>43794.37</v>
       </c>
       <c r="B405" t="n">
-        <v>43987.65234375</v>
+        <v>41698.640625</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>5922.41</v>
       </c>
       <c r="B406" t="n">
-        <v>5282.35693359375</v>
+        <v>5006.6044921875</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>42511.1</v>
       </c>
       <c r="B407" t="n">
-        <v>42340.62109375</v>
+        <v>42537.5390625</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>55777.63</v>
       </c>
       <c r="B408" t="n">
-        <v>55125.09375</v>
+        <v>54846.48828125</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>10925.57</v>
       </c>
       <c r="B409" t="n">
-        <v>10432.79296875</v>
+        <v>9986.267578125</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>7864.5</v>
       </c>
       <c r="B410" t="n">
-        <v>6961.96875</v>
+        <v>7535.52392578125</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>11369.02</v>
       </c>
       <c r="B411" t="n">
-        <v>10979.5546875</v>
+        <v>10721.3212890625</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>5236.900000000001</v>
       </c>
       <c r="B412" t="n">
-        <v>4756.89404296875</v>
+        <v>5278.0888671875</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>20468.81</v>
       </c>
       <c r="B413" t="n">
-        <v>21906.4296875</v>
+        <v>21423.98828125</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>25805.05</v>
       </c>
       <c r="B414" t="n">
-        <v>25671.5078125</v>
+        <v>26071.94140625</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>6895.8</v>
       </c>
       <c r="B415" t="n">
-        <v>7251.34228515625</v>
+        <v>5921.89208984375</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>9364.999999999998</v>
       </c>
       <c r="B416" t="n">
-        <v>9013.537109375</v>
+        <v>9316.2685546875</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>24842.2</v>
       </c>
       <c r="B417" t="n">
-        <v>23690.970703125</v>
+        <v>23865.435546875</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>5361.3</v>
       </c>
       <c r="B418" t="n">
-        <v>5762.14404296875</v>
+        <v>5541.72412109375</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>25598.49</v>
       </c>
       <c r="B419" t="n">
-        <v>25746.990234375</v>
+        <v>25742.09375</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>61498.33</v>
       </c>
       <c r="B420" t="n">
-        <v>63429.9609375</v>
+        <v>62272.859375</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>44042.99</v>
       </c>
       <c r="B421" t="n">
-        <v>44641.6171875</v>
+        <v>41831.7734375</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>9315.84</v>
       </c>
       <c r="B422" t="n">
-        <v>9564.5576171875</v>
+        <v>9618.662109375</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>7604.58</v>
       </c>
       <c r="B423" t="n">
-        <v>7844.68212890625</v>
+        <v>8137.80517578125</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>49224.94</v>
       </c>
       <c r="B424" t="n">
-        <v>49704.90234375</v>
+        <v>48234.98828125</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>34525.89</v>
       </c>
       <c r="B425" t="n">
-        <v>33091.078125</v>
+        <v>33511.8828125</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>46834.48</v>
       </c>
       <c r="B426" t="n">
-        <v>47301.59765625</v>
+        <v>45969.26953125</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>68352.17</v>
       </c>
       <c r="B427" t="n">
-        <v>68647.6328125</v>
+        <v>66735.25</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>9896.799999999999</v>
       </c>
       <c r="B428" t="n">
-        <v>9143.5322265625</v>
+        <v>9367.15234375</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>56714.62</v>
       </c>
       <c r="B429" t="n">
-        <v>58063.359375</v>
+        <v>56140.4921875</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>3875.21</v>
       </c>
       <c r="B430" t="n">
-        <v>4241.41552734375</v>
+        <v>3453.36181640625</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>8873.030000000001</v>
       </c>
       <c r="B431" t="n">
-        <v>9542.783203125</v>
+        <v>9034.94921875</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>39280.33</v>
       </c>
       <c r="B432" t="n">
-        <v>40407.50390625</v>
+        <v>39193.84765625</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>9058.26</v>
       </c>
       <c r="B433" t="n">
-        <v>9167.6572265625</v>
+        <v>8863.8525390625</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>35546.11000000001</v>
       </c>
       <c r="B434" t="n">
-        <v>37895.56640625</v>
+        <v>36136.04296875</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>22916.45</v>
       </c>
       <c r="B435" t="n">
-        <v>21614.224609375</v>
+        <v>22155.056640625</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>63606.74</v>
       </c>
       <c r="B436" t="n">
-        <v>64875.50390625</v>
+        <v>63683.99609375</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>9310</v>
       </c>
       <c r="B437" t="n">
-        <v>8882.7587890625</v>
+        <v>9203.5498046875</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>57541.06</v>
       </c>
       <c r="B438" t="n">
-        <v>58605.84765625</v>
+        <v>59048.76171875</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>22583.72</v>
       </c>
       <c r="B439" t="n">
-        <v>22619.298828125</v>
+        <v>21637.541015625</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>3224.17</v>
       </c>
       <c r="B440" t="n">
-        <v>3394.729248046875</v>
+        <v>2682.387939453125</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>8491.02</v>
       </c>
       <c r="B441" t="n">
-        <v>8216.73828125</v>
+        <v>8516.27734375</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>5024.95</v>
       </c>
       <c r="B442" t="n">
-        <v>4958.18701171875</v>
+        <v>5544.82666015625</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>16738.21</v>
       </c>
       <c r="B443" t="n">
-        <v>16555.49609375</v>
+        <v>16468.994140625</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>43789.51</v>
       </c>
       <c r="B444" t="n">
-        <v>41827.2890625</v>
+        <v>41739.75</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>46580.51000000001</v>
       </c>
       <c r="B445" t="n">
-        <v>46817.828125</v>
+        <v>45208.390625</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>3434.1</v>
       </c>
       <c r="B446" t="n">
-        <v>2674.382080078125</v>
+        <v>3326.707275390625</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>64774.26</v>
       </c>
       <c r="B447" t="n">
-        <v>65703.390625</v>
+        <v>65624.4375</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>47100.89</v>
       </c>
       <c r="B448" t="n">
-        <v>49765.05859375</v>
+        <v>48055.0390625</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>6070.780000000001</v>
       </c>
       <c r="B449" t="n">
-        <v>6158.9765625</v>
+        <v>6050.86083984375</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>3819.93</v>
       </c>
       <c r="B450" t="n">
-        <v>3731.389892578125</v>
+        <v>4069.857666015625</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>63866</v>
       </c>
       <c r="B451" t="n">
-        <v>64429.59765625</v>
+        <v>62353.69140625</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>3434.15</v>
       </c>
       <c r="B452" t="n">
-        <v>2805.12158203125</v>
+        <v>3443.73779296875</v>
       </c>
     </row>
     <row r="453">
@@ -4058,7 +4058,7 @@
         <v>30304.65</v>
       </c>
       <c r="B453" t="n">
-        <v>30395.3359375</v>
+        <v>29852.154296875</v>
       </c>
     </row>
     <row r="454">
@@ -4066,7 +4066,7 @@
         <v>26844.35</v>
       </c>
       <c r="B454" t="n">
-        <v>26401.837890625</v>
+        <v>26755.9765625</v>
       </c>
     </row>
     <row r="455">
@@ -4074,7 +4074,7 @@
         <v>46374.87</v>
       </c>
       <c r="B455" t="n">
-        <v>43005.37890625</v>
+        <v>42468.1015625</v>
       </c>
     </row>
     <row r="456">
@@ -4082,7 +4082,7 @@
         <v>6285</v>
       </c>
       <c r="B456" t="n">
-        <v>6371.25146484375</v>
+        <v>6982.13037109375</v>
       </c>
     </row>
     <row r="457">
@@ -4090,7 +4090,7 @@
         <v>55953.45</v>
       </c>
       <c r="B457" t="n">
-        <v>59080.28515625</v>
+        <v>58493.23046875</v>
       </c>
     </row>
     <row r="458">
@@ -4098,7 +4098,7 @@
         <v>68549.99000000001</v>
       </c>
       <c r="B458" t="n">
-        <v>68488.9765625</v>
+        <v>66479.8515625</v>
       </c>
     </row>
     <row r="459">
@@ -4106,7 +4106,7 @@
         <v>68398.39</v>
       </c>
       <c r="B459" t="n">
-        <v>68768.3671875</v>
+        <v>66789.578125</v>
       </c>
     </row>
     <row r="460">
@@ -4114,7 +4114,7 @@
         <v>44349.6</v>
       </c>
       <c r="B460" t="n">
-        <v>44790.80078125</v>
+        <v>43786.5</v>
       </c>
     </row>
     <row r="461">
@@ -4122,7 +4122,7 @@
         <v>30086.74</v>
       </c>
       <c r="B461" t="n">
-        <v>28835.322265625</v>
+        <v>27504.1640625</v>
       </c>
     </row>
     <row r="462">
@@ -4130,7 +4130,7 @@
         <v>7487</v>
       </c>
       <c r="B462" t="n">
-        <v>7216.19384765625</v>
+        <v>7226.39892578125</v>
       </c>
     </row>
     <row r="463">
@@ -4138,7 +4138,7 @@
         <v>6433.98</v>
       </c>
       <c r="B463" t="n">
-        <v>5961.53759765625</v>
+        <v>5589.904296875</v>
       </c>
     </row>
     <row r="464">
@@ -4146,7 +4146,7 @@
         <v>49699.59</v>
       </c>
       <c r="B464" t="n">
-        <v>49525.1640625</v>
+        <v>48092.80859375</v>
       </c>
     </row>
     <row r="465">
@@ -4154,7 +4154,7 @@
         <v>3951.64</v>
       </c>
       <c r="B465" t="n">
-        <v>3468.145263671875</v>
+        <v>2834.333251953125</v>
       </c>
     </row>
     <row r="466">
@@ -4162,7 +4162,7 @@
         <v>11699.99</v>
       </c>
       <c r="B466" t="n">
-        <v>12451.7119140625</v>
+        <v>12262.71484375</v>
       </c>
     </row>
     <row r="467">
@@ -4170,7 +4170,7 @@
         <v>41382.59</v>
       </c>
       <c r="B467" t="n">
-        <v>40779.51953125</v>
+        <v>38714.921875</v>
       </c>
     </row>
     <row r="468">
@@ -4178,7 +4178,7 @@
         <v>16542.4</v>
       </c>
       <c r="B468" t="n">
-        <v>16658.087890625</v>
+        <v>16311.982421875</v>
       </c>
     </row>
     <row r="469">
@@ -4186,7 +4186,7 @@
         <v>25934.25</v>
       </c>
       <c r="B469" t="n">
-        <v>25859.072265625</v>
+        <v>25946.875</v>
       </c>
     </row>
     <row r="470">
@@ -4194,7 +4194,7 @@
         <v>29201.35</v>
       </c>
       <c r="B470" t="n">
-        <v>31381.505859375</v>
+        <v>28933.064453125</v>
       </c>
     </row>
     <row r="471">
@@ -4202,7 +4202,7 @@
         <v>10728.6</v>
       </c>
       <c r="B471" t="n">
-        <v>10586.1416015625</v>
+        <v>10154.34375</v>
       </c>
     </row>
     <row r="472">
@@ -4210,7 +4210,7 @@
         <v>8555</v>
       </c>
       <c r="B472" t="n">
-        <v>7927.13671875</v>
+        <v>8517.5634765625</v>
       </c>
     </row>
     <row r="473">
@@ -4218,7 +4218,7 @@
         <v>25759.95</v>
       </c>
       <c r="B473" t="n">
-        <v>25137.45703125</v>
+        <v>25559.53515625</v>
       </c>
     </row>
     <row r="474">
@@ -4226,7 +4226,7 @@
         <v>63201.05</v>
       </c>
       <c r="B474" t="n">
-        <v>62310.6484375</v>
+        <v>61306.0859375</v>
       </c>
     </row>
     <row r="475">
@@ -4234,7 +4234,7 @@
         <v>29864.04</v>
       </c>
       <c r="B475" t="n">
-        <v>31252.369140625</v>
+        <v>28903.986328125</v>
       </c>
     </row>
     <row r="476">
@@ -4242,7 +4242,7 @@
         <v>30319.23</v>
       </c>
       <c r="B476" t="n">
-        <v>31863.876953125</v>
+        <v>30161.013671875</v>
       </c>
     </row>
     <row r="477">
@@ -4250,7 +4250,7 @@
         <v>10159.98</v>
       </c>
       <c r="B477" t="n">
-        <v>9716.587890625</v>
+        <v>8724.5693359375</v>
       </c>
     </row>
     <row r="478">
@@ -4258,7 +4258,7 @@
         <v>3839.26</v>
       </c>
       <c r="B478" t="n">
-        <v>3651.466796875</v>
+        <v>3642.299072265625</v>
       </c>
     </row>
     <row r="479">
@@ -4266,7 +4266,7 @@
         <v>24631.95</v>
       </c>
       <c r="B479" t="n">
-        <v>22904.46875</v>
+        <v>23055.640625</v>
       </c>
     </row>
     <row r="480">
@@ -4274,7 +4274,7 @@
         <v>57970.9</v>
       </c>
       <c r="B480" t="n">
-        <v>58389.078125</v>
+        <v>57107.42578125</v>
       </c>
     </row>
     <row r="481">
@@ -4282,7 +4282,7 @@
         <v>7257.45</v>
       </c>
       <c r="B481" t="n">
-        <v>7452.9287109375</v>
+        <v>8021.328125</v>
       </c>
     </row>
     <row r="482">
@@ -4290,7 +4290,7 @@
         <v>50399.66</v>
       </c>
       <c r="B482" t="n">
-        <v>49831.6875</v>
+        <v>48762.765625</v>
       </c>
     </row>
     <row r="483">
@@ -4298,7 +4298,7 @@
         <v>3861.84</v>
       </c>
       <c r="B483" t="n">
-        <v>3493.441162109375</v>
+        <v>3972.82568359375</v>
       </c>
     </row>
     <row r="484">
@@ -4306,7 +4306,7 @@
         <v>3553.06</v>
       </c>
       <c r="B484" t="n">
-        <v>3142.62841796875</v>
+        <v>3577.13330078125</v>
       </c>
     </row>
     <row r="485">
@@ -4314,7 +4314,7 @@
         <v>37359.86</v>
       </c>
       <c r="B485" t="n">
-        <v>36307.3125</v>
+        <v>36663.51953125</v>
       </c>
     </row>
     <row r="486">
@@ -4322,7 +4322,7 @@
         <v>10142.57</v>
       </c>
       <c r="B486" t="n">
-        <v>10818.7197265625</v>
+        <v>10134.48046875</v>
       </c>
     </row>
     <row r="487">
@@ -4330,7 +4330,7 @@
         <v>7964.87</v>
       </c>
       <c r="B487" t="n">
-        <v>8061.10498046875</v>
+        <v>8513.837890625</v>
       </c>
     </row>
     <row r="488">
@@ -4338,7 +4338,7 @@
         <v>7693.1</v>
       </c>
       <c r="B488" t="n">
-        <v>7411.0625</v>
+        <v>7351.919921875</v>
       </c>
     </row>
     <row r="489">
@@ -4346,7 +4346,7 @@
         <v>4161.01</v>
       </c>
       <c r="B489" t="n">
-        <v>3800.04150390625</v>
+        <v>3070.49560546875</v>
       </c>
     </row>
     <row r="490">
@@ -4354,7 +4354,7 @@
         <v>3476.81</v>
       </c>
       <c r="B490" t="n">
-        <v>3184.420654296875</v>
+        <v>3483.18359375</v>
       </c>
     </row>
     <row r="491">
@@ -4362,7 +4362,7 @@
         <v>3838.66</v>
       </c>
       <c r="B491" t="n">
-        <v>3486.130615234375</v>
+        <v>2981.479248046875</v>
       </c>
     </row>
     <row r="492">
@@ -4370,7 +4370,7 @@
         <v>11039</v>
       </c>
       <c r="B492" t="n">
-        <v>10656.50390625</v>
+        <v>9463.74609375</v>
       </c>
     </row>
     <row r="493">
@@ -4378,7 +4378,7 @@
         <v>6505.6</v>
       </c>
       <c r="B493" t="n">
-        <v>6489.978515625</v>
+        <v>6539.68603515625</v>
       </c>
     </row>
     <row r="494">
@@ -4386,7 +4386,7 @@
         <v>27598.75</v>
       </c>
       <c r="B494" t="n">
-        <v>27777.34765625</v>
+        <v>28117.630859375</v>
       </c>
     </row>
     <row r="495">
@@ -4394,7 +4394,7 @@
         <v>8725.98</v>
       </c>
       <c r="B495" t="n">
-        <v>7872.060546875</v>
+        <v>8567.9248046875</v>
       </c>
     </row>
     <row r="496">
@@ -4402,7 +4402,7 @@
         <v>29031.33</v>
       </c>
       <c r="B496" t="n">
-        <v>31153.556640625</v>
+        <v>28426.564453125</v>
       </c>
     </row>
     <row r="497">
@@ -4410,7 +4410,7 @@
         <v>11454</v>
       </c>
       <c r="B497" t="n">
-        <v>10564.42578125</v>
+        <v>9382.708984375</v>
       </c>
     </row>
     <row r="498">
@@ -4418,7 +4418,7 @@
         <v>63892.04</v>
       </c>
       <c r="B498" t="n">
-        <v>63126.52734375</v>
+        <v>60811.65234375</v>
       </c>
     </row>
     <row r="499">
@@ -4426,7 +4426,7 @@
         <v>35796.31</v>
       </c>
       <c r="B499" t="n">
-        <v>38178.9765625</v>
+        <v>37339.7265625</v>
       </c>
     </row>
     <row r="500">
@@ -4434,7 +4434,7 @@
         <v>30083.75</v>
       </c>
       <c r="B500" t="n">
-        <v>29581.57421875</v>
+        <v>29957.82421875</v>
       </c>
     </row>
     <row r="501">
@@ -4442,7 +4442,7 @@
         <v>3665.18</v>
       </c>
       <c r="B501" t="n">
-        <v>2725.744873046875</v>
+        <v>3410.92529296875</v>
       </c>
     </row>
     <row r="502">
@@ -4450,7 +4450,7 @@
         <v>7303</v>
       </c>
       <c r="B502" t="n">
-        <v>6071.14501953125</v>
+        <v>6801.29345703125</v>
       </c>
     </row>
     <row r="503">
@@ -4458,7 +4458,7 @@
         <v>9128.02</v>
       </c>
       <c r="B503" t="n">
-        <v>8300.5712890625</v>
+        <v>8737.0927734375</v>
       </c>
     </row>
     <row r="504">
@@ -4466,7 +4466,7 @@
         <v>10446.25</v>
       </c>
       <c r="B504" t="n">
-        <v>10445.19921875</v>
+        <v>10396.8408203125</v>
       </c>
     </row>
     <row r="505">
@@ -4474,7 +4474,7 @@
         <v>46025.24</v>
       </c>
       <c r="B505" t="n">
-        <v>46355.37890625</v>
+        <v>44379.80078125</v>
       </c>
     </row>
     <row r="506">
@@ -4482,7 +4482,7 @@
         <v>38466.9</v>
       </c>
       <c r="B506" t="n">
-        <v>38411.28125</v>
+        <v>37205.30859375</v>
       </c>
     </row>
     <row r="507">
@@ -4490,7 +4490,7 @@
         <v>7064.04</v>
       </c>
       <c r="B507" t="n">
-        <v>5957.85888671875</v>
+        <v>6688.67333984375</v>
       </c>
     </row>
     <row r="508">
@@ -4498,7 +4498,7 @@
         <v>7210</v>
       </c>
       <c r="B508" t="n">
-        <v>7295.41845703125</v>
+        <v>6926.0380859375</v>
       </c>
     </row>
     <row r="509">
@@ -4506,7 +4506,7 @@
         <v>61528.33</v>
       </c>
       <c r="B509" t="n">
-        <v>62712.8125</v>
+        <v>61154.6953125</v>
       </c>
     </row>
     <row r="510">
@@ -4514,7 +4514,7 @@
         <v>23191.2</v>
       </c>
       <c r="B510" t="n">
-        <v>22806.345703125</v>
+        <v>22419.708984375</v>
       </c>
     </row>
     <row r="511">
@@ -4522,7 +4522,7 @@
         <v>26575.96</v>
       </c>
       <c r="B511" t="n">
-        <v>26045.287109375</v>
+        <v>26324.828125</v>
       </c>
     </row>
     <row r="512">
@@ -4530,7 +4530,7 @@
         <v>10760.05</v>
       </c>
       <c r="B512" t="n">
-        <v>11071.9931640625</v>
+        <v>10773.353515625</v>
       </c>
     </row>
     <row r="513">
@@ -4538,7 +4538,7 @@
         <v>66001.41</v>
       </c>
       <c r="B513" t="n">
-        <v>66598.8359375</v>
+        <v>64375.55859375</v>
       </c>
     </row>
     <row r="514">
@@ -4546,7 +4546,7 @@
         <v>6208.36</v>
       </c>
       <c r="B514" t="n">
-        <v>5649.4619140625</v>
+        <v>5265.3662109375</v>
       </c>
     </row>
     <row r="515">
@@ -4554,7 +4554,7 @@
         <v>56900.75</v>
       </c>
       <c r="B515" t="n">
-        <v>56843.67578125</v>
+        <v>56747.51171875</v>
       </c>
     </row>
     <row r="516">
@@ -4562,7 +4562,7 @@
         <v>5709.99</v>
       </c>
       <c r="B516" t="n">
-        <v>5272.162109375</v>
+        <v>5573.3564453125</v>
       </c>
     </row>
     <row r="517">
@@ -4570,7 +4570,7 @@
         <v>69582.17999999999</v>
       </c>
       <c r="B517" t="n">
-        <v>69063.9609375</v>
+        <v>69062.7734375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized model to achieve higher accuracy on validation data
</commit_message>
<xml_diff>
--- a/Stored_data/predictions_test.xlsx
+++ b/Stored_data/predictions_test.xlsx
@@ -450,7 +450,7 @@
         <v>8278</v>
       </c>
       <c r="B2" t="n">
-        <v>8099.30078125</v>
+        <v>8375.7392578125</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>31454.23046875</v>
       </c>
       <c r="B3" t="n">
-        <v>32547.916015625</v>
+        <v>31067.517578125</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>21491.189453125</v>
       </c>
       <c r="B4" t="n">
-        <v>22064.91796875</v>
+        <v>21012.27734375</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>63165.1875</v>
       </c>
       <c r="B5" t="n">
-        <v>65199.96875</v>
+        <v>61096.11328125</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>39678.1171875</v>
       </c>
       <c r="B6" t="n">
-        <v>41252.70703125</v>
+        <v>39339.890625</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>8821.939453125</v>
       </c>
       <c r="B7" t="n">
-        <v>8647.69140625</v>
+        <v>8405.0869140625</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>11388.5400390625</v>
       </c>
       <c r="B8" t="n">
-        <v>11634.837890625</v>
+        <v>11052.595703125</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>59034.8984375</v>
       </c>
       <c r="B9" t="n">
-        <v>61614.90234375</v>
+        <v>57249.97265625</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>8471.7294921875</v>
       </c>
       <c r="B10" t="n">
-        <v>8603.8349609375</v>
+        <v>8533.12109375</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>37253.8125</v>
       </c>
       <c r="B11" t="n">
-        <v>38196.80859375</v>
+        <v>35740.92578125</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>3601.31005859375</v>
       </c>
       <c r="B12" t="n">
-        <v>3884.33349609375</v>
+        <v>3677.15185546875</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>53554.99609375</v>
       </c>
       <c r="B13" t="n">
-        <v>55561.83984375</v>
+        <v>52505.11328125</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>9227</v>
       </c>
       <c r="B14" t="n">
-        <v>10105.841796875</v>
+        <v>9696.7275390625</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>7115.03955078125</v>
       </c>
       <c r="B15" t="n">
-        <v>6056.91455078125</v>
+        <v>6314.21142578125</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>7240.06005859375</v>
       </c>
       <c r="B16" t="n">
-        <v>6138.2119140625</v>
+        <v>6463.27587890625</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>8170</v>
       </c>
       <c r="B17" t="n">
-        <v>8761.2744140625</v>
+        <v>8864.8994140625</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>20236.708984375</v>
       </c>
       <c r="B18" t="n">
-        <v>21085.89453125</v>
+        <v>19730.931640625</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>29031.330078125</v>
       </c>
       <c r="B19" t="n">
-        <v>30837.80859375</v>
+        <v>28779.478515625</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>25934.251953125</v>
       </c>
       <c r="B20" t="n">
-        <v>27354.2890625</v>
+        <v>25848.279296875</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>37449.7265625</v>
       </c>
       <c r="B21" t="n">
-        <v>41209.08984375</v>
+        <v>38806.609375</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>59123.98828125</v>
       </c>
       <c r="B22" t="n">
-        <v>62027.42578125</v>
+        <v>57516.8359375</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>6410</v>
       </c>
       <c r="B23" t="n">
-        <v>6031.04345703125</v>
+        <v>6111.50390625</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>19327.439453125</v>
       </c>
       <c r="B24" t="n">
-        <v>18550.703125</v>
+        <v>18160.34375</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>39742.06640625</v>
       </c>
       <c r="B25" t="n">
-        <v>41232.10546875</v>
+        <v>39219.38671875</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>5236.89990234375</v>
       </c>
       <c r="B26" t="n">
-        <v>4670.1015625</v>
+        <v>4940.833984375</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>3819.929931640625</v>
       </c>
       <c r="B27" t="n">
-        <v>3957.49169921875</v>
+        <v>3961.15234375</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>43199.99609375</v>
       </c>
       <c r="B28" t="n">
-        <v>45226.9375</v>
+        <v>41891.83984375</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>34669.12890625</v>
       </c>
       <c r="B29" t="n">
-        <v>35890.7265625</v>
+        <v>33112.48046875</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>26060.01171875</v>
       </c>
       <c r="B30" t="n">
-        <v>27261.412109375</v>
+        <v>25582.875</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>29314.138671875</v>
       </c>
       <c r="B31" t="n">
-        <v>30291.849609375</v>
+        <v>28986.98046875</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>9529.9296875</v>
       </c>
       <c r="B32" t="n">
-        <v>9144.669921875</v>
+        <v>8866.7890625</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>46048.30859375</v>
       </c>
       <c r="B33" t="n">
-        <v>48284.59375</v>
+        <v>45624.09765625</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>10925.5703125</v>
       </c>
       <c r="B34" t="n">
-        <v>11671.4697265625</v>
+        <v>10606.34765625</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>30086.740234375</v>
       </c>
       <c r="B35" t="n">
-        <v>31035.9453125</v>
+        <v>30045.4453125</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>58230.12890625</v>
       </c>
       <c r="B36" t="n">
-        <v>59347.92578125</v>
+        <v>56178.00390625</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>29468.099609375</v>
       </c>
       <c r="B37" t="n">
-        <v>30681.64453125</v>
+        <v>28612.935546875</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>7541.89013671875</v>
       </c>
       <c r="B38" t="n">
-        <v>7555.4208984375</v>
+        <v>7604.259765625</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>9131.33984375</v>
       </c>
       <c r="B39" t="n">
-        <v>9168.2158203125</v>
+        <v>9255.8681640625</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>31801.041015625</v>
       </c>
       <c r="B40" t="n">
-        <v>31484.01171875</v>
+        <v>29766.740234375</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>21826.87109375</v>
       </c>
       <c r="B41" t="n">
-        <v>21690.099609375</v>
+        <v>20423.529296875</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>30267.990234375</v>
       </c>
       <c r="B42" t="n">
-        <v>31777.443359375</v>
+        <v>29402.013671875</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>10785.310546875</v>
       </c>
       <c r="B43" t="n">
-        <v>10786.53125</v>
+        <v>10208.986328125</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>8172.99951171875</v>
       </c>
       <c r="B44" t="n">
-        <v>7986.78173828125</v>
+        <v>8153.49365234375</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>60923.5078125</v>
       </c>
       <c r="B45" t="n">
-        <v>61820.84765625</v>
+        <v>59126.51953125</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>10241.4599609375</v>
       </c>
       <c r="B46" t="n">
-        <v>11223.75</v>
+        <v>10400.7607421875</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>57635.98828125</v>
       </c>
       <c r="B47" t="n">
-        <v>60256.46484375</v>
+        <v>56735.13671875</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>17774.69921875</v>
       </c>
       <c r="B48" t="n">
-        <v>18006.490234375</v>
+        <v>16986.322265625</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>48121.40625</v>
       </c>
       <c r="B49" t="n">
-        <v>49181.69921875</v>
+        <v>46548.609375</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>47287.6015625</v>
       </c>
       <c r="B50" t="n">
-        <v>49106.65625</v>
+        <v>44994.8828125</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>67840.5078125</v>
       </c>
       <c r="B51" t="n">
-        <v>68633.1328125</v>
+        <v>64013.51953125</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>39148.65625</v>
       </c>
       <c r="B52" t="n">
-        <v>41264.453125</v>
+        <v>38800.15625</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>48588.15625</v>
       </c>
       <c r="B53" t="n">
-        <v>50553.76953125</v>
+        <v>46706.09375</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>8400</v>
       </c>
       <c r="B54" t="n">
-        <v>8736.91015625</v>
+        <v>8987.099609375</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>30289.51953125</v>
       </c>
       <c r="B55" t="n">
-        <v>31651.962890625</v>
+        <v>30025.16796875</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>37371.37890625</v>
       </c>
       <c r="B56" t="n">
-        <v>38094.14453125</v>
+        <v>36414.99609375</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>30692.44140625</v>
       </c>
       <c r="B57" t="n">
-        <v>31937.443359375</v>
+        <v>29586.51171875</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>6796.099609375</v>
       </c>
       <c r="B58" t="n">
-        <v>7266.0830078125</v>
+        <v>7217.66357421875</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>9687.880859375</v>
       </c>
       <c r="B59" t="n">
-        <v>9967.4423828125</v>
+        <v>10018.69140625</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>6353.009765625</v>
       </c>
       <c r="B60" t="n">
-        <v>6870.673828125</v>
+        <v>6799.125</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>8340.5791015625</v>
       </c>
       <c r="B61" t="n">
-        <v>8678.6435546875</v>
+        <v>8387.5703125</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>10890.009765625</v>
       </c>
       <c r="B62" t="n">
-        <v>11307.4658203125</v>
+        <v>10994.984375</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>46834.48046875</v>
       </c>
       <c r="B63" t="n">
-        <v>49767.02734375</v>
+        <v>45850.68359375</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>9917.2705078125</v>
       </c>
       <c r="B64" t="n">
-        <v>9754.2529296875</v>
+        <v>9770.7021484375</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>10174.1796875</v>
       </c>
       <c r="B65" t="n">
-        <v>10757.494140625</v>
+        <v>10642.56640625</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>43428.84765625</v>
       </c>
       <c r="B66" t="n">
-        <v>45243.26953125</v>
+        <v>42485.6640625</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>29637.33984375</v>
       </c>
       <c r="B67" t="n">
-        <v>30087.048828125</v>
+        <v>27650.583984375</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>6609.77978515625</v>
       </c>
       <c r="B68" t="n">
-        <v>6349.85107421875</v>
+        <v>6777.87451171875</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>6618.9599609375</v>
       </c>
       <c r="B69" t="n">
-        <v>6416.5849609375</v>
+        <v>6507.93408203125</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>9525.58984375</v>
       </c>
       <c r="B70" t="n">
-        <v>10045.0244140625</v>
+        <v>9296.2939453125</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>37854.63671875</v>
       </c>
       <c r="B71" t="n">
-        <v>38817.9765625</v>
+        <v>37196.125</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>49239.21875</v>
       </c>
       <c r="B72" t="n">
-        <v>49794.1875</v>
+        <v>47222.55859375</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>35796.30859375</v>
       </c>
       <c r="B73" t="n">
-        <v>38880.08984375</v>
+        <v>36058.30859375</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>67092.7578125</v>
       </c>
       <c r="B74" t="n">
-        <v>68378.8359375</v>
+        <v>63765.49609375</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>31734.220703125</v>
       </c>
       <c r="B75" t="n">
-        <v>30753.482421875</v>
+        <v>29102.287109375</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>7521.01025390625</v>
       </c>
       <c r="B76" t="n">
-        <v>7418.802734375</v>
+        <v>7486.16455078125</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>68245.7109375</v>
       </c>
       <c r="B77" t="n">
-        <v>68844.1953125</v>
+        <v>63494.5625</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>3875.2099609375</v>
       </c>
       <c r="B78" t="n">
-        <v>4624.35009765625</v>
+        <v>4599.10986328125</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>47153.6875</v>
       </c>
       <c r="B79" t="n">
-        <v>48159.05078125</v>
+        <v>44262.69140625</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>11029.9599609375</v>
       </c>
       <c r="B80" t="n">
-        <v>11205.08203125</v>
+        <v>10428.4501953125</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>22963.001953125</v>
       </c>
       <c r="B81" t="n">
-        <v>21908.333984375</v>
+        <v>21608.224609375</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>26574.529296875</v>
       </c>
       <c r="B82" t="n">
-        <v>27075.87890625</v>
+        <v>25930.826171875</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>7055.99951171875</v>
       </c>
       <c r="B83" t="n">
-        <v>7253.49365234375</v>
+        <v>7173.85693359375</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>56628.78515625</v>
       </c>
       <c r="B84" t="n">
-        <v>56420.38671875</v>
+        <v>54071.38671875</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>10387.8896484375</v>
       </c>
       <c r="B85" t="n">
-        <v>10996.0634765625</v>
+        <v>10392.1259765625</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>22622.98046875</v>
       </c>
       <c r="B86" t="n">
-        <v>22413.697265625</v>
+        <v>21615.81640625</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>30411.5703125</v>
       </c>
       <c r="B87" t="n">
-        <v>31308.357421875</v>
+        <v>29878.642578125</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>39422</v>
       </c>
       <c r="B88" t="n">
-        <v>40301.7578125</v>
+        <v>38618.8203125</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>7854.25</v>
       </c>
       <c r="B89" t="n">
-        <v>7823.62548828125</v>
+        <v>7787.32275390625</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>71452.015625</v>
       </c>
       <c r="B90" t="n">
-        <v>73292.2421875</v>
+        <v>67341.578125</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>5655.93994140625</v>
       </c>
       <c r="B91" t="n">
-        <v>5318.7353515625</v>
+        <v>5420.298828125</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>63793.390625</v>
       </c>
       <c r="B92" t="n">
-        <v>66060.3046875</v>
+        <v>62113.234375</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>6197.919921875</v>
       </c>
       <c r="B93" t="n">
-        <v>6164.96142578125</v>
+        <v>6516.68359375</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>6298.009765625</v>
       </c>
       <c r="B94" t="n">
-        <v>6293.3525390625</v>
+        <v>6430.095703125</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>28300.7890625</v>
       </c>
       <c r="B95" t="n">
-        <v>29306.134765625</v>
+        <v>27570.46875</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>10666.6298828125</v>
       </c>
       <c r="B96" t="n">
-        <v>11354.341796875</v>
+        <v>10422.369140625</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>64262.0078125</v>
       </c>
       <c r="B97" t="n">
-        <v>64986.8359375</v>
+        <v>62103.1484375</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>6410.43994140625</v>
       </c>
       <c r="B98" t="n">
-        <v>6967.85791015625</v>
+        <v>6474.10595703125</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>7817.759765625</v>
       </c>
       <c r="B99" t="n">
-        <v>7941.8125</v>
+        <v>7609.0830078125</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>45832.0078125</v>
       </c>
       <c r="B100" t="n">
-        <v>48060.4296875</v>
+        <v>44548.74609375</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>51568.21875</v>
       </c>
       <c r="B101" t="n">
-        <v>53765.9296875</v>
+        <v>49461.9375</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>46863.7265625</v>
       </c>
       <c r="B102" t="n">
-        <v>49073.49609375</v>
+        <v>46309.11328125</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>40074.94140625</v>
       </c>
       <c r="B103" t="n">
-        <v>40975.4140625</v>
+        <v>39387.1875</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>7019.97998046875</v>
       </c>
       <c r="B104" t="n">
-        <v>5964.90185546875</v>
+        <v>6209.40869140625</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>9197.6005859375</v>
       </c>
       <c r="B105" t="n">
-        <v>9711.7138671875</v>
+        <v>9084.9931640625</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>23326.83984375</v>
       </c>
       <c r="B106" t="n">
-        <v>22479.01953125</v>
+        <v>22061.130859375</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>9170.2802734375</v>
       </c>
       <c r="B107" t="n">
-        <v>9582.5244140625</v>
+        <v>9129.8125</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>27454.470703125</v>
       </c>
       <c r="B108" t="n">
-        <v>27639.2890625</v>
+        <v>26060.70703125</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>34051.2421875</v>
       </c>
       <c r="B109" t="n">
-        <v>36343.31640625</v>
+        <v>34673.25390625</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>57221.71875</v>
       </c>
       <c r="B110" t="n">
-        <v>58453.28515625</v>
+        <v>54929.2734375</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>11744.91015625</v>
       </c>
       <c r="B111" t="n">
-        <v>11776.330078125</v>
+        <v>11052.2275390625</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>38150.015625</v>
       </c>
       <c r="B112" t="n">
-        <v>38956.37109375</v>
+        <v>36714.05859375</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>26180.05078125</v>
       </c>
       <c r="B113" t="n">
-        <v>27201.189453125</v>
+        <v>25662.2421875</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>8145.27978515625</v>
       </c>
       <c r="B114" t="n">
-        <v>7539.83056640625</v>
+        <v>7434.89990234375</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>52137.66796875</v>
       </c>
       <c r="B115" t="n">
-        <v>53575.1171875</v>
+        <v>48961.08203125</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>48821.8671875</v>
       </c>
       <c r="B116" t="n">
-        <v>49648.23046875</v>
+        <v>46892.4375</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>19412.8203125</v>
       </c>
       <c r="B117" t="n">
-        <v>19129.546875</v>
+        <v>18323.423828125</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>8041.45947265625</v>
       </c>
       <c r="B118" t="n">
-        <v>8030.3720703125</v>
+        <v>8277.35546875</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>47722.6484375</v>
       </c>
       <c r="B119" t="n">
-        <v>50419.671875</v>
+        <v>45810.359375</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>43159.99609375</v>
       </c>
       <c r="B120" t="n">
-        <v>42853.26171875</v>
+        <v>40789.8984375</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>3594.8701171875</v>
       </c>
       <c r="B121" t="n">
-        <v>3751.30322265625</v>
+        <v>3626.84423828125</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>67540.0078125</v>
       </c>
       <c r="B122" t="n">
-        <v>70297.0546875</v>
+        <v>65311.18359375</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>64498.33984375</v>
       </c>
       <c r="B123" t="n">
-        <v>66792.953125</v>
+        <v>62481.9453125</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>7824.7998046875</v>
       </c>
       <c r="B124" t="n">
-        <v>8323.8173828125</v>
+        <v>8840.724609375</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>23810.7890625</v>
       </c>
       <c r="B125" t="n">
-        <v>24351.521484375</v>
+        <v>22583.77734375</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>7009.83984375</v>
       </c>
       <c r="B126" t="n">
-        <v>7081.10693359375</v>
+        <v>6991.24267578125</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>63865.99609375</v>
       </c>
       <c r="B127" t="n">
-        <v>65241.21484375</v>
+        <v>61351.41796875</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>20401.30859375</v>
       </c>
       <c r="B128" t="n">
-        <v>22393.630859375</v>
+        <v>21864.26953125</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>28713.7109375</v>
       </c>
       <c r="B129" t="n">
-        <v>30653.771484375</v>
+        <v>29017.357421875</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>28033.8203125</v>
       </c>
       <c r="B130" t="n">
-        <v>28696.267578125</v>
+        <v>26657.197265625</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>21134.810546875</v>
       </c>
       <c r="B131" t="n">
-        <v>21702.517578125</v>
+        <v>20328.544921875</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>26339.970703125</v>
       </c>
       <c r="B132" t="n">
-        <v>28091.96875</v>
+        <v>26556.044921875</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>20131.4609375</v>
       </c>
       <c r="B133" t="n">
-        <v>19825.029296875</v>
+        <v>19298.865234375</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>42941.09765625</v>
       </c>
       <c r="B134" t="n">
-        <v>44301.44140625</v>
+        <v>41719.19921875</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>46760.6171875</v>
       </c>
       <c r="B135" t="n">
-        <v>48641.64453125</v>
+        <v>45760.4375</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>7338.64013671875</v>
       </c>
       <c r="B136" t="n">
-        <v>7585.16650390625</v>
+        <v>7480.52587890625</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>20591.130859375</v>
       </c>
       <c r="B137" t="n">
-        <v>19834.931640625</v>
+        <v>19174.5546875</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>45811</v>
       </c>
       <c r="B138" t="n">
-        <v>48718.9375</v>
+        <v>44895.6953125</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>7390.89013671875</v>
       </c>
       <c r="B139" t="n">
-        <v>7573.8857421875</v>
+        <v>7586.31884765625</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>8907.5703125</v>
       </c>
       <c r="B140" t="n">
-        <v>8744.41015625</v>
+        <v>8621.9658203125</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>7277.830078125</v>
       </c>
       <c r="B141" t="n">
-        <v>6969.2294921875</v>
+        <v>7047.79150390625</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>8655.01953125</v>
       </c>
       <c r="B142" t="n">
-        <v>8258.1552734375</v>
+        <v>8304.7763671875</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>48864.9765625</v>
       </c>
       <c r="B143" t="n">
-        <v>51086.65625</v>
+        <v>47292.640625</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>11761.41015625</v>
       </c>
       <c r="B144" t="n">
-        <v>11888.71484375</v>
+        <v>11305.98046875</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>68124.1875</v>
       </c>
       <c r="B145" t="n">
-        <v>69568.6640625</v>
+        <v>63618.83984375</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>16598.94921875</v>
       </c>
       <c r="B146" t="n">
-        <v>16556.9765625</v>
+        <v>15857.8310546875</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>42511.09765625</v>
       </c>
       <c r="B147" t="n">
-        <v>45067.7734375</v>
+        <v>41746.5</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>37237.6015625</v>
       </c>
       <c r="B148" t="n">
-        <v>39289.34375</v>
+        <v>36956.45703125</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>27210.3515625</v>
       </c>
       <c r="B149" t="n">
-        <v>28602.552734375</v>
+        <v>26661.56640625</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>17149.470703125</v>
       </c>
       <c r="B150" t="n">
-        <v>18446.509765625</v>
+        <v>17602.22265625</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>67314.234375</v>
       </c>
       <c r="B151" t="n">
-        <v>69448.1328125</v>
+        <v>65327.21875</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>22432.580078125</v>
       </c>
       <c r="B152" t="n">
-        <v>22492.212890625</v>
+        <v>21584.44921875</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>65354.01953125</v>
       </c>
       <c r="B153" t="n">
-        <v>67349.8828125</v>
+        <v>62786.69921875</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>13326.6103515625</v>
       </c>
       <c r="B154" t="n">
-        <v>15280.6728515625</v>
+        <v>15256.5458984375</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>19570.400390625</v>
       </c>
       <c r="B155" t="n">
-        <v>18810.38671875</v>
+        <v>18463.447265625</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>18036.53125</v>
       </c>
       <c r="B156" t="n">
-        <v>19301.712890625</v>
+        <v>18001.3046875</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>9231.6103515625</v>
       </c>
       <c r="B157" t="n">
-        <v>9363.787109375</v>
+        <v>9057.419921875</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>7795.509765625</v>
       </c>
       <c r="B158" t="n">
-        <v>8204.8662109375</v>
+        <v>7778.80224609375</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>9224.51953125</v>
       </c>
       <c r="B159" t="n">
-        <v>10450.1728515625</v>
+        <v>10060.580078125</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>27261.0703125</v>
       </c>
       <c r="B160" t="n">
-        <v>27917.265625</v>
+        <v>25600.861328125</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>9292.240234375</v>
       </c>
       <c r="B161" t="n">
-        <v>9125.30859375</v>
+        <v>9033.39453125</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>8900.3505859375</v>
       </c>
       <c r="B162" t="n">
-        <v>9309.15625</v>
+        <v>9083.3232421875</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>58132.3203125</v>
       </c>
       <c r="B163" t="n">
-        <v>59745.30859375</v>
+        <v>56433.44140625</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>10331.5400390625</v>
       </c>
       <c r="B164" t="n">
-        <v>10146.4921875</v>
+        <v>9977.9189453125</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>3567.909912109375</v>
       </c>
       <c r="B165" t="n">
-        <v>3944.38623046875</v>
+        <v>3876.536376953125</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>46025.23828125</v>
       </c>
       <c r="B166" t="n">
-        <v>47175.875</v>
+        <v>44692.36328125</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>30766.51171875</v>
       </c>
       <c r="B167" t="n">
-        <v>32134.25390625</v>
+        <v>30383.85546875</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>26880.259765625</v>
       </c>
       <c r="B168" t="n">
-        <v>27784.001953125</v>
+        <v>26337.59375</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>48973.31640625</v>
       </c>
       <c r="B169" t="n">
-        <v>48921.22265625</v>
+        <v>46703.02734375</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>9342.1005859375</v>
       </c>
       <c r="B170" t="n">
-        <v>10140.0595703125</v>
+        <v>9392.1474609375</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>5415</v>
       </c>
       <c r="B171" t="n">
-        <v>5080.775390625</v>
+        <v>5223.115234375</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>36742.21875</v>
       </c>
       <c r="B172" t="n">
-        <v>37265.0078125</v>
+        <v>35448.6171875</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>6214.5703125</v>
       </c>
       <c r="B173" t="n">
-        <v>6849.84521484375</v>
+        <v>6869.17724609375</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>57351.55859375</v>
       </c>
       <c r="B174" t="n">
-        <v>57785.01953125</v>
+        <v>54583.4609375</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>10728.599609375</v>
       </c>
       <c r="B175" t="n">
-        <v>11251.978515625</v>
+        <v>10440.3232421875</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>16291.8603515625</v>
       </c>
       <c r="B176" t="n">
-        <v>16139.634765625</v>
+        <v>15259.6064453125</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>7693.099609375</v>
       </c>
       <c r="B177" t="n">
-        <v>7908.71923828125</v>
+        <v>7588.1181640625</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>8168.39013671875</v>
       </c>
       <c r="B178" t="n">
-        <v>8078.68017578125</v>
+        <v>7937.7802734375</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>8197.26953125</v>
       </c>
       <c r="B179" t="n">
-        <v>8144.25537109375</v>
+        <v>8242.9326171875</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>7948.009765625</v>
       </c>
       <c r="B180" t="n">
-        <v>8100.10009765625</v>
+        <v>7960.17138671875</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>35466.23828125</v>
       </c>
       <c r="B181" t="n">
-        <v>36798.54296875</v>
+        <v>34701.30078125</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>7575.01025390625</v>
       </c>
       <c r="B182" t="n">
-        <v>7671.52099609375</v>
+        <v>7756.4619140625</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>10164.7099609375</v>
       </c>
       <c r="B183" t="n">
-        <v>9733.72265625</v>
+        <v>9879.298828125</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>22783.55078125</v>
       </c>
       <c r="B184" t="n">
-        <v>22320.572265625</v>
+        <v>20819.240234375</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>36675.71875</v>
       </c>
       <c r="B185" t="n">
-        <v>38171.16796875</v>
+        <v>35453.2734375</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>6208.35986328125</v>
       </c>
       <c r="B186" t="n">
-        <v>6104.6953125</v>
+        <v>5987.38623046875</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>21038.0703125</v>
       </c>
       <c r="B187" t="n">
-        <v>21592.0234375</v>
+        <v>20671.791015625</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>11903.1298828125</v>
       </c>
       <c r="B188" t="n">
-        <v>11143.580078125</v>
+        <v>11129.37109375</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>42053.65625</v>
       </c>
       <c r="B189" t="n">
-        <v>44614.30078125</v>
+        <v>41087.43359375</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>12968.5205078125</v>
       </c>
       <c r="B190" t="n">
-        <v>13235.8740234375</v>
+        <v>12371.818359375</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>41660.0078125</v>
       </c>
       <c r="B191" t="n">
-        <v>43444.01953125</v>
+        <v>40882.421875</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>46464.66015625</v>
       </c>
       <c r="B192" t="n">
-        <v>49507.40234375</v>
+        <v>45182.47265625</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>26817.9296875</v>
       </c>
       <c r="B193" t="n">
-        <v>28400.31640625</v>
+        <v>26553.0390625</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>4117.76025390625</v>
       </c>
       <c r="B194" t="n">
-        <v>3948.07861328125</v>
+        <v>4172.22314453125</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>9138.5498046875</v>
       </c>
       <c r="B195" t="n">
-        <v>9326.40234375</v>
+        <v>8985.1708984375</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>27395.12890625</v>
       </c>
       <c r="B196" t="n">
-        <v>26533.119140625</v>
+        <v>25280.28515625</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>29352.900390625</v>
       </c>
       <c r="B197" t="n">
-        <v>30485.373046875</v>
+        <v>29116.919921875</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>11256.490234375</v>
       </c>
       <c r="B198" t="n">
-        <v>11281.111328125</v>
+        <v>11039.4580078125</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>8359.939453125</v>
       </c>
       <c r="B199" t="n">
-        <v>8264.7041015625</v>
+        <v>8515.3076171875</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>34081</v>
       </c>
       <c r="B200" t="n">
-        <v>34662.1953125</v>
+        <v>32537.92578125</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>9910</v>
       </c>
       <c r="B201" t="n">
-        <v>10843.841796875</v>
+        <v>10258.654296875</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>32078</v>
       </c>
       <c r="B202" t="n">
-        <v>33604.1171875</v>
+        <v>32200.140625</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>23223.30078125</v>
       </c>
       <c r="B203" t="n">
-        <v>23541.34375</v>
+        <v>22669.21875</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>11564.330078125</v>
       </c>
       <c r="B204" t="n">
-        <v>12074.931640625</v>
+        <v>11332.712890625</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>9518.16015625</v>
       </c>
       <c r="B205" t="n">
-        <v>9601.71484375</v>
+        <v>9183.732421875</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>23157.0703125</v>
       </c>
       <c r="B206" t="n">
-        <v>23008.595703125</v>
+        <v>22426.54296875</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>27162.140625</v>
       </c>
       <c r="B207" t="n">
-        <v>28207.7890625</v>
+        <v>26976.216796875</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>3745.789794921875</v>
       </c>
       <c r="B208" t="n">
-        <v>3922.619384765625</v>
+        <v>3925.56298828125</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>19131.869140625</v>
       </c>
       <c r="B209" t="n">
-        <v>19361.421875</v>
+        <v>18914.7578125</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>5308.25</v>
       </c>
       <c r="B210" t="n">
-        <v>4827.6982421875</v>
+        <v>5046.58349609375</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>43902.65625</v>
       </c>
       <c r="B211" t="n">
-        <v>45141.07421875</v>
+        <v>42565.3203125</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>5024.94970703125</v>
       </c>
       <c r="B212" t="n">
-        <v>4980.0439453125</v>
+        <v>5149.43994140625</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>9666.30078125</v>
       </c>
       <c r="B213" t="n">
-        <v>10240.7392578125</v>
+        <v>9503.3798828125</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>11820.8603515625</v>
       </c>
       <c r="B214" t="n">
-        <v>11623.017578125</v>
+        <v>11369.1376953125</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>3861.83984375</v>
       </c>
       <c r="B215" t="n">
-        <v>3846.647705078125</v>
+        <v>3835.291015625</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>14400.0009765625</v>
       </c>
       <c r="B216" t="n">
-        <v>15155.580078125</v>
+        <v>14995.28125</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>9419</v>
       </c>
       <c r="B217" t="n">
-        <v>9206.548828125</v>
+        <v>9118.482421875</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>46914.15625</v>
       </c>
       <c r="B218" t="n">
-        <v>50024.95703125</v>
+        <v>46196.91015625</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>6250.81005859375</v>
       </c>
       <c r="B219" t="n">
-        <v>6597.98291015625</v>
+        <v>6730.51904296875</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>38092.96875</v>
       </c>
       <c r="B220" t="n">
-        <v>38832.2734375</v>
+        <v>36041.1015625</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>4027.81005859375</v>
       </c>
       <c r="B221" t="n">
-        <v>3840.59716796875</v>
+        <v>3979.731201171875</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>18254.62890625</v>
       </c>
       <c r="B222" t="n">
-        <v>19046.314453125</v>
+        <v>17798.337890625</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>6506.9794921875</v>
       </c>
       <c r="B223" t="n">
-        <v>6380.9169921875</v>
+        <v>6536.0341796875</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>26747.779296875</v>
       </c>
       <c r="B224" t="n">
-        <v>27705.15234375</v>
+        <v>26242.982421875</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>35044.99609375</v>
       </c>
       <c r="B225" t="n">
-        <v>36418.29296875</v>
+        <v>33269.234375</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>40480.0078125</v>
       </c>
       <c r="B226" t="n">
-        <v>41422.26171875</v>
+        <v>39467.0625</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>49224.94140625</v>
       </c>
       <c r="B227" t="n">
-        <v>50378.2890625</v>
+        <v>47314.09765625</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>6479.84033203125</v>
       </c>
       <c r="B228" t="n">
-        <v>6884.5849609375</v>
+        <v>6794.6494140625</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>19166.900390625</v>
       </c>
       <c r="B229" t="n">
-        <v>19628.1484375</v>
+        <v>18607.1640625</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>7197.31982421875</v>
       </c>
       <c r="B230" t="n">
-        <v>7346.865234375</v>
+        <v>6754.9189453125</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>10842.849609375</v>
       </c>
       <c r="B231" t="n">
-        <v>10656.5234375</v>
+        <v>10337.38671875</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>54884.5</v>
       </c>
       <c r="B232" t="n">
-        <v>54905.33984375</v>
+        <v>51815.0546875</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>29700.2109375</v>
       </c>
       <c r="B233" t="n">
-        <v>31607.47265625</v>
+        <v>29570.498046875</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>42782.7265625</v>
       </c>
       <c r="B234" t="n">
-        <v>46938.859375</v>
+        <v>43555.1640625</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>9160.7802734375</v>
       </c>
       <c r="B235" t="n">
-        <v>9529.4501953125</v>
+        <v>9076.3984375</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>41262.10546875</v>
       </c>
       <c r="B236" t="n">
-        <v>43555.0234375</v>
+        <v>40883.46484375</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>8856.98046875</v>
       </c>
       <c r="B237" t="n">
-        <v>8308.4951171875</v>
+        <v>8706.806640625</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>33892.01953125</v>
       </c>
       <c r="B238" t="n">
-        <v>34839.94921875</v>
+        <v>32788.5</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>29770.419921875</v>
       </c>
       <c r="B239" t="n">
-        <v>31307.310546875</v>
+        <v>29709.447265625</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>27250.970703125</v>
       </c>
       <c r="B240" t="n">
-        <v>27580.45703125</v>
+        <v>25442.33203125</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>22707.87890625</v>
       </c>
       <c r="B241" t="n">
-        <v>22349.31640625</v>
+        <v>20898.33203125</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>35624.71875</v>
       </c>
       <c r="B242" t="n">
-        <v>36850.13671875</v>
+        <v>34843.7421875</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>7894.5595703125</v>
       </c>
       <c r="B243" t="n">
-        <v>7753.1103515625</v>
+        <v>7636.8818359375</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>10340.3095703125</v>
       </c>
       <c r="B244" t="n">
-        <v>10565.9189453125</v>
+        <v>10286.0751953125</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>19831.900390625</v>
       </c>
       <c r="B245" t="n">
-        <v>20116.619140625</v>
+        <v>19422.39453125</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>25805.05078125</v>
       </c>
       <c r="B246" t="n">
-        <v>27275.138671875</v>
+        <v>25533.861328125</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>65300.62890625</v>
       </c>
       <c r="B247" t="n">
-        <v>69192.078125</v>
+        <v>64104.44921875</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>35911.73046875</v>
       </c>
       <c r="B248" t="n">
-        <v>36838.58984375</v>
+        <v>33878.48046875</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>7991.73974609375</v>
       </c>
       <c r="B249" t="n">
-        <v>8518.4189453125</v>
+        <v>8110.6533203125</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>10374.990234375</v>
       </c>
       <c r="B250" t="n">
-        <v>10249.37109375</v>
+        <v>10496.7314453125</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>9265.9990234375</v>
       </c>
       <c r="B251" t="n">
-        <v>8994.373046875</v>
+        <v>9195.71484375</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>11648.1298828125</v>
       </c>
       <c r="B252" t="n">
-        <v>11951.625</v>
+        <v>11569.376953125</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>61937.3984375</v>
       </c>
       <c r="B253" t="n">
-        <v>66368.953125</v>
+        <v>63033.4375</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>44695.94921875</v>
       </c>
       <c r="B254" t="n">
-        <v>46665.44140625</v>
+        <v>43737.9296875</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>16632.12109375</v>
       </c>
       <c r="B255" t="n">
-        <v>16938.13671875</v>
+        <v>16078.361328125</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>65463.98828125</v>
       </c>
       <c r="B256" t="n">
-        <v>69993.328125</v>
+        <v>66627.8515625</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>3403.550048828125</v>
       </c>
       <c r="B257" t="n">
-        <v>3591.072998046875</v>
+        <v>3572.980224609375</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>3224.169921875</v>
       </c>
       <c r="B258" t="n">
-        <v>3597.146728515625</v>
+        <v>3485.8427734375</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>26968.62109375</v>
       </c>
       <c r="B259" t="n">
-        <v>28540.955078125</v>
+        <v>27061.515625</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>66660</v>
       </c>
       <c r="B260" t="n">
-        <v>68279.484375</v>
+        <v>62471.765625</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>43576.12890625</v>
       </c>
       <c r="B261" t="n">
-        <v>45248.375</v>
+        <v>42683.66015625</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>59132.12890625</v>
       </c>
       <c r="B262" t="n">
-        <v>60653.9296875</v>
+        <v>56778.046875</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>52663.8984375</v>
       </c>
       <c r="B263" t="n">
-        <v>53582.88671875</v>
+        <v>50486.875</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>36769.359375</v>
       </c>
       <c r="B264" t="n">
-        <v>38280.27734375</v>
+        <v>35148.2265625</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>31383.87109375</v>
       </c>
       <c r="B265" t="n">
-        <v>33414.9765625</v>
+        <v>31239.599609375</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>6485.85009765625</v>
       </c>
       <c r="B266" t="n">
-        <v>6223.2275390625</v>
+        <v>6344.66943359375</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>36445.30859375</v>
       </c>
       <c r="B267" t="n">
-        <v>39111.72265625</v>
+        <v>36915.5</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>6708</v>
       </c>
       <c r="B268" t="n">
-        <v>6220.9052734375</v>
+        <v>6505.76220703125</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>27938.380859375</v>
       </c>
       <c r="B269" t="n">
-        <v>28460.470703125</v>
+        <v>26562.017578125</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>26100.009765625</v>
       </c>
       <c r="B270" t="n">
-        <v>27269.162109375</v>
+        <v>25798.98828125</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>27154.150390625</v>
       </c>
       <c r="B271" t="n">
-        <v>27696.62890625</v>
+        <v>27051.939453125</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>7283.5400390625</v>
       </c>
       <c r="B272" t="n">
-        <v>7418.7490234375</v>
+        <v>6774.99462890625</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>29581.990234375</v>
       </c>
       <c r="B273" t="n">
-        <v>31254.078125</v>
+        <v>29357.203125</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>17224.1015625</v>
       </c>
       <c r="B274" t="n">
-        <v>17162.384765625</v>
+        <v>16296.244140625</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>55025.58984375</v>
       </c>
       <c r="B275" t="n">
-        <v>57244.3203125</v>
+        <v>53162.3203125</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>7658.83984375</v>
       </c>
       <c r="B276" t="n">
-        <v>7282.658203125</v>
+        <v>7459.228515625</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>13699.3408203125</v>
       </c>
       <c r="B277" t="n">
-        <v>14068.0537109375</v>
+        <v>14658.826171875</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>7461.28955078125</v>
       </c>
       <c r="B278" t="n">
-        <v>7362.97998046875</v>
+        <v>7350.45263671875</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>63201.05078125</v>
       </c>
       <c r="B279" t="n">
-        <v>65565.0078125</v>
+        <v>60540.38671875</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>22762.51953125</v>
       </c>
       <c r="B280" t="n">
-        <v>21942.9765625</v>
+        <v>21628.765625</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>57037.33984375</v>
       </c>
       <c r="B281" t="n">
-        <v>60207.5703125</v>
+        <v>55403.83203125</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>39280.328125</v>
       </c>
       <c r="B282" t="n">
-        <v>40806.5625</v>
+        <v>38898.328125</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>3743.56005859375</v>
       </c>
       <c r="B283" t="n">
-        <v>3943.985107421875</v>
+        <v>4085.529541015625</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>37716.55859375</v>
       </c>
       <c r="B284" t="n">
-        <v>39605.69140625</v>
+        <v>36830.6953125</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>22932.91015625</v>
       </c>
       <c r="B285" t="n">
-        <v>22046.12890625</v>
+        <v>21642.474609375</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>65769.9453125</v>
       </c>
       <c r="B286" t="n">
-        <v>67521.0859375</v>
+        <v>62592.03515625</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>50775.48828125</v>
       </c>
       <c r="B287" t="n">
-        <v>52168.96875</v>
+        <v>48051.16015625</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>7120.73974609375</v>
       </c>
       <c r="B288" t="n">
-        <v>7572.3837890625</v>
+        <v>6936.20556640625</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>66074.0390625</v>
       </c>
       <c r="B289" t="n">
-        <v>67654.328125</v>
+        <v>62050.3671875</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>54476.46484375</v>
       </c>
       <c r="B290" t="n">
-        <v>57144.515625</v>
+        <v>52470.97265625</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>5922.40966796875</v>
       </c>
       <c r="B291" t="n">
-        <v>5889.71142578125</v>
+        <v>5822.30810546875</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>32283.650390625</v>
       </c>
       <c r="B292" t="n">
-        <v>35252.953125</v>
+        <v>32679.15234375</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>24452.16015625</v>
       </c>
       <c r="B293" t="n">
-        <v>24354.41015625</v>
+        <v>23397.693359375</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>6723.0498046875</v>
       </c>
       <c r="B294" t="n">
-        <v>6157.9892578125</v>
+        <v>6422.97265625</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>7187.830078125</v>
       </c>
       <c r="B295" t="n">
-        <v>7189.77099609375</v>
+        <v>7081.26953125</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>45584.98828125</v>
       </c>
       <c r="B296" t="n">
-        <v>46772.0390625</v>
+        <v>43805.0703125</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>3583.1298828125</v>
       </c>
       <c r="B297" t="n">
-        <v>3846.74755859375</v>
+        <v>3667.59130859375</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>44421.19921875</v>
       </c>
       <c r="B298" t="n">
-        <v>43422.02734375</v>
+        <v>41244.28125</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>3862.199951171875</v>
       </c>
       <c r="B299" t="n">
-        <v>4525.89794921875</v>
+        <v>4581.47314453125</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>10939.990234375</v>
       </c>
       <c r="B300" t="n">
-        <v>11220.5166015625</v>
+        <v>10596.748046875</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>68896</v>
       </c>
       <c r="B301" t="n">
-        <v>70822.421875</v>
+        <v>66114.296875</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>6010.009765625</v>
       </c>
       <c r="B302" t="n">
-        <v>5507.72900390625</v>
+        <v>5605.60107421875</v>
       </c>
     </row>
     <row r="303">
@@ -2858,7 +2858,7 @@
         <v>59769.12890625</v>
       </c>
       <c r="B303" t="n">
-        <v>63220.97265625</v>
+        <v>58538.08984375</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>48343.27734375</v>
       </c>
       <c r="B304" t="n">
-        <v>50553.26953125</v>
+        <v>47502.68359375</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>20564.509765625</v>
       </c>
       <c r="B305" t="n">
-        <v>21522.880859375</v>
+        <v>20317.521484375</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>64882.42578125</v>
       </c>
       <c r="B306" t="n">
-        <v>67344.890625</v>
+        <v>62855.015625</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>69436.4296875</v>
       </c>
       <c r="B307" t="n">
-        <v>70904.4765625</v>
+        <v>66014.7890625</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>67652.4140625</v>
       </c>
       <c r="B308" t="n">
-        <v>70072.5859375</v>
+        <v>65594.9765625</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>30076.310546875</v>
       </c>
       <c r="B309" t="n">
-        <v>33213.59375</v>
+        <v>32154.498046875</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>10303.1201171875</v>
       </c>
       <c r="B310" t="n">
-        <v>10574.236328125</v>
+        <v>10041.7353515625</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>9162.2099609375</v>
       </c>
       <c r="B311" t="n">
-        <v>9493.6943359375</v>
+        <v>9063.3193359375</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>32820.01953125</v>
       </c>
       <c r="B312" t="n">
-        <v>34078.08984375</v>
+        <v>31762.2890625</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>5170.27001953125</v>
       </c>
       <c r="B313" t="n">
-        <v>4580.9287109375</v>
+        <v>4790.755859375</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>3823</v>
       </c>
       <c r="B314" t="n">
-        <v>3973.903076171875</v>
+        <v>3971.093994140625</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>6144.009765625</v>
       </c>
       <c r="B315" t="n">
-        <v>6489.900390625</v>
+        <v>6383.68115234375</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>8462</v>
       </c>
       <c r="B316" t="n">
-        <v>8125.025390625</v>
+        <v>8447.1904296875</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>6720.06005859375</v>
       </c>
       <c r="B317" t="n">
-        <v>6812.689453125</v>
+        <v>6805.185546875</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>16150.029296875</v>
       </c>
       <c r="B318" t="n">
-        <v>16214.44140625</v>
+        <v>16657.439453125</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>33092.98046875</v>
       </c>
       <c r="B319" t="n">
-        <v>34176.30078125</v>
+        <v>32988.8359375</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>55134.15625</v>
       </c>
       <c r="B320" t="n">
-        <v>58433.73046875</v>
+        <v>56108.16796875</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>65963.28125</v>
       </c>
       <c r="B321" t="n">
-        <v>69378.734375</v>
+        <v>65047.984375</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>43084.28515625</v>
       </c>
       <c r="B322" t="n">
-        <v>44870.1328125</v>
+        <v>41788.74609375</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>9851.830078125</v>
       </c>
       <c r="B323" t="n">
-        <v>9864.3173828125</v>
+        <v>9832.486328125</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>7375.9599609375</v>
       </c>
       <c r="B324" t="n">
-        <v>7389.3359375</v>
+        <v>7426.291015625</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>19164.37109375</v>
       </c>
       <c r="B325" t="n">
-        <v>17959.443359375</v>
+        <v>17896.615234375</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>48440.64453125</v>
       </c>
       <c r="B326" t="n">
-        <v>49998.640625</v>
+        <v>47390.34375</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>43892.9765625</v>
       </c>
       <c r="B327" t="n">
-        <v>43576.1875</v>
+        <v>41245.34765625</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>28028.53125</v>
       </c>
       <c r="B328" t="n">
-        <v>28794.609375</v>
+        <v>26539.748046875</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>70780.59375</v>
       </c>
       <c r="B329" t="n">
-        <v>72013.0625</v>
+        <v>67572.125</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>9772</v>
       </c>
       <c r="B330" t="n">
-        <v>9394.296875</v>
+        <v>9352.4365234375</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>27124.91015625</v>
       </c>
       <c r="B331" t="n">
-        <v>27995.865234375</v>
+        <v>25691.14453125</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>6967.3095703125</v>
       </c>
       <c r="B332" t="n">
-        <v>6534.7177734375</v>
+        <v>6619.55419921875</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>8733.2705078125</v>
       </c>
       <c r="B333" t="n">
-        <v>8773.6171875</v>
+        <v>8483.85546875</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>29211.060546875</v>
       </c>
       <c r="B334" t="n">
-        <v>30492.884765625</v>
+        <v>28812.146484375</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>26345</v>
       </c>
       <c r="B335" t="n">
-        <v>27330.4140625</v>
+        <v>25886.78125</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>7316.1396484375</v>
       </c>
       <c r="B336" t="n">
-        <v>7092.693359375</v>
+        <v>6997.3583984375</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>5017.3701171875</v>
       </c>
       <c r="B337" t="n">
-        <v>4877.43994140625</v>
+        <v>5050.10107421875</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>26473.7890625</v>
       </c>
       <c r="B338" t="n">
-        <v>27350.65234375</v>
+        <v>25915.08203125</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>18808.689453125</v>
       </c>
       <c r="B339" t="n">
-        <v>19728.7421875</v>
+        <v>18794.728515625</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>28838.16015625</v>
       </c>
       <c r="B340" t="n">
-        <v>29839.599609375</v>
+        <v>28210.154296875</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>43789.5078125</v>
       </c>
       <c r="B341" t="n">
-        <v>44394.69140625</v>
+        <v>41351.7109375</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>23149.951171875</v>
       </c>
       <c r="B342" t="n">
-        <v>23987.865234375</v>
+        <v>23054.189453125</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>11911</v>
       </c>
       <c r="B343" t="n">
-        <v>12374.9072265625</v>
+        <v>11620.3271484375</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>8439</v>
       </c>
       <c r="B344" t="n">
-        <v>8727.0556640625</v>
+        <v>8424.0498046875</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>38166.83984375</v>
       </c>
       <c r="B345" t="n">
-        <v>40263.82421875</v>
+        <v>37339.10546875</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>57314.74609375</v>
       </c>
       <c r="B346" t="n">
-        <v>59936.828125</v>
+        <v>55889.703125</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>24998.78125</v>
       </c>
       <c r="B347" t="n">
-        <v>24810.98828125</v>
+        <v>23557.875</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>37448.77734375</v>
       </c>
       <c r="B348" t="n">
-        <v>38545.84765625</v>
+        <v>36992.109375</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>61672.41796875</v>
       </c>
       <c r="B349" t="n">
-        <v>64438.875</v>
+        <v>58846.11328125</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>14378.900390625</v>
       </c>
       <c r="B350" t="n">
-        <v>14542.7841796875</v>
+        <v>15144.9169921875</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>18846.619140625</v>
       </c>
       <c r="B351" t="n">
-        <v>19723.12109375</v>
+        <v>18848.7578125</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>11526.91015625</v>
       </c>
       <c r="B352" t="n">
-        <v>11648.666015625</v>
+        <v>11378.49609375</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>33862.12109375</v>
       </c>
       <c r="B353" t="n">
-        <v>35918.53125</v>
+        <v>33395.078125</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>7603.43994140625</v>
       </c>
       <c r="B354" t="n">
-        <v>7275.3671875</v>
+        <v>7470.5751953125</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>3631.050048828125</v>
       </c>
       <c r="B355" t="n">
-        <v>3591.726806640625</v>
+        <v>3670.275634765625</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>34474.73046875</v>
       </c>
       <c r="B356" t="n">
-        <v>35236.97265625</v>
+        <v>33004.64453125</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>24271.759765625</v>
       </c>
       <c r="B357" t="n">
-        <v>23815.994140625</v>
+        <v>23117.484375</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>27242.591796875</v>
       </c>
       <c r="B358" t="n">
-        <v>28499.8046875</v>
+        <v>26778.017578125</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>8189.98974609375</v>
       </c>
       <c r="B359" t="n">
-        <v>8150.48876953125</v>
+        <v>8643.51953125</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>3792.010009765625</v>
       </c>
       <c r="B360" t="n">
-        <v>3886.077880859375</v>
+        <v>3818.492431640625</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>9513.2099609375</v>
       </c>
       <c r="B361" t="n">
-        <v>9110.8662109375</v>
+        <v>8941.6318359375</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>19401.630859375</v>
       </c>
       <c r="B362" t="n">
-        <v>19505.453125</v>
+        <v>18583.154296875</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>15328.41015625</v>
       </c>
       <c r="B363" t="n">
-        <v>15147.07421875</v>
+        <v>14397.2421875</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>63327.58984375</v>
       </c>
       <c r="B364" t="n">
-        <v>67376.34375</v>
+        <v>62279.2734375</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>8725.9794921875</v>
       </c>
       <c r="B365" t="n">
-        <v>8077.08349609375</v>
+        <v>8359.65234375</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>6162.3701171875</v>
       </c>
       <c r="B366" t="n">
-        <v>6032.423828125</v>
+        <v>6008.16943359375</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>46762.98828125</v>
       </c>
       <c r="B367" t="n">
-        <v>49189.87890625</v>
+        <v>46449.34375</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>8650</v>
       </c>
       <c r="B368" t="n">
-        <v>8399.1279296875</v>
+        <v>8237.2431640625</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>39450.12890625</v>
       </c>
       <c r="B369" t="n">
-        <v>40044.8046875</v>
+        <v>38048.57421875</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>6712.10009765625</v>
       </c>
       <c r="B370" t="n">
-        <v>6562.61181640625</v>
+        <v>6986.44287109375</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>7784.01953125</v>
       </c>
       <c r="B371" t="n">
-        <v>8387.6435546875</v>
+        <v>8301.56640625</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>3434.10009765625</v>
       </c>
       <c r="B372" t="n">
-        <v>3373.006103515625</v>
+        <v>3200.69677734375</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>67421.7734375</v>
       </c>
       <c r="B373" t="n">
-        <v>70237.03125</v>
+        <v>65447.56640625</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>66947.65625</v>
       </c>
       <c r="B374" t="n">
-        <v>68254.1171875</v>
+        <v>63124.4453125</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>10446.25</v>
       </c>
       <c r="B375" t="n">
-        <v>10834.087890625</v>
+        <v>10390.203125</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>26498.609375</v>
       </c>
       <c r="B376" t="n">
-        <v>27970.05859375</v>
+        <v>26503.875</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>9603.26953125</v>
       </c>
       <c r="B377" t="n">
-        <v>9794.9765625</v>
+        <v>9411.5166015625</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>19960.669921875</v>
       </c>
       <c r="B378" t="n">
-        <v>20134.14453125</v>
+        <v>19519.27734375</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>47067.98828125</v>
       </c>
       <c r="B379" t="n">
-        <v>49645.3984375</v>
+        <v>45841.83203125</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>6468.98974609375</v>
       </c>
       <c r="B380" t="n">
-        <v>6351.85009765625</v>
+        <v>6483.87109375</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>43082.9375</v>
       </c>
       <c r="B381" t="n">
-        <v>44833.73046875</v>
+        <v>41853.6015625</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>64011.99609375</v>
       </c>
       <c r="B382" t="n">
-        <v>65562.3515625</v>
+        <v>61530.4921875</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>9800.0107421875</v>
       </c>
       <c r="B383" t="n">
-        <v>10263.01953125</v>
+        <v>9655.6416015625</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>7456.99951171875</v>
       </c>
       <c r="B384" t="n">
-        <v>7587.58642578125</v>
+        <v>7661.1591796875</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>11392.080078125</v>
       </c>
       <c r="B385" t="n">
-        <v>12015.095703125</v>
+        <v>11302.669921875</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>4295.83984375</v>
       </c>
       <c r="B386" t="n">
-        <v>4450.07275390625</v>
+        <v>4348.4833984375</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>29895.431640625</v>
       </c>
       <c r="B387" t="n">
-        <v>31105.802734375</v>
+        <v>29583.013671875</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>43839.98828125</v>
       </c>
       <c r="B388" t="n">
-        <v>45617.69921875</v>
+        <v>42225.2421875</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>24670.41015625</v>
       </c>
       <c r="B389" t="n">
-        <v>23939.923828125</v>
+        <v>22839.78125</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>7302.01025390625</v>
       </c>
       <c r="B390" t="n">
-        <v>6757.45068359375</v>
+        <v>6935.47705078125</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>37699.0703125</v>
       </c>
       <c r="B391" t="n">
-        <v>39954.91015625</v>
+        <v>37765.2734375</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>13636.169921875</v>
       </c>
       <c r="B392" t="n">
-        <v>14101.1923828125</v>
+        <v>12692.6875</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>5683.89990234375</v>
       </c>
       <c r="B393" t="n">
-        <v>5400.4248046875</v>
+        <v>5550.4501953125</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>59013.796875</v>
       </c>
       <c r="B394" t="n">
-        <v>61201.44921875</v>
+        <v>58765.87109375</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>40515.6953125</v>
       </c>
       <c r="B395" t="n">
-        <v>43450.66796875</v>
+        <v>40509.59375</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>3545.3701171875</v>
       </c>
       <c r="B396" t="n">
-        <v>3717.730224609375</v>
+        <v>3632.19970703125</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>20123.009765625</v>
       </c>
       <c r="B397" t="n">
-        <v>20525.185546875</v>
+        <v>19779.275390625</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>27598.75</v>
       </c>
       <c r="B398" t="n">
-        <v>29049.537109375</v>
+        <v>27499.455078125</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>52303.6484375</v>
       </c>
       <c r="B399" t="n">
-        <v>54538.2578125</v>
+        <v>50963.90234375</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>23009.650390625</v>
       </c>
       <c r="B400" t="n">
-        <v>22905.869140625</v>
+        <v>21840.88671875</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>9694.509765625</v>
       </c>
       <c r="B401" t="n">
-        <v>10107.5107421875</v>
+        <v>9663.7802734375</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>27426.458984375</v>
       </c>
       <c r="B402" t="n">
-        <v>28377.640625</v>
+        <v>27026.001953125</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>19123.96875</v>
       </c>
       <c r="B403" t="n">
-        <v>18254.06640625</v>
+        <v>17944.6640625</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>11940</v>
       </c>
       <c r="B404" t="n">
-        <v>10896.2099609375</v>
+        <v>10615.3076171875</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>20771.591796875</v>
       </c>
       <c r="B405" t="n">
-        <v>20075.236328125</v>
+        <v>19428.728515625</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>19059.998046875</v>
       </c>
       <c r="B406" t="n">
-        <v>19179.056640625</v>
+        <v>18967.4765625</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>6387.9599609375</v>
       </c>
       <c r="B407" t="n">
-        <v>6381.7646484375</v>
+        <v>6429.6328125</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>8810.7900390625</v>
       </c>
       <c r="B408" t="n">
-        <v>9196.4404296875</v>
+        <v>9139.5302734375</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>11754.58984375</v>
       </c>
       <c r="B409" t="n">
-        <v>12218.802734375</v>
+        <v>11634.9140625</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>32945.171875</v>
       </c>
       <c r="B410" t="n">
-        <v>32059.326171875</v>
+        <v>30975.09375</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>3932.440185546875</v>
       </c>
       <c r="B411" t="n">
-        <v>4590.02587890625</v>
+        <v>4705.9951171875</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>67070</v>
       </c>
       <c r="B412" t="n">
-        <v>67998.828125</v>
+        <v>63752.22265625</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>50819.99609375</v>
       </c>
       <c r="B413" t="n">
-        <v>51860.7421875</v>
+        <v>47850.80078125</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>6185.0498046875</v>
       </c>
       <c r="B414" t="n">
-        <v>6675.3359375</v>
+        <v>6789.8642578125</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>7851.509765625</v>
       </c>
       <c r="B415" t="n">
-        <v>7832.376953125</v>
+        <v>7886.46630859375</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>8064.919921875</v>
       </c>
       <c r="B416" t="n">
-        <v>8115.0224609375</v>
+        <v>8144.0185546875</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>3665.179931640625</v>
       </c>
       <c r="B417" t="n">
-        <v>3471.584716796875</v>
+        <v>3504.611083984375</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>40144.0390625</v>
       </c>
       <c r="B418" t="n">
-        <v>40879.859375</v>
+        <v>37887.5546875</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>3715.2998046875</v>
       </c>
       <c r="B419" t="n">
-        <v>3888.19140625</v>
+        <v>3934.322998046875</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>49999.140625</v>
       </c>
       <c r="B420" t="n">
-        <v>51976.8984375</v>
+        <v>48990.07421875</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>4041.31982421875</v>
       </c>
       <c r="B421" t="n">
-        <v>4288.12646484375</v>
+        <v>4204.22216796875</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>11099.609375</v>
       </c>
       <c r="B422" t="n">
-        <v>11753.7080078125</v>
+        <v>10983.2158203125</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>51690.95703125</v>
       </c>
       <c r="B423" t="n">
-        <v>54534.80859375</v>
+        <v>51038.1953125</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>23455.51953125</v>
       </c>
       <c r="B424" t="n">
-        <v>24298.20703125</v>
+        <v>22797.349609375</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>7864.49951171875</v>
       </c>
       <c r="B425" t="n">
-        <v>6268.27587890625</v>
+        <v>6775.9794921875</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>61277.3671875</v>
       </c>
       <c r="B426" t="n">
-        <v>65051.9453125</v>
+        <v>60971.1953125</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>8269.5400390625</v>
       </c>
       <c r="B427" t="n">
-        <v>7930.8046875</v>
+        <v>8249.6689453125</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>21195.6015625</v>
       </c>
       <c r="B428" t="n">
-        <v>21143.625</v>
+        <v>20417.599609375</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>67609.984375</v>
       </c>
       <c r="B429" t="n">
-        <v>70453.125</v>
+        <v>65877.7421875</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>6895.7998046875</v>
       </c>
       <c r="B430" t="n">
-        <v>7304.263671875</v>
+        <v>7206.69384765625</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>9365</v>
       </c>
       <c r="B431" t="n">
-        <v>9323.2880859375</v>
+        <v>9488.181640625</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>57169.390625</v>
       </c>
       <c r="B432" t="n">
-        <v>59267.01953125</v>
+        <v>55193.9765625</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>3434.150146484375</v>
       </c>
       <c r="B433" t="n">
-        <v>3431.22509765625</v>
+        <v>3268.31591796875</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>3665.300048828125</v>
       </c>
       <c r="B434" t="n">
-        <v>3716.5888671875</v>
+        <v>3581.704833984375</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>6868.69970703125</v>
       </c>
       <c r="B435" t="n">
-        <v>7401.90185546875</v>
+        <v>6769.06298828125</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>11406.240234375</v>
       </c>
       <c r="B436" t="n">
-        <v>11438.5732421875</v>
+        <v>11450.53515625</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>38420.80859375</v>
       </c>
       <c r="B437" t="n">
-        <v>40466.703125</v>
+        <v>38523.8203125</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>8785.25</v>
       </c>
       <c r="B438" t="n">
-        <v>8641.8486328125</v>
+        <v>8504.0830078125</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>7604.580078125</v>
       </c>
       <c r="B439" t="n">
-        <v>7443.07666015625</v>
+        <v>7357.3076171875</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>43444.1875</v>
       </c>
       <c r="B440" t="n">
-        <v>45185.86328125</v>
+        <v>42869.54296875</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>37858.19921875</v>
       </c>
       <c r="B441" t="n">
-        <v>38304.0859375</v>
+        <v>36637.484375</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>42560.10546875</v>
       </c>
       <c r="B442" t="n">
-        <v>45078.30859375</v>
+        <v>42108.1640625</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>11219.810546875</v>
       </c>
       <c r="B443" t="n">
-        <v>11810.83984375</v>
+        <v>11057.498046875</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>9896.7998046875</v>
       </c>
       <c r="B444" t="n">
-        <v>9461.28515625</v>
+        <v>9722.1357421875</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>67907.9921875</v>
       </c>
       <c r="B445" t="n">
-        <v>69723.46875</v>
+        <v>64109.3515625</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>5219.89990234375</v>
       </c>
       <c r="B446" t="n">
-        <v>5044.95458984375</v>
+        <v>5218.90576171875</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>8873.0302734375</v>
       </c>
       <c r="B447" t="n">
-        <v>9785.103515625</v>
+        <v>9371.69921875</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>41493.17578125</v>
       </c>
       <c r="B448" t="n">
-        <v>41957.1796875</v>
+        <v>40062.4296875</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>42120.62890625</v>
       </c>
       <c r="B449" t="n">
-        <v>43719.76171875</v>
+        <v>41039.46484375</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>3680.06005859375</v>
       </c>
       <c r="B450" t="n">
-        <v>3515.10302734375</v>
+        <v>3588.208984375</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>46580.5078125</v>
       </c>
       <c r="B451" t="n">
-        <v>49222.17578125</v>
+        <v>45588.109375</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>67074.140625</v>
       </c>
       <c r="B452" t="n">
-        <v>69782.1015625</v>
+        <v>65191.83984375</v>
       </c>
     </row>
     <row r="453">
@@ -4058,7 +4058,7 @@
         <v>9310</v>
       </c>
       <c r="B453" t="n">
-        <v>9174.40234375</v>
+        <v>9434.9423828125</v>
       </c>
     </row>
     <row r="454">
@@ -4066,7 +4066,7 @@
         <v>39116.71875</v>
       </c>
       <c r="B454" t="n">
-        <v>41113.81640625</v>
+        <v>38715.38671875</v>
       </c>
     </row>
     <row r="455">
@@ -4074,7 +4074,7 @@
         <v>42283.578125</v>
       </c>
       <c r="B455" t="n">
-        <v>45058.1875</v>
+        <v>42135.7265625</v>
       </c>
     </row>
     <row r="456">
@@ -4082,7 +4082,7 @@
         <v>29201.3515625</v>
       </c>
       <c r="B456" t="n">
-        <v>30478.419921875</v>
+        <v>28658.7109375</v>
       </c>
     </row>
     <row r="457">
@@ -4090,7 +4090,7 @@
         <v>62772.0078125</v>
       </c>
       <c r="B457" t="n">
-        <v>63293.38671875</v>
+        <v>60107.4609375</v>
       </c>
     </row>
     <row r="458">
@@ -4098,7 +4098,7 @@
         <v>35546.109375</v>
       </c>
       <c r="B458" t="n">
-        <v>38603.48828125</v>
+        <v>35777.57421875</v>
       </c>
     </row>
     <row r="459">
@@ -4106,7 +4106,7 @@
         <v>32259.900390625</v>
       </c>
       <c r="B459" t="n">
-        <v>33061.48046875</v>
+        <v>31873.376953125</v>
       </c>
     </row>
     <row r="460">
@@ -4114,7 +4114,7 @@
         <v>36462.9296875</v>
       </c>
       <c r="B460" t="n">
-        <v>38266.3984375</v>
+        <v>36264.62109375</v>
       </c>
     </row>
     <row r="461">
@@ -4122,7 +4122,7 @@
         <v>9128.0205078125</v>
       </c>
       <c r="B461" t="n">
-        <v>8480.78125</v>
+        <v>8997.201171875</v>
       </c>
     </row>
     <row r="462">
@@ -4130,7 +4130,7 @@
         <v>7257.44970703125</v>
       </c>
       <c r="B462" t="n">
-        <v>7465.58935546875</v>
+        <v>7226.0634765625</v>
       </c>
     </row>
     <row r="463">
@@ -4138,7 +4138,7 @@
         <v>50588.94921875</v>
       </c>
       <c r="B463" t="n">
-        <v>52561.3203125</v>
+        <v>49507.2265625</v>
       </c>
     </row>
     <row r="464">
@@ -4146,7 +4146,7 @@
         <v>48141.60546875</v>
       </c>
       <c r="B464" t="n">
-        <v>49281.26953125</v>
+        <v>46289.69140625</v>
       </c>
     </row>
     <row r="465">
@@ -4154,7 +4154,7 @@
         <v>6070.77978515625</v>
       </c>
       <c r="B465" t="n">
-        <v>6277.4443359375</v>
+        <v>6504.3671875</v>
       </c>
     </row>
     <row r="466">
@@ -4162,7 +4162,7 @@
         <v>3987.81005859375</v>
       </c>
       <c r="B466" t="n">
-        <v>3737.10791015625</v>
+        <v>3816.091796875</v>
       </c>
     </row>
     <row r="467">
@@ -4170,7 +4170,7 @@
         <v>21360.111328125</v>
       </c>
       <c r="B467" t="n">
-        <v>20548.958984375</v>
+        <v>19836.392578125</v>
       </c>
     </row>
     <row r="468">
@@ -4178,7 +4178,7 @@
         <v>69850.5390625</v>
       </c>
       <c r="B468" t="n">
-        <v>70802.4140625</v>
+        <v>66467.953125</v>
       </c>
     </row>
     <row r="469">
@@ -4186,7 +4186,7 @@
         <v>54018.80859375</v>
       </c>
       <c r="B469" t="n">
-        <v>55420.796875</v>
+        <v>53165.94921875</v>
       </c>
     </row>
     <row r="470">
@@ -4194,7 +4194,7 @@
         <v>10760.05078125</v>
       </c>
       <c r="B470" t="n">
-        <v>11402.3828125</v>
+        <v>11662.47265625</v>
       </c>
     </row>
     <row r="471">
@@ -4202,7 +4202,7 @@
         <v>21559.041015625</v>
       </c>
       <c r="B471" t="n">
-        <v>21057.462890625</v>
+        <v>20542.17578125</v>
       </c>
     </row>
     <row r="472">
@@ -4210,7 +4210,7 @@
         <v>50349.3671875</v>
       </c>
       <c r="B472" t="n">
-        <v>51410.25</v>
+        <v>48592.765625</v>
       </c>
     </row>
     <row r="473">
@@ -4218,7 +4218,7 @@
         <v>6285</v>
       </c>
       <c r="B473" t="n">
-        <v>6652.5283203125</v>
+        <v>6606.185546875</v>
       </c>
     </row>
     <row r="474">
@@ -4226,7 +4226,7 @@
         <v>68549.9921875</v>
       </c>
       <c r="B474" t="n">
-        <v>70863.546875</v>
+        <v>65860.6171875</v>
       </c>
     </row>
     <row r="475">
@@ -4234,7 +4234,7 @@
         <v>8614.4296875</v>
       </c>
       <c r="B475" t="n">
-        <v>8025.55419921875</v>
+        <v>8328.115234375</v>
       </c>
     </row>
     <row r="476">
@@ -4242,7 +4242,7 @@
         <v>11293.2197265625</v>
       </c>
       <c r="B476" t="n">
-        <v>11907.2294921875</v>
+        <v>10929.513671875</v>
       </c>
     </row>
     <row r="477">
@@ -4250,7 +4250,7 @@
         <v>9465.1396484375</v>
       </c>
       <c r="B477" t="n">
-        <v>9982.8828125</v>
+        <v>9265.8623046875</v>
       </c>
     </row>
     <row r="478">
@@ -4258,7 +4258,7 @@
         <v>16542.400390625</v>
       </c>
       <c r="B478" t="n">
-        <v>16750.126953125</v>
+        <v>16205.9033203125</v>
       </c>
     </row>
     <row r="479">
@@ -4266,7 +4266,7 @@
         <v>7487</v>
       </c>
       <c r="B479" t="n">
-        <v>7347.5166015625</v>
+        <v>7410.52587890625</v>
       </c>
     </row>
     <row r="480">
@@ -4274,7 +4274,7 @@
         <v>6433.9794921875</v>
       </c>
       <c r="B480" t="n">
-        <v>6130.83056640625</v>
+        <v>6225.1728515625</v>
       </c>
     </row>
     <row r="481">
@@ -4282,7 +4282,7 @@
         <v>62387.8984375</v>
       </c>
       <c r="B481" t="n">
-        <v>64074.80859375</v>
+        <v>59199.0390625</v>
       </c>
     </row>
     <row r="482">
@@ -4290,7 +4290,7 @@
         <v>3951.64013671875</v>
       </c>
       <c r="B482" t="n">
-        <v>3879.902099609375</v>
+        <v>3972.484130859375</v>
       </c>
     </row>
     <row r="483">
@@ -4298,7 +4298,7 @@
         <v>11699.990234375</v>
       </c>
       <c r="B483" t="n">
-        <v>12736.857421875</v>
+        <v>12534.939453125</v>
       </c>
     </row>
     <row r="484">
@@ -4306,7 +4306,7 @@
         <v>25940.78125</v>
       </c>
       <c r="B484" t="n">
-        <v>27397.837890625</v>
+        <v>25719.09765625</v>
       </c>
     </row>
     <row r="485">
@@ -4314,7 +4314,7 @@
         <v>23732.66015625</v>
       </c>
       <c r="B485" t="n">
-        <v>23562.384765625</v>
+        <v>22606.734375</v>
       </c>
     </row>
     <row r="486">
@@ -4322,7 +4322,7 @@
         <v>16280.23046875</v>
       </c>
       <c r="B486" t="n">
-        <v>16532.53515625</v>
+        <v>15634.900390625</v>
       </c>
     </row>
     <row r="487">
@@ -4330,7 +4330,7 @@
         <v>57339.890625</v>
       </c>
       <c r="B487" t="n">
-        <v>60270.19921875</v>
+        <v>57274.7890625</v>
       </c>
     </row>
     <row r="488">
@@ -4338,7 +4338,7 @@
         <v>47434.796875</v>
       </c>
       <c r="B488" t="n">
-        <v>49412.703125</v>
+        <v>45746.75</v>
       </c>
     </row>
     <row r="489">
@@ -4346,7 +4346,7 @@
         <v>6209.1796875</v>
       </c>
       <c r="B489" t="n">
-        <v>5884.140625</v>
+        <v>5993.71142578125</v>
       </c>
     </row>
     <row r="490">
@@ -4354,7 +4354,7 @@
         <v>44850.91015625</v>
       </c>
       <c r="B490" t="n">
-        <v>47069</v>
+        <v>44616.15234375</v>
       </c>
     </row>
     <row r="491">
@@ -4362,7 +4362,7 @@
         <v>11503.1396484375</v>
       </c>
       <c r="B491" t="n">
-        <v>12097.7236328125</v>
+        <v>11143.7412109375</v>
       </c>
     </row>
     <row r="492">
@@ -4370,7 +4370,7 @@
         <v>8169.86962890625</v>
       </c>
       <c r="B492" t="n">
-        <v>7228.50634765625</v>
+        <v>7321.44384765625</v>
       </c>
     </row>
     <row r="493">
@@ -4378,7 +4378,7 @@
         <v>25905.189453125</v>
       </c>
       <c r="B493" t="n">
-        <v>27294.9609375</v>
+        <v>25903.033203125</v>
       </c>
     </row>
     <row r="494">
@@ -4386,7 +4386,7 @@
         <v>37881.7578125</v>
       </c>
       <c r="B494" t="n">
-        <v>40400.37890625</v>
+        <v>37503.73828125</v>
       </c>
     </row>
     <row r="495">
@@ -4394,7 +4394,7 @@
         <v>10159.9794921875</v>
       </c>
       <c r="B495" t="n">
-        <v>10279.3720703125</v>
+        <v>9598.93359375</v>
       </c>
     </row>
     <row r="496">
@@ -4402,7 +4402,7 @@
         <v>3839.260009765625</v>
       </c>
       <c r="B496" t="n">
-        <v>3993.46533203125</v>
+        <v>3913.7001953125</v>
       </c>
     </row>
     <row r="497">
@@ -4410,7 +4410,7 @@
         <v>58950.0078125</v>
       </c>
       <c r="B497" t="n">
-        <v>60931.98828125</v>
+        <v>56677.01953125</v>
       </c>
     </row>
     <row r="498">
@@ -4418,7 +4418,7 @@
         <v>8159.2900390625</v>
       </c>
       <c r="B498" t="n">
-        <v>8598.6474609375</v>
+        <v>8224.1845703125</v>
       </c>
     </row>
     <row r="499">
@@ -4426,7 +4426,7 @@
         <v>37008.16015625</v>
       </c>
       <c r="B499" t="n">
-        <v>39609.1640625</v>
+        <v>37054.671875</v>
       </c>
     </row>
     <row r="500">
@@ -4434,7 +4434,7 @@
         <v>13791</v>
       </c>
       <c r="B500" t="n">
-        <v>14562.1748046875</v>
+        <v>13255.9833984375</v>
       </c>
     </row>
     <row r="501">
@@ -4442,7 +4442,7 @@
         <v>42563.7578125</v>
       </c>
       <c r="B501" t="n">
-        <v>44473.66796875</v>
+        <v>41777.8671875</v>
       </c>
     </row>
     <row r="502">
@@ -4450,7 +4450,7 @@
         <v>3553.06005859375</v>
       </c>
       <c r="B502" t="n">
-        <v>3805.910400390625</v>
+        <v>3666.48486328125</v>
       </c>
     </row>
     <row r="503">
@@ -4458,7 +4458,7 @@
         <v>3969.739990234375</v>
       </c>
       <c r="B503" t="n">
-        <v>3827.37109375</v>
+        <v>4044.833984375</v>
       </c>
     </row>
     <row r="504">
@@ -4466,7 +4466,7 @@
         <v>54869.94921875</v>
       </c>
       <c r="B504" t="n">
-        <v>57637.2890625</v>
+        <v>54919.59765625</v>
       </c>
     </row>
     <row r="505">
@@ -4474,7 +4474,7 @@
         <v>8115.81982421875</v>
       </c>
       <c r="B505" t="n">
-        <v>7962.80859375</v>
+        <v>8164.20654296875</v>
       </c>
     </row>
     <row r="506">
@@ -4482,7 +4482,7 @@
         <v>10740.2294921875</v>
       </c>
       <c r="B506" t="n">
-        <v>10707.396484375</v>
+        <v>10552.2958984375</v>
       </c>
     </row>
     <row r="507">
@@ -4490,7 +4490,7 @@
         <v>4161.009765625</v>
       </c>
       <c r="B507" t="n">
-        <v>4046.661865234375</v>
+        <v>4167.33740234375</v>
       </c>
     </row>
     <row r="508">
@@ -4498,7 +4498,7 @@
         <v>3476.81005859375</v>
       </c>
       <c r="B508" t="n">
-        <v>3821.958740234375</v>
+        <v>3642.124267578125</v>
       </c>
     </row>
     <row r="509">
@@ -4506,7 +4506,7 @@
         <v>3838.66015625</v>
       </c>
       <c r="B509" t="n">
-        <v>3724.888427734375</v>
+        <v>3801.914306640625</v>
       </c>
     </row>
     <row r="510">
@@ -4514,7 +4514,7 @@
         <v>11039</v>
       </c>
       <c r="B510" t="n">
-        <v>11177.021484375</v>
+        <v>11050.3759765625</v>
       </c>
     </row>
     <row r="511">
@@ -4522,7 +4522,7 @@
         <v>6505.599609375</v>
       </c>
       <c r="B511" t="n">
-        <v>6656.3623046875</v>
+        <v>6796.94775390625</v>
       </c>
     </row>
     <row r="512">
@@ -4530,7 +4530,7 @@
         <v>67896.5</v>
       </c>
       <c r="B512" t="n">
-        <v>70570.734375</v>
+        <v>65236.80078125</v>
       </c>
     </row>
     <row r="513">
@@ -4538,7 +4538,7 @@
         <v>39568.01953125</v>
       </c>
       <c r="B513" t="n">
-        <v>42244.53125</v>
+        <v>39950.546875</v>
       </c>
     </row>
     <row r="514">
@@ -4546,7 +4546,7 @@
         <v>29794</v>
       </c>
       <c r="B514" t="n">
-        <v>30385.697265625</v>
+        <v>29312.8203125</v>
       </c>
     </row>
     <row r="515">
@@ -4554,7 +4554,7 @@
         <v>11454</v>
       </c>
       <c r="B515" t="n">
-        <v>11714.8662109375</v>
+        <v>11594.822265625</v>
       </c>
     </row>
     <row r="516">
@@ -4562,7 +4562,7 @@
         <v>6841.3701171875</v>
       </c>
       <c r="B516" t="n">
-        <v>7374.2685546875</v>
+        <v>6814.2998046875</v>
       </c>
     </row>
     <row r="517">
@@ -4570,7 +4570,7 @@
         <v>7303</v>
       </c>
       <c r="B517" t="n">
-        <v>6452.779296875</v>
+        <v>6627.111328125</v>
       </c>
     </row>
     <row r="518">
@@ -4578,7 +4578,7 @@
         <v>10142.5693359375</v>
       </c>
       <c r="B518" t="n">
-        <v>10179.2412109375</v>
+        <v>10043.7119140625</v>
       </c>
     </row>
     <row r="519">
@@ -4586,7 +4586,7 @@
         <v>10666.390625</v>
       </c>
       <c r="B519" t="n">
-        <v>11727.349609375</v>
+        <v>10483.8486328125</v>
       </c>
     </row>
     <row r="520">
@@ -4594,7 +4594,7 @@
         <v>7064.0400390625</v>
       </c>
       <c r="B520" t="n">
-        <v>6345.48974609375</v>
+        <v>6484.9130859375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>